<commit_message>
Almost finished translating 0_1_Config...
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Ark1'!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Ark2'!$A$2:$D$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Ark2'!$A$2:$D$157</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="582">
   <si>
     <t>dat</t>
   </si>
@@ -580,24 +580,15 @@
     <t>Andre driftsinntekter (post 391 i eRapp)</t>
   </si>
   <si>
-    <t>d_sub</t>
-  </si>
-  <si>
     <t>Abonnenter i distribusjonsnett</t>
   </si>
   <si>
     <t>Avkastningsgrunnlag bidragsfinansiert inkl 1% arbeidskapital</t>
   </si>
   <si>
-    <t>d_rab.gf</t>
-  </si>
-  <si>
     <t>Grants funded regulatory asset base, including 1% working capital</t>
   </si>
   <si>
-    <t>d_dep.gfa</t>
-  </si>
-  <si>
     <t>Depreciation associated with assets in transmission services that are grants funded</t>
   </si>
   <si>
@@ -607,54 +598,33 @@
     <t>Anleggsbidragsfinansierte bokførteverdier</t>
   </si>
   <si>
-    <t>d_gfa</t>
-  </si>
-  <si>
     <t>Assets in transmission services that are grants funded</t>
   </si>
   <si>
     <t>Avkastningsgrunnlag egenfinansiert Dnett inkl 1% arbeidskapital</t>
   </si>
   <si>
-    <t>d_rab</t>
-  </si>
-  <si>
     <t>Regulatory asset base, including 1% working capital</t>
   </si>
   <si>
     <t>Sum avkastningsgrunnlag DEA Dnett inkl 1% arbeidskapital</t>
   </si>
   <si>
-    <t>d_RAB</t>
-  </si>
-  <si>
     <t>Total regulatory asset base, including 1% working capital</t>
   </si>
   <si>
     <t>Sum avskrivninger DEA Dnett</t>
   </si>
   <si>
-    <t>d_DEP</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total depreciations </t>
   </si>
   <si>
-    <t>d_dep.as</t>
-  </si>
-  <si>
     <t>Depreciation associated with self-funded assets</t>
   </si>
   <si>
     <t>Avskrivinger i distribusjonsnett knyttet til egenfinansiert kapital</t>
   </si>
   <si>
-    <t>d_as</t>
-  </si>
-  <si>
-    <t>Self-funded assets</t>
-  </si>
-  <si>
     <t>Bokførte verdier</t>
   </si>
   <si>
@@ -679,21 +649,12 @@
     <t>d_hv</t>
   </si>
   <si>
-    <t>Kilometers highvoltage lines in distributional grid</t>
-  </si>
-  <si>
     <t>Km høyspent nett distribusjonsnett</t>
   </si>
   <si>
     <t>KILE Dnett</t>
   </si>
   <si>
-    <t>d_cens</t>
-  </si>
-  <si>
-    <t>Cost of energy not supplied in distributional grid (Value of Loast Load)</t>
-  </si>
-  <si>
     <t>Implementerte pensjonskost Dnett</t>
   </si>
   <si>
@@ -727,12 +688,6 @@
     <t>Antall nettstasjoner Dnett</t>
   </si>
   <si>
-    <t>d_gs</t>
-  </si>
-  <si>
-    <t>Number of grid stations in distribution grid</t>
-  </si>
-  <si>
     <t>Pensjonskostnnader periodisert Dnett</t>
   </si>
   <si>
@@ -772,9 +727,6 @@
     <t>Frost, Geovariabel estimert vha faktoranalyse</t>
   </si>
   <si>
-    <t>dg_inc.av</t>
-  </si>
-  <si>
     <t>Average inclination in network companies map grid squares, distribution grid</t>
   </si>
   <si>
@@ -790,33 +742,12 @@
     <t>Selskapets andel sjøkabler</t>
   </si>
   <si>
-    <t>dg_sppc.sz</t>
-  </si>
-  <si>
-    <t>Scaled value of d_sppc, to make it size independent</t>
-  </si>
-  <si>
     <t>Størrelsesuavhengig mål på installert småkraftytelse i konsesjonsområde</t>
   </si>
   <si>
-    <t>dg_ice</t>
-  </si>
-  <si>
-    <t>dg_f4</t>
-  </si>
-  <si>
-    <t>dg_f7</t>
-  </si>
-  <si>
-    <t>dg_temp</t>
-  </si>
-  <si>
     <t>Gjennomsnittstemperatur for en 30-års periode (1985-2015)</t>
   </si>
   <si>
-    <t>dg_snow</t>
-  </si>
-  <si>
     <t>Temperature variable multiplied by -1</t>
   </si>
   <si>
@@ -826,9 +757,6 @@
     <t>dg_wind2_cod</t>
   </si>
   <si>
-    <t>Coast varaible, dg_wind2 divided by dr_cod</t>
-  </si>
-  <si>
     <t>Kystklimavariabel, kvadrertverdi for vind delt på avstand til kyst</t>
   </si>
   <si>
@@ -844,9 +772,6 @@
     <t>Vektet verdi av sjøkabler</t>
   </si>
   <si>
-    <t>rg_inc.av</t>
-  </si>
-  <si>
     <t>Average inclination in network companies map grid squares, regional grid</t>
   </si>
   <si>
@@ -976,9 +901,6 @@
     <t>Vekten for normkostnad</t>
   </si>
   <si>
-    <t>rg_s12</t>
-  </si>
-  <si>
     <t>Share of company's network components located in forest</t>
   </si>
   <si>
@@ -991,9 +913,6 @@
     <t>rg_Geo1</t>
   </si>
   <si>
-    <t>d_coeff</t>
-  </si>
-  <si>
     <t>d_lambda.avg</t>
   </si>
   <si>
@@ -1018,12 +937,6 @@
     <t>Gjennomsnittlig breddegrad i området hvor selskapet har nettverkskomponenter</t>
   </si>
   <si>
-    <t>dg_isl.sz</t>
-  </si>
-  <si>
-    <t>dg_lat.av</t>
-  </si>
-  <si>
     <t>Scaled value of isl, making GEO-variabel size independent</t>
   </si>
   <si>
@@ -1090,12 +1003,6 @@
     <t>NVE.ir</t>
   </si>
   <si>
-    <t>wm</t>
-  </si>
-  <si>
-    <t>Working mark used to calculate the regulatory asset base</t>
-  </si>
-  <si>
     <t>Arbeidskapitalpåslag brukt i beregningen av avkastningsgrunnlaget</t>
   </si>
   <si>
@@ -1177,9 +1084,6 @@
     <t>Vector containing variables that are to be used in the construction of the average fronts</t>
   </si>
   <si>
-    <t>Weighted value of a company's network components</t>
-  </si>
-  <si>
     <t>Weighted value of a company's underground cables</t>
   </si>
   <si>
@@ -1195,9 +1099,6 @@
     <t>Years for which historical pension costs are to be used</t>
   </si>
   <si>
-    <t>r_wv.cig</t>
-  </si>
-  <si>
     <t>r_wv.ol</t>
   </si>
   <si>
@@ -1219,9 +1120,6 @@
     <t>Pris på grensesnittskomponenter</t>
   </si>
   <si>
-    <t>The price of grid components in interface, regional and distributional grid</t>
-  </si>
-  <si>
     <t>decision</t>
   </si>
   <si>
@@ -1393,21 +1291,9 @@
     <t>d_EVAL</t>
   </si>
   <si>
-    <t>Cost associated with grid assesments in distribution grid</t>
-  </si>
-  <si>
     <t>drs_cost.RC.x.NL.A.r</t>
   </si>
   <si>
-    <t>d_cga</t>
-  </si>
-  <si>
-    <t>drs_RC_y.cb</t>
-  </si>
-  <si>
-    <t>The revenue cap for the cost base year</t>
-  </si>
-  <si>
     <t>drs_TOTcost.precal</t>
   </si>
   <si>
@@ -1435,9 +1321,6 @@
     <t>NVE.ir.RC</t>
   </si>
   <si>
-    <t>sysp.t-2</t>
-  </si>
-  <si>
     <t>NVE.ir.t-2</t>
   </si>
   <si>
@@ -1450,9 +1333,6 @@
     <t>ap.t-2</t>
   </si>
   <si>
-    <t>gci.NOK</t>
-  </si>
-  <si>
     <t>Companies set to industry's average efficiency</t>
   </si>
   <si>
@@ -1516,12 +1396,6 @@
     <t>d_OPEX</t>
   </si>
   <si>
-    <t>d_OPEXxL</t>
-  </si>
-  <si>
-    <t>Operation and maintenence costs, with labour and pension costs excluded</t>
-  </si>
-  <si>
     <t>Data frame for companies that are exempted from the regular model, critereas described in … (out of the ordinary)</t>
   </si>
   <si>
@@ -1637,6 +1511,270 @@
   </si>
   <si>
     <t>pnl.rc</t>
+  </si>
+  <si>
+    <t>sysp.t_2</t>
+  </si>
+  <si>
+    <t>Working Capital premium used to calculate the regulatory asset base</t>
+  </si>
+  <si>
+    <t>wcp</t>
+  </si>
+  <si>
+    <t>gci.p</t>
+  </si>
+  <si>
+    <t>The price of grid components in interface, regional and local distribution grid</t>
+  </si>
+  <si>
+    <t>ir.dea</t>
+  </si>
+  <si>
+    <t>pnl.dea</t>
+  </si>
+  <si>
+    <t>Price of network losses used in DEA calculation</t>
+  </si>
+  <si>
+    <t>d_nettap</t>
+  </si>
+  <si>
+    <t>nettap i MWh</t>
+  </si>
+  <si>
+    <t>ld_nl</t>
+  </si>
+  <si>
+    <t>Network losses in MWh</t>
+  </si>
+  <si>
+    <t>ld_coeff</t>
+  </si>
+  <si>
+    <t>ld_391</t>
+  </si>
+  <si>
+    <t>ld_sub</t>
+  </si>
+  <si>
+    <t>ld_rab.gf</t>
+  </si>
+  <si>
+    <t>ld_gfa</t>
+  </si>
+  <si>
+    <t>ld_rab</t>
+  </si>
+  <si>
+    <t>ld_RAB</t>
+  </si>
+  <si>
+    <t>ld_DEP</t>
+  </si>
+  <si>
+    <t>ld_dep.sf</t>
+  </si>
+  <si>
+    <t>ld_cens</t>
+  </si>
+  <si>
+    <t>ld_cga</t>
+  </si>
+  <si>
+    <t>ld_dep.gf</t>
+  </si>
+  <si>
+    <t>ld_bv.sf</t>
+  </si>
+  <si>
+    <t>Book value 31.12 of  Self-funded assets</t>
+  </si>
+  <si>
+    <t>ld_ss</t>
+  </si>
+  <si>
+    <t>Number of substations in local distribution grid</t>
+  </si>
+  <si>
+    <t>d_hsll</t>
+  </si>
+  <si>
+    <t>ld_hvoh</t>
+  </si>
+  <si>
+    <t>Kilometers highvoltage lines in local distribution grid</t>
+  </si>
+  <si>
+    <t>Kilometers highvoltage over head lines in local distribution grid</t>
+  </si>
+  <si>
+    <t>Cost of energy not supplied in distributional grid (Value of Lost Load)</t>
+  </si>
+  <si>
+    <t>Cost associated with grid assesments in local distribution grid</t>
+  </si>
+  <si>
+    <t>d_hsjord</t>
+  </si>
+  <si>
+    <t>Km høyspent luflinje distribusjonsnett</t>
+  </si>
+  <si>
+    <t>km høyspent jordkabel, Dnett</t>
+  </si>
+  <si>
+    <t>ld_hvug</t>
+  </si>
+  <si>
+    <t>d_hssjo</t>
+  </si>
+  <si>
+    <t>km høyspent sjøkabel, Dnett</t>
+  </si>
+  <si>
+    <t>ld_hvsc</t>
+  </si>
+  <si>
+    <t>Kilometers highvoltage under ground cabel in local distribution grid</t>
+  </si>
+  <si>
+    <t>Kilometers highvoltage sea cabel in local distribution grid</t>
+  </si>
+  <si>
+    <t>d_OPEXxS</t>
+  </si>
+  <si>
+    <t>Operation and maintenence costs, with salaries and pension costs excluded</t>
+  </si>
+  <si>
+    <t>d_gci</t>
+  </si>
+  <si>
+    <t>ld_gci</t>
+  </si>
+  <si>
+    <t>Grid components in interface between regional and distirbution grid</t>
+  </si>
+  <si>
+    <t>r_wv.ss</t>
+  </si>
+  <si>
+    <t>Weighted value of a company's substations</t>
+  </si>
+  <si>
+    <t>rdz_inc.av</t>
+  </si>
+  <si>
+    <t>rdz_f12</t>
+  </si>
+  <si>
+    <t>ldz_f4</t>
+  </si>
+  <si>
+    <t>ldz_f7</t>
+  </si>
+  <si>
+    <t>dr_vr</t>
+  </si>
+  <si>
+    <t>vindvariabel</t>
+  </si>
+  <si>
+    <t>ldz_wind.avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average wind (m/s) 50 m above ground, calculated by Kjeller Windtechnic </t>
+  </si>
+  <si>
+    <t>Coast varaible, dg_wind2 divided by dr_cod2c</t>
+  </si>
+  <si>
+    <t>dr_k2lukk</t>
+  </si>
+  <si>
+    <t>Kystavstand, med lukking av større fjorder og sund</t>
+  </si>
+  <si>
+    <t>ldz_cod2c</t>
+  </si>
+  <si>
+    <t>Coastal distande, closing of specific fjords and straits whit 2nd appraoch.</t>
+  </si>
+  <si>
+    <t>ldz_snow</t>
+  </si>
+  <si>
+    <t>ldz_inc.av</t>
+  </si>
+  <si>
+    <t>ldz_ice.av</t>
+  </si>
+  <si>
+    <t>ldz_temp</t>
+  </si>
+  <si>
+    <t>d_aoey1</t>
+  </si>
+  <si>
+    <t>ldz_isl</t>
+  </si>
+  <si>
+    <t>Antall øyer: Forsyning av øyer uten fastlandsforbindelse og mer enn 1 km fra fastland eller nærmeste forsynte øy</t>
+  </si>
+  <si>
+    <t>Number of islands connected without mainland connection, more than 1 km of coast and without power production</t>
+  </si>
+  <si>
+    <t>dr_skytelse</t>
+  </si>
+  <si>
+    <t>installed capacity micro power plants</t>
+  </si>
+  <si>
+    <t>ldz_cmpp</t>
+  </si>
+  <si>
+    <t>ldz_cmpp.sz</t>
+  </si>
+  <si>
+    <t>Scaled value of ldz_cmpp, to make it size independent</t>
+  </si>
+  <si>
+    <t>rr_antall_ruter</t>
+  </si>
+  <si>
+    <t>Antall kart-ruter i konsesjonærenes område</t>
+  </si>
+  <si>
+    <t>dr_antall_ruter</t>
+  </si>
+  <si>
+    <t>rdz_mgc</t>
+  </si>
+  <si>
+    <t>Antall ruter med nettanlegg i konsesjonærenes område</t>
+  </si>
+  <si>
+    <t>ldz_isl.sz</t>
+  </si>
+  <si>
+    <t>ldz_lat.av</t>
+  </si>
+  <si>
+    <t>ldz_mgc</t>
+  </si>
+  <si>
+    <t>Number of map grid cells in licensee area with grid components, regional distribution</t>
+  </si>
+  <si>
+    <t>Number of map grid cells in licensee area with grid components, local distribution</t>
+  </si>
+  <si>
+    <t>The revenue cap for the cost base year ???</t>
+  </si>
+  <si>
+    <t>lrt_RC_dec.y.cb</t>
   </si>
 </sst>
 </file>
@@ -1693,7 +1831,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1704,6 +1842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dårlig" xfId="1" builtinId="27"/>
@@ -3182,10 +3321,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D146"/>
+  <dimension ref="A2:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3212,1872 +3351,2031 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>345</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>472</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>344</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>484</v>
+        <v>324</v>
       </c>
       <c r="C4" t="s">
-        <v>275</v>
+        <v>496</v>
       </c>
       <c r="D4" t="s">
-        <v>276</v>
+        <v>495</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>296</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>297</v>
+        <v>506</v>
       </c>
       <c r="D5" t="s">
-        <v>300</v>
+        <v>442</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>298</v>
+        <v>507</v>
       </c>
       <c r="D6" t="s">
-        <v>367</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>508</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>206</v>
+        <v>509</v>
       </c>
       <c r="D8" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>440</v>
+        <v>517</v>
       </c>
       <c r="D9" t="s">
-        <v>474</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>66</v>
+      </c>
+      <c r="B10" t="s">
+        <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>510</v>
       </c>
       <c r="D10" t="s">
-        <v>475</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>443</v>
+        <v>511</v>
       </c>
       <c r="D11" t="s">
-        <v>444</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>512</v>
       </c>
       <c r="D12" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>561</v>
+      </c>
+      <c r="B13" t="s">
+        <v>563</v>
       </c>
       <c r="C13" t="s">
-        <v>456</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>454</v>
+        <v>562</v>
+      </c>
+      <c r="D13" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>422</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
-        <v>480</v>
+        <v>513</v>
       </c>
       <c r="D14" t="s">
-        <v>481</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>120</v>
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>197</v>
       </c>
       <c r="C15" t="s">
-        <v>320</v>
+        <v>514</v>
       </c>
       <c r="D15" t="s">
-        <v>482</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>198</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>518</v>
       </c>
       <c r="D16" t="s">
-        <v>483</v>
+        <v>519</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>152</v>
-      </c>
-      <c r="B17" t="s">
-        <v>415</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>416</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>156</v>
+      </c>
+      <c r="B18" t="s">
+        <v>388</v>
       </c>
       <c r="C18" t="s">
-        <v>158</v>
+        <v>440</v>
       </c>
       <c r="D18" t="s">
-        <v>485</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>159</v>
-      </c>
-      <c r="B19" t="s">
-        <v>434</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>152</v>
+      </c>
+      <c r="B20" t="s">
+        <v>381</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>486</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" t="s">
-        <v>200</v>
+        <v>158</v>
       </c>
       <c r="C21" t="s">
-        <v>201</v>
+        <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
+        <v>445</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>205</v>
+        <v>400</v>
       </c>
       <c r="C22" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>204</v>
+        <v>401</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B23" t="s">
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>188</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>189</v>
+        <v>446</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>488</v>
+        <v>406</v>
+      </c>
+      <c r="D24" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>505</v>
+        <v>411</v>
       </c>
       <c r="D25" t="s">
-        <v>506</v>
+        <v>412</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
+        <v>199</v>
       </c>
       <c r="C26" t="s">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="D26" t="s">
-        <v>448</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
+        <v>201</v>
       </c>
       <c r="C27" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="D27" t="s">
-        <v>452</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" t="s">
-        <v>445</v>
-      </c>
-      <c r="D28" t="s">
-        <v>446</v>
+        <v>149</v>
+      </c>
+      <c r="B28" t="s">
+        <v>314</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>204</v>
       </c>
       <c r="C29" t="s">
-        <v>442</v>
+        <v>537</v>
       </c>
       <c r="D29" t="s">
-        <v>489</v>
+        <v>538</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>453</v>
-      </c>
-      <c r="D30" t="s">
-        <v>490</v>
+        <v>112</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>476</v>
+        <v>413</v>
       </c>
       <c r="D31" t="s">
-        <v>477</v>
+        <v>414</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>539</v>
       </c>
       <c r="C32" t="s">
-        <v>478</v>
+        <v>540</v>
       </c>
       <c r="D32" t="s">
-        <v>479</v>
+        <v>541</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" t="s">
-        <v>191</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>192</v>
+        <v>436</v>
       </c>
       <c r="D33" t="s">
-        <v>193</v>
+        <v>437</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" t="s">
-        <v>231</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>232</v>
+        <v>438</v>
       </c>
       <c r="D34" t="s">
-        <v>233</v>
+        <v>439</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>337</v>
+        <v>206</v>
       </c>
       <c r="C35" t="s">
-        <v>340</v>
+        <v>205</v>
       </c>
       <c r="D35" t="s">
-        <v>403</v>
+        <v>524</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>528</v>
       </c>
       <c r="B36" t="s">
-        <v>217</v>
+        <v>530</v>
       </c>
       <c r="C36" t="s">
-        <v>215</v>
+        <v>531</v>
       </c>
       <c r="D36" t="s">
-        <v>216</v>
+        <v>535</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>522</v>
       </c>
       <c r="B37" t="s">
-        <v>336</v>
+        <v>529</v>
       </c>
       <c r="C37" t="s">
-        <v>339</v>
+        <v>523</v>
       </c>
       <c r="D37" t="s">
-        <v>404</v>
+        <v>525</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>532</v>
       </c>
       <c r="B38" t="s">
-        <v>221</v>
+        <v>533</v>
       </c>
       <c r="C38" t="s">
-        <v>48</v>
+        <v>534</v>
       </c>
       <c r="D38" t="s">
-        <v>222</v>
+        <v>536</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>415</v>
       </c>
       <c r="D39" t="s">
-        <v>491</v>
+        <v>416</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>208</v>
       </c>
       <c r="C40" t="s">
-        <v>321</v>
+        <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>492</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="C41" t="s">
-        <v>229</v>
+        <v>515</v>
       </c>
       <c r="D41" t="s">
-        <v>230</v>
+        <v>526</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>147</v>
       </c>
       <c r="C42" t="s">
-        <v>449</v>
+        <v>409</v>
       </c>
       <c r="D42" t="s">
-        <v>450</v>
+        <v>410</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="D43" t="s">
-        <v>497</v>
+        <v>451</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>499</v>
+        <v>294</v>
       </c>
       <c r="D44" t="s">
-        <v>498</v>
+        <v>452</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C45" t="s">
-        <v>493</v>
+        <v>211</v>
       </c>
       <c r="D45" t="s">
-        <v>210</v>
+        <v>462</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C46" t="s">
-        <v>494</v>
+        <v>213</v>
       </c>
       <c r="D46" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>502</v>
       </c>
       <c r="B47" t="s">
-        <v>343</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>213</v>
+        <v>503</v>
+      </c>
+      <c r="C47" t="s">
+        <v>504</v>
+      </c>
+      <c r="D47" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C48" t="s">
-        <v>495</v>
+        <v>216</v>
       </c>
       <c r="D48" t="s">
-        <v>496</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>322</v>
+        <v>408</v>
       </c>
       <c r="D49" t="s">
-        <v>501</v>
+        <v>449</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>75</v>
+      </c>
+      <c r="B50" t="s">
+        <v>218</v>
       </c>
       <c r="C50" t="s">
-        <v>323</v>
+        <v>520</v>
       </c>
       <c r="D50" t="s">
-        <v>500</v>
+        <v>521</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" t="s">
-        <v>234</v>
+        <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>235</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
-        <v>502</v>
+        <v>455</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>47</v>
-      </c>
-      <c r="B52" t="s">
-        <v>236</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B52" s="6"/>
       <c r="C52" t="s">
-        <v>237</v>
+        <v>295</v>
       </c>
       <c r="D52" t="s">
-        <v>503</v>
+        <v>459</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>195</v>
+        <v>296</v>
       </c>
       <c r="D53" t="s">
-        <v>196</v>
+        <v>458</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="C54" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="D54" t="s">
-        <v>199</v>
+        <v>460</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="C55" t="s">
-        <v>186</v>
+        <v>222</v>
       </c>
       <c r="D55" t="s">
-        <v>187</v>
+        <v>461</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>223</v>
+        <v>306</v>
       </c>
       <c r="C56" t="s">
-        <v>224</v>
+        <v>309</v>
       </c>
       <c r="D56" t="s">
-        <v>504</v>
+        <v>466</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>225</v>
+        <v>307</v>
       </c>
       <c r="C57" t="s">
-        <v>226</v>
+        <v>310</v>
       </c>
       <c r="D57" t="s">
-        <v>227</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>140</v>
+      </c>
+      <c r="B58" t="s">
+        <v>308</v>
       </c>
       <c r="C58" t="s">
-        <v>441</v>
+        <v>311</v>
       </c>
       <c r="D58" t="s">
-        <v>507</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>9</v>
-      </c>
-      <c r="B59" t="s">
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
+        <v>463</v>
       </c>
       <c r="D59" t="s">
-        <v>509</v>
+        <v>464</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>138</v>
-      </c>
-      <c r="B60" t="s">
-        <v>335</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>338</v>
+        <v>407</v>
       </c>
       <c r="D60" t="s">
-        <v>508</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>151</v>
-      </c>
-      <c r="B61" t="s">
-        <v>414</v>
+        <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>151</v>
+        <v>417</v>
       </c>
       <c r="D61" t="s">
-        <v>510</v>
+        <v>418</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>457</v>
       </c>
       <c r="D62" t="s">
-        <v>511</v>
+        <v>456</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>151</v>
+      </c>
+      <c r="B63" t="s">
+        <v>380</v>
       </c>
       <c r="C63" t="s">
-        <v>324</v>
+        <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>512</v>
+        <v>468</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>325</v>
+        <v>419</v>
       </c>
       <c r="D64" t="s">
-        <v>513</v>
+        <v>450</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>326</v>
+        <v>72</v>
       </c>
       <c r="D65" t="s">
-        <v>514</v>
+        <v>469</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" t="s">
-        <v>378</v>
+        <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>397</v>
-      </c>
-      <c r="D66" t="s">
-        <v>515</v>
+        <v>516</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>119</v>
-      </c>
-      <c r="B67" t="s">
-        <v>286</v>
+        <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>257</v>
+        <v>297</v>
       </c>
       <c r="D67" t="s">
-        <v>291</v>
+        <v>470</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>101</v>
-      </c>
-      <c r="B68" t="s">
-        <v>287</v>
+        <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
       <c r="D68" t="s">
-        <v>292</v>
+        <v>472</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>114</v>
-      </c>
-      <c r="B69" t="s">
-        <v>240</v>
+        <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>238</v>
+        <v>298</v>
       </c>
       <c r="D69" t="s">
-        <v>239</v>
+        <v>471</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>572</v>
       </c>
       <c r="B70" t="s">
-        <v>243</v>
+        <v>574</v>
       </c>
       <c r="C70" t="s">
-        <v>241</v>
+        <v>577</v>
       </c>
       <c r="D70" t="s">
-        <v>242</v>
+        <v>579</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>246</v>
+        <v>300</v>
       </c>
       <c r="C71" t="s">
-        <v>244</v>
+        <v>575</v>
       </c>
       <c r="D71" t="s">
-        <v>245</v>
+        <v>302</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>252</v>
+        <v>301</v>
       </c>
       <c r="C72" t="s">
-        <v>392</v>
+        <v>576</v>
       </c>
       <c r="D72" t="s">
-        <v>516</v>
+        <v>303</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>251</v>
+        <v>225</v>
       </c>
       <c r="C73" t="s">
-        <v>393</v>
+        <v>223</v>
       </c>
       <c r="D73" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>289</v>
+        <v>228</v>
       </c>
       <c r="C74" t="s">
-        <v>256</v>
+        <v>226</v>
       </c>
       <c r="D74" t="s">
-        <v>290</v>
+        <v>227</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B75" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="C75" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="D75" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>327</v>
+        <v>233</v>
       </c>
       <c r="C76" t="s">
-        <v>329</v>
+        <v>558</v>
       </c>
       <c r="D76" t="s">
-        <v>331</v>
+        <v>232</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>328</v>
+        <v>235</v>
       </c>
       <c r="C77" t="s">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="D77" t="s">
-        <v>332</v>
+        <v>234</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>288</v>
+        <v>236</v>
       </c>
       <c r="C78" t="s">
-        <v>261</v>
+        <v>359</v>
       </c>
       <c r="D78" t="s">
-        <v>293</v>
+        <v>474</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B79" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="C79" t="s">
-        <v>253</v>
+        <v>559</v>
       </c>
       <c r="D79" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>553</v>
       </c>
       <c r="B80" t="s">
-        <v>260</v>
+        <v>554</v>
       </c>
       <c r="C80" t="s">
-        <v>259</v>
+        <v>555</v>
       </c>
       <c r="D80" t="s">
-        <v>294</v>
+        <v>556</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C81" t="s">
-        <v>394</v>
+        <v>546</v>
       </c>
       <c r="D81" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>265</v>
+      <c r="C82" t="s">
+        <v>547</v>
+      </c>
+      <c r="D82" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>154</v>
+        <v>565</v>
       </c>
       <c r="B83" t="s">
-        <v>419</v>
+        <v>566</v>
       </c>
       <c r="C83" t="s">
-        <v>417</v>
+        <v>567</v>
       </c>
       <c r="D83" t="s">
-        <v>418</v>
+        <v>566</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>172</v>
+        <v>102</v>
       </c>
       <c r="B84" t="s">
-        <v>433</v>
+        <v>237</v>
       </c>
       <c r="C84" t="s">
-        <v>409</v>
+        <v>568</v>
       </c>
       <c r="D84" t="s">
-        <v>517</v>
+        <v>569</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>527</v>
+        <v>110</v>
+      </c>
+      <c r="B85" t="s">
+        <v>263</v>
       </c>
       <c r="C85" t="s">
-        <v>527</v>
+        <v>557</v>
       </c>
       <c r="D85" t="s">
-        <v>528</v>
+        <v>268</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
       <c r="B86" t="s">
-        <v>420</v>
+        <v>238</v>
       </c>
       <c r="C86" t="s">
-        <v>455</v>
+        <v>560</v>
       </c>
       <c r="D86" t="s">
-        <v>529</v>
+        <v>269</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>175</v>
+        <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>427</v>
+        <v>240</v>
       </c>
       <c r="C87" t="s">
-        <v>429</v>
+        <v>361</v>
       </c>
       <c r="D87" t="s">
-        <v>431</v>
+        <v>239</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>548</v>
       </c>
       <c r="B88" t="s">
-        <v>428</v>
+        <v>549</v>
       </c>
       <c r="C88" t="s">
-        <v>430</v>
+        <v>550</v>
       </c>
       <c r="D88" t="s">
-        <v>432</v>
+        <v>551</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>165</v>
-      </c>
-      <c r="C89" t="s">
-        <v>165</v>
-      </c>
-      <c r="D89" t="s">
-        <v>519</v>
+      <c r="A89" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B90" t="s">
-        <v>424</v>
+        <v>378</v>
       </c>
       <c r="C90" t="s">
-        <v>399</v>
+        <v>371</v>
       </c>
       <c r="D90" t="s">
-        <v>425</v>
+        <v>373</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B91" t="s">
-        <v>423</v>
+        <v>379</v>
       </c>
       <c r="C91" t="s">
-        <v>400</v>
+        <v>372</v>
       </c>
       <c r="D91" t="s">
-        <v>426</v>
+        <v>374</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>34</v>
+        <v>154</v>
+      </c>
+      <c r="B92" t="s">
+        <v>385</v>
       </c>
       <c r="C92" t="s">
-        <v>457</v>
+        <v>383</v>
       </c>
       <c r="D92" t="s">
-        <v>458</v>
+        <v>384</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>485</v>
       </c>
       <c r="C93" t="s">
-        <v>167</v>
+        <v>485</v>
       </c>
       <c r="D93" t="s">
-        <v>518</v>
+        <v>486</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>170</v>
+        <v>153</v>
+      </c>
+      <c r="B94" t="s">
+        <v>386</v>
       </c>
       <c r="C94" t="s">
-        <v>533</v>
+        <v>420</v>
       </c>
       <c r="D94" t="s">
-        <v>522</v>
+        <v>487</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>168</v>
+        <v>172</v>
+      </c>
+      <c r="B95" t="s">
+        <v>399</v>
       </c>
       <c r="C95" t="s">
-        <v>168</v>
+        <v>375</v>
       </c>
       <c r="D95" t="s">
-        <v>530</v>
+        <v>475</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>169</v>
+        <v>175</v>
+      </c>
+      <c r="B96" t="s">
+        <v>393</v>
       </c>
       <c r="C96" t="s">
-        <v>169</v>
+        <v>395</v>
       </c>
       <c r="D96" t="s">
-        <v>520</v>
+        <v>397</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B97" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C97" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="D97" t="s">
-        <v>521</v>
+        <v>398</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B98" t="s">
-        <v>412</v>
+        <v>390</v>
       </c>
       <c r="C98" t="s">
-        <v>405</v>
+        <v>365</v>
       </c>
       <c r="D98" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B99" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="C99" t="s">
-        <v>406</v>
+        <v>366</v>
       </c>
       <c r="D99" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>155</v>
-      </c>
-      <c r="B100" t="s">
-        <v>421</v>
-      </c>
-      <c r="C100" t="s">
-        <v>531</v>
-      </c>
-      <c r="D100" t="s">
-        <v>532</v>
+      <c r="A100" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C101" t="s">
-        <v>459</v>
+        <v>165</v>
       </c>
       <c r="D101" t="s">
-        <v>526</v>
+        <v>477</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C102" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D102" t="s">
-        <v>525</v>
+        <v>476</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C103" t="s">
-        <v>402</v>
+        <v>491</v>
       </c>
       <c r="D103" t="s">
-        <v>524</v>
+        <v>480</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C104" t="s">
-        <v>401</v>
+        <v>168</v>
       </c>
       <c r="D104" t="s">
-        <v>523</v>
+        <v>488</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>92</v>
+      <c r="A105" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="C105" t="s">
-        <v>460</v>
+        <v>169</v>
       </c>
       <c r="D105" t="s">
-        <v>462</v>
+        <v>478</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>96</v>
+        <v>171</v>
+      </c>
+      <c r="B106" t="s">
+        <v>376</v>
       </c>
       <c r="C106" t="s">
-        <v>461</v>
+        <v>377</v>
       </c>
       <c r="D106" t="s">
-        <v>463</v>
+        <v>479</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>60</v>
+        <v>155</v>
+      </c>
+      <c r="B107" t="s">
+        <v>387</v>
       </c>
       <c r="C107" t="s">
-        <v>464</v>
+        <v>489</v>
       </c>
       <c r="D107" t="s">
-        <v>465</v>
+        <v>490</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>33</v>
-      </c>
-      <c r="B108" t="s">
-        <v>395</v>
+        <v>164</v>
       </c>
       <c r="C108" t="s">
-        <v>473</v>
+        <v>421</v>
       </c>
       <c r="D108" t="s">
-        <v>396</v>
+        <v>484</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>18</v>
-      </c>
-      <c r="B109" t="s">
-        <v>341</v>
+        <v>174</v>
       </c>
       <c r="C109" t="s">
-        <v>18</v>
+        <v>368</v>
       </c>
       <c r="D109" t="s">
-        <v>342</v>
+        <v>482</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>1</v>
-      </c>
-      <c r="B110" t="s">
-        <v>278</v>
+        <v>163</v>
       </c>
       <c r="C110" t="s">
-        <v>1</v>
+        <v>367</v>
       </c>
       <c r="D110" t="s">
-        <v>277</v>
+        <v>481</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>10</v>
-      </c>
-      <c r="B111" t="s">
-        <v>281</v>
+        <v>166</v>
       </c>
       <c r="C111" t="s">
-        <v>279</v>
+        <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>280</v>
+        <v>483</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="C112" t="s">
-        <v>398</v>
+        <v>422</v>
       </c>
       <c r="D112" t="s">
-        <v>534</v>
+        <v>424</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>21</v>
-      </c>
-      <c r="B113" t="s">
-        <v>334</v>
+        <v>96</v>
       </c>
       <c r="C113" t="s">
-        <v>535</v>
+        <v>423</v>
       </c>
       <c r="D113" t="s">
-        <v>333</v>
+        <v>425</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>364</v>
+        <v>403</v>
       </c>
       <c r="C114" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="D114" t="s">
-        <v>363</v>
+        <v>402</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="D115" s="4" t="s">
-        <v>350</v>
+      <c r="A115" t="s">
+        <v>60</v>
+      </c>
+      <c r="C115" t="s">
+        <v>426</v>
+      </c>
+      <c r="D115" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4" t="s">
-        <v>467</v>
-      </c>
-      <c r="D116" s="4"/>
+      <c r="A116" t="s">
+        <v>33</v>
+      </c>
+      <c r="B116" t="s">
+        <v>362</v>
+      </c>
+      <c r="C116" t="s">
+        <v>497</v>
+      </c>
+      <c r="D116" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>466</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>362</v>
+      <c r="A117" t="s">
+        <v>18</v>
+      </c>
+      <c r="B117" t="s">
+        <v>312</v>
+      </c>
+      <c r="C117" t="s">
+        <v>18</v>
+      </c>
+      <c r="D117" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>469</v>
-      </c>
-      <c r="D118" s="4" t="s">
-        <v>361</v>
+      <c r="A118" t="s">
+        <v>25</v>
+      </c>
+      <c r="B118" t="s">
+        <v>270</v>
+      </c>
+      <c r="C118" t="s">
+        <v>354</v>
+      </c>
+      <c r="D118" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="C119" t="s">
-        <v>282</v>
+        <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C120" t="s">
-        <v>388</v>
+        <v>254</v>
       </c>
       <c r="D120" t="s">
-        <v>382</v>
+        <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>269</v>
+        <v>405</v>
       </c>
       <c r="C121" t="s">
-        <v>389</v>
+        <v>327</v>
       </c>
       <c r="D121" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="B122" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C122" t="s">
-        <v>390</v>
+        <v>272</v>
       </c>
       <c r="D122" t="s">
-        <v>385</v>
+        <v>275</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C123" t="s">
-        <v>391</v>
+        <v>273</v>
       </c>
       <c r="D123" t="s">
-        <v>383</v>
+        <v>336</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>123</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C124" t="s">
-        <v>319</v>
-      </c>
-      <c r="D124" t="s">
-        <v>318</v>
-      </c>
+      <c r="A124" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>125</v>
-      </c>
-      <c r="B125" t="s">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>271</v>
+        <v>364</v>
       </c>
       <c r="D125" t="s">
-        <v>272</v>
+        <v>492</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>148</v>
-      </c>
-      <c r="B126" t="s">
-        <v>274</v>
-      </c>
-      <c r="C126" t="s">
-        <v>315</v>
-      </c>
-      <c r="D126" t="s">
-        <v>316</v>
+      <c r="A126" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="C127" t="s">
-        <v>32</v>
+        <v>493</v>
       </c>
       <c r="D127" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B128" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>320</v>
+      </c>
       <c r="C128" s="4" t="s">
-        <v>468</v>
+        <v>322</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>471</v>
+        <v>321</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>58</v>
-      </c>
-      <c r="B129" t="s">
-        <v>373</v>
-      </c>
-      <c r="C129" t="s">
-        <v>371</v>
-      </c>
-      <c r="D129" t="s">
-        <v>380</v>
+      <c r="A129" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>41</v>
-      </c>
-      <c r="B130" t="s">
-        <v>375</v>
-      </c>
-      <c r="C130" t="s">
-        <v>369</v>
-      </c>
-      <c r="D130" t="s">
-        <v>365</v>
+      <c r="A130" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B131" t="s">
-        <v>376</v>
+        <v>333</v>
       </c>
       <c r="C131" t="s">
-        <v>368</v>
+        <v>323</v>
       </c>
       <c r="D131" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>374</v>
+        <v>316</v>
       </c>
       <c r="C132" t="s">
-        <v>370</v>
+        <v>433</v>
       </c>
       <c r="D132" t="s">
-        <v>379</v>
+        <v>315</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>73</v>
+        <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>377</v>
+        <v>259</v>
       </c>
       <c r="C133" t="s">
-        <v>372</v>
+        <v>257</v>
       </c>
       <c r="D133" t="s">
-        <v>381</v>
+        <v>258</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="B134" t="s">
-        <v>355</v>
+        <v>243</v>
       </c>
       <c r="C134" t="s">
-        <v>353</v>
+        <v>542</v>
       </c>
       <c r="D134" t="s">
-        <v>354</v>
+        <v>543</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B135" t="s">
-        <v>305</v>
+        <v>244</v>
       </c>
       <c r="C135" t="s">
-        <v>309</v>
+        <v>358</v>
       </c>
       <c r="D135" t="s">
-        <v>301</v>
+        <v>351</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B136" t="s">
-        <v>306</v>
+        <v>245</v>
       </c>
       <c r="C136" t="s">
-        <v>311</v>
+        <v>356</v>
       </c>
       <c r="D136" t="s">
-        <v>302</v>
+        <v>352</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="B137" t="s">
-        <v>8</v>
+        <v>246</v>
       </c>
       <c r="C137" t="s">
-        <v>89</v>
+        <v>357</v>
       </c>
       <c r="D137" t="s">
-        <v>285</v>
+        <v>353</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>88</v>
-      </c>
-      <c r="B138" t="s">
-        <v>307</v>
-      </c>
-      <c r="C138" t="s">
-        <v>310</v>
-      </c>
-      <c r="D138" t="s">
-        <v>303</v>
-      </c>
+      <c r="A138" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B138" s="4"/>
+      <c r="C138" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="D138" s="4"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>22</v>
-      </c>
-      <c r="B139" t="s">
-        <v>346</v>
-      </c>
-      <c r="C139" t="s">
-        <v>359</v>
-      </c>
-      <c r="D139" t="s">
-        <v>347</v>
-      </c>
+      <c r="A139" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B139" s="4"/>
+      <c r="C139" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="D139" s="4"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="C140" t="s">
-        <v>312</v>
+        <v>32</v>
       </c>
       <c r="D140" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>23</v>
+        <v>570</v>
       </c>
       <c r="B141" t="s">
-        <v>437</v>
+        <v>571</v>
       </c>
       <c r="C141" t="s">
-        <v>357</v>
+        <v>573</v>
       </c>
       <c r="D141" t="s">
-        <v>436</v>
+        <v>578</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>25</v>
-      </c>
-      <c r="B142" t="s">
-        <v>295</v>
+        <v>123</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="C142" t="s">
-        <v>386</v>
+        <v>293</v>
       </c>
       <c r="D142" t="s">
-        <v>387</v>
+        <v>292</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>24</v>
+        <v>125</v>
       </c>
       <c r="B143" t="s">
-        <v>439</v>
+        <v>248</v>
       </c>
       <c r="C143" t="s">
-        <v>358</v>
+        <v>544</v>
       </c>
       <c r="D143" t="s">
-        <v>438</v>
+        <v>247</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
+      <c r="A144" t="s">
+        <v>148</v>
+      </c>
+      <c r="B144" t="s">
+        <v>249</v>
+      </c>
+      <c r="C144" t="s">
+        <v>545</v>
+      </c>
+      <c r="D144" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
+      <c r="A145" t="s">
+        <v>7</v>
+      </c>
+      <c r="B145" t="s">
+        <v>444</v>
+      </c>
+      <c r="C145" t="s">
+        <v>250</v>
+      </c>
+      <c r="D145" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B146" s="4"/>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
+      <c r="A146" t="s">
+        <v>22</v>
+      </c>
+      <c r="B146" t="s">
+        <v>317</v>
+      </c>
+      <c r="C146" t="s">
+        <v>328</v>
+      </c>
+      <c r="D146" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B147" s="4"/>
+      <c r="C147" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>58</v>
+      </c>
+      <c r="B148" t="s">
+        <v>342</v>
+      </c>
+      <c r="C148" t="s">
+        <v>340</v>
+      </c>
+      <c r="D148" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>56</v>
+      </c>
+      <c r="B149" t="s">
+        <v>343</v>
+      </c>
+      <c r="C149" t="s">
+        <v>339</v>
+      </c>
+      <c r="D149" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>41</v>
+      </c>
+      <c r="B150" t="s">
+        <v>344</v>
+      </c>
+      <c r="C150" t="s">
+        <v>338</v>
+      </c>
+      <c r="D150" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>44</v>
+      </c>
+      <c r="B151" t="s">
+        <v>345</v>
+      </c>
+      <c r="C151" t="s">
+        <v>337</v>
+      </c>
+      <c r="D151" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>73</v>
+      </c>
+      <c r="B152" t="s">
+        <v>346</v>
+      </c>
+      <c r="C152" t="s">
+        <v>341</v>
+      </c>
+      <c r="D152" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>26</v>
+      </c>
+      <c r="B153" t="s">
+        <v>347</v>
+      </c>
+      <c r="C153" t="s">
+        <v>363</v>
+      </c>
+      <c r="D153" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>87</v>
+      </c>
+      <c r="B154" t="s">
+        <v>280</v>
+      </c>
+      <c r="C154" t="s">
+        <v>284</v>
+      </c>
+      <c r="D154" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>85</v>
+      </c>
+      <c r="B155" t="s">
+        <v>281</v>
+      </c>
+      <c r="C155" t="s">
+        <v>286</v>
+      </c>
+      <c r="D155" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>88</v>
+      </c>
+      <c r="B156" t="s">
+        <v>282</v>
+      </c>
+      <c r="C156" t="s">
+        <v>285</v>
+      </c>
+      <c r="D156" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>86</v>
+      </c>
+      <c r="B157" t="s">
+        <v>283</v>
+      </c>
+      <c r="C157" t="s">
+        <v>287</v>
+      </c>
+      <c r="D157" t="s">
+        <v>279</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D146">
-    <sortState ref="A3:D145">
-      <sortCondition ref="C2:C145"/>
+  <autoFilter ref="A2:D157">
+    <sortState ref="A3:D154">
+      <sortCondition ref="A2:A154"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
translate ok including CPI/CPI.L adjustment
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -1336,9 +1336,6 @@
     <t>Costs of grid components in interface, regional and distribution grid</t>
   </si>
   <si>
-    <t>d_gci.dummy</t>
-  </si>
-  <si>
     <t>Dummy equal to one if gci &gt; 0</t>
   </si>
   <si>
@@ -1775,6 +1772,9 @@
   </si>
   <si>
     <t>ap.t_2</t>
+  </si>
+  <si>
+    <t>ld_gci.dummy</t>
   </si>
 </sst>
 </file>
@@ -3323,8 +3323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3371,10 +3371,10 @@
         <v>324</v>
       </c>
       <c r="C4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3382,10 +3382,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3396,7 +3396,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3410,10 +3410,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3424,7 +3424,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3438,7 +3438,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3452,7 +3452,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3466,7 +3466,7 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D11" t="s">
         <v>191</v>
@@ -3480,7 +3480,7 @@
         <v>192</v>
       </c>
       <c r="C12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D12" t="s">
         <v>193</v>
@@ -3488,16 +3488,16 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>555</v>
+      </c>
+      <c r="B13" t="s">
+        <v>557</v>
+      </c>
+      <c r="C13" t="s">
         <v>556</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>558</v>
-      </c>
-      <c r="C13" t="s">
-        <v>557</v>
-      </c>
-      <c r="D13" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3508,7 +3508,7 @@
         <v>194</v>
       </c>
       <c r="C14" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D14" t="s">
         <v>195</v>
@@ -3522,7 +3522,7 @@
         <v>197</v>
       </c>
       <c r="C15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D15" t="s">
         <v>196</v>
@@ -3536,10 +3536,10 @@
         <v>198</v>
       </c>
       <c r="C16" t="s">
+        <v>512</v>
+      </c>
+      <c r="D16" t="s">
         <v>513</v>
-      </c>
-      <c r="D16" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3561,10 +3561,10 @@
         <v>388</v>
       </c>
       <c r="C18" t="s">
+        <v>436</v>
+      </c>
+      <c r="D18" t="s">
         <v>437</v>
-      </c>
-      <c r="D18" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3575,7 +3575,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,7 +3600,7 @@
         <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,7 +3625,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3633,10 +3633,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
+        <v>578</v>
+      </c>
+      <c r="D24" t="s">
         <v>579</v>
-      </c>
-      <c r="D24" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,7 +3658,7 @@
         <v>199</v>
       </c>
       <c r="C26" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D26" t="s">
         <v>200</v>
@@ -3672,7 +3672,7 @@
         <v>201</v>
       </c>
       <c r="C27" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D27" t="s">
         <v>202</v>
@@ -3686,7 +3686,7 @@
         <v>314</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>203</v>
@@ -3700,10 +3700,10 @@
         <v>204</v>
       </c>
       <c r="C29" t="s">
+        <v>531</v>
+      </c>
+      <c r="D29" t="s">
         <v>532</v>
-      </c>
-      <c r="D29" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3714,7 +3714,7 @@
         <v>112</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3730,13 +3730,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>533</v>
+      </c>
+      <c r="C32" t="s">
         <v>534</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>535</v>
-      </c>
-      <c r="D32" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3755,10 +3755,10 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
+        <v>581</v>
+      </c>
+      <c r="D34" t="s">
         <v>435</v>
-      </c>
-      <c r="D34" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3772,49 +3772,49 @@
         <v>205</v>
       </c>
       <c r="D35" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B36" t="s">
+        <v>524</v>
+      </c>
+      <c r="C36" t="s">
         <v>525</v>
       </c>
-      <c r="C36" t="s">
-        <v>526</v>
-      </c>
       <c r="D36" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>516</v>
+      </c>
+      <c r="B37" t="s">
+        <v>523</v>
+      </c>
+      <c r="C37" t="s">
         <v>517</v>
       </c>
-      <c r="B37" t="s">
-        <v>524</v>
-      </c>
-      <c r="C37" t="s">
-        <v>518</v>
-      </c>
       <c r="D37" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>526</v>
+      </c>
+      <c r="B38" t="s">
         <v>527</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>528</v>
       </c>
-      <c r="C38" t="s">
-        <v>529</v>
-      </c>
       <c r="D38" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3850,10 +3850,10 @@
         <v>207</v>
       </c>
       <c r="C41" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D41" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3875,7 +3875,7 @@
         <v>93</v>
       </c>
       <c r="D43" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3886,7 +3886,7 @@
         <v>294</v>
       </c>
       <c r="D44" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3900,7 +3900,7 @@
         <v>211</v>
       </c>
       <c r="D45" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3919,16 +3919,16 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>496</v>
+      </c>
+      <c r="B47" t="s">
         <v>497</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>498</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>499</v>
-      </c>
-      <c r="D47" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3953,7 +3953,7 @@
         <v>407</v>
       </c>
       <c r="D49" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3964,10 +3964,10 @@
         <v>218</v>
       </c>
       <c r="C50" t="s">
+        <v>514</v>
+      </c>
+      <c r="D50" t="s">
         <v>515</v>
-      </c>
-      <c r="D50" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3975,10 +3975,10 @@
         <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D51" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3990,7 +3990,7 @@
         <v>295</v>
       </c>
       <c r="D52" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4001,7 +4001,7 @@
         <v>296</v>
       </c>
       <c r="D53" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4015,7 +4015,7 @@
         <v>220</v>
       </c>
       <c r="D54" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4029,7 +4029,7 @@
         <v>222</v>
       </c>
       <c r="D55" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4043,7 +4043,7 @@
         <v>309</v>
       </c>
       <c r="D56" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4079,10 +4079,10 @@
         <v>113</v>
       </c>
       <c r="C59" t="s">
+        <v>457</v>
+      </c>
+      <c r="D59" t="s">
         <v>458</v>
-      </c>
-      <c r="D59" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4093,7 +4093,7 @@
         <v>406</v>
       </c>
       <c r="D60" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4112,10 +4112,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>136</v>
+        <v>577</v>
       </c>
       <c r="D62" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4129,7 +4129,7 @@
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4140,7 +4140,7 @@
         <v>418</v>
       </c>
       <c r="D64" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4151,7 +4151,7 @@
         <v>72</v>
       </c>
       <c r="D65" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4159,10 +4159,10 @@
         <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4173,7 +4173,7 @@
         <v>297</v>
       </c>
       <c r="D67" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4184,7 +4184,7 @@
         <v>299</v>
       </c>
       <c r="D68" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4195,21 +4195,21 @@
         <v>298</v>
       </c>
       <c r="D69" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B70" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C70" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D70" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4220,7 +4220,7 @@
         <v>300</v>
       </c>
       <c r="C71" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D71" t="s">
         <v>302</v>
@@ -4234,7 +4234,7 @@
         <v>301</v>
       </c>
       <c r="C72" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D72" t="s">
         <v>303</v>
@@ -4290,7 +4290,7 @@
         <v>233</v>
       </c>
       <c r="C76" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D76" t="s">
         <v>232</v>
@@ -4321,7 +4321,7 @@
         <v>359</v>
       </c>
       <c r="D78" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4332,7 +4332,7 @@
         <v>264</v>
       </c>
       <c r="C79" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D79" t="s">
         <v>265</v>
@@ -4340,16 +4340,16 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>547</v>
+      </c>
+      <c r="B80" t="s">
         <v>548</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>549</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>550</v>
-      </c>
-      <c r="D80" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4360,7 +4360,7 @@
         <v>261</v>
       </c>
       <c r="C81" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D81" t="s">
         <v>266</v>
@@ -4374,7 +4374,7 @@
         <v>262</v>
       </c>
       <c r="C82" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D82" t="s">
         <v>267</v>
@@ -4382,16 +4382,16 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>559</v>
+      </c>
+      <c r="B83" t="s">
         <v>560</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>561</v>
       </c>
-      <c r="C83" t="s">
-        <v>562</v>
-      </c>
       <c r="D83" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4402,10 +4402,10 @@
         <v>237</v>
       </c>
       <c r="C84" t="s">
+        <v>562</v>
+      </c>
+      <c r="D84" t="s">
         <v>563</v>
-      </c>
-      <c r="D84" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4416,7 +4416,7 @@
         <v>263</v>
       </c>
       <c r="C85" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D85" t="s">
         <v>268</v>
@@ -4430,7 +4430,7 @@
         <v>238</v>
       </c>
       <c r="C86" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D86" t="s">
         <v>269</v>
@@ -4452,16 +4452,16 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>542</v>
+      </c>
+      <c r="B88" t="s">
         <v>543</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>544</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>545</v>
-      </c>
-      <c r="D88" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4475,7 +4475,7 @@
         <v>241</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4522,13 +4522,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>479</v>
+      </c>
+      <c r="C93" t="s">
+        <v>479</v>
+      </c>
+      <c r="D93" t="s">
         <v>480</v>
-      </c>
-      <c r="C93" t="s">
-        <v>480</v>
-      </c>
-      <c r="D93" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4542,7 +4542,7 @@
         <v>419</v>
       </c>
       <c r="D94" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4556,7 +4556,7 @@
         <v>375</v>
       </c>
       <c r="D95" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4621,10 +4621,10 @@
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4635,7 +4635,7 @@
         <v>165</v>
       </c>
       <c r="D101" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4646,7 +4646,7 @@
         <v>167</v>
       </c>
       <c r="D102" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4654,10 +4654,10 @@
         <v>170</v>
       </c>
       <c r="C103" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D103" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4668,7 +4668,7 @@
         <v>168</v>
       </c>
       <c r="D104" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4679,7 +4679,7 @@
         <v>169</v>
       </c>
       <c r="D105" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4693,7 +4693,7 @@
         <v>377</v>
       </c>
       <c r="D106" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4704,10 +4704,10 @@
         <v>387</v>
       </c>
       <c r="C107" t="s">
+        <v>483</v>
+      </c>
+      <c r="D107" t="s">
         <v>484</v>
-      </c>
-      <c r="D107" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4718,7 +4718,7 @@
         <v>420</v>
       </c>
       <c r="D108" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4729,7 +4729,7 @@
         <v>368</v>
       </c>
       <c r="D109" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4740,7 +4740,7 @@
         <v>367</v>
       </c>
       <c r="D110" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4751,7 +4751,7 @@
         <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4809,10 +4809,10 @@
         <v>362</v>
       </c>
       <c r="C116" t="s">
+        <v>491</v>
+      </c>
+      <c r="D116" t="s">
         <v>492</v>
-      </c>
-      <c r="D116" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4931,7 +4931,7 @@
         <v>364</v>
       </c>
       <c r="D125" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4942,10 +4942,10 @@
         <v>430</v>
       </c>
       <c r="C126" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="D126" s="4" t="s">
         <v>495</v>
-      </c>
-      <c r="D126" s="4" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>305</v>
       </c>
       <c r="C127" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D127" t="s">
         <v>304</v>
@@ -5026,7 +5026,7 @@
         <v>316</v>
       </c>
       <c r="C132" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D132" t="s">
         <v>315</v>
@@ -5054,10 +5054,10 @@
         <v>243</v>
       </c>
       <c r="C134" t="s">
+        <v>536</v>
+      </c>
+      <c r="D134" t="s">
         <v>537</v>
-      </c>
-      <c r="D134" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D138" s="4"/>
     </row>
@@ -5138,16 +5138,16 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>564</v>
+      </c>
+      <c r="B141" t="s">
         <v>565</v>
       </c>
-      <c r="B141" t="s">
-        <v>566</v>
-      </c>
       <c r="C141" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D141" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -5172,7 +5172,7 @@
         <v>248</v>
       </c>
       <c r="C143" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D143" t="s">
         <v>247</v>
@@ -5186,7 +5186,7 @@
         <v>249</v>
       </c>
       <c r="C144" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D144" t="s">
         <v>290</v>
@@ -5197,7 +5197,7 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C145" t="s">
         <v>250</v>
@@ -5226,7 +5226,7 @@
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D147" s="4" t="s">
         <v>431</v>
@@ -5313,7 +5313,7 @@
         <v>363</v>
       </c>
       <c r="D153" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
0_2_Calculated input values translated
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -604,9 +604,6 @@
     <t>Avkastningsgrunnlag egenfinansiert Dnett inkl 1% arbeidskapital</t>
   </si>
   <si>
-    <t>Regulatory asset base, including 1% working capital</t>
-  </si>
-  <si>
     <t>Sum avkastningsgrunnlag DEA Dnett inkl 1% arbeidskapital</t>
   </si>
   <si>
@@ -1039,9 +1036,6 @@
     <t xml:space="preserve">Vector containing variables that are to be adjusted with CPI (labor) </t>
   </si>
   <si>
-    <t>Price index with labor as the dominant factor (Norwegian)</t>
-  </si>
-  <si>
     <t>v_cpi.l</t>
   </si>
   <si>
@@ -1051,9 +1045,6 @@
     <t>v_hist</t>
   </si>
   <si>
-    <t>v_avg</t>
-  </si>
-  <si>
     <t>v_sf</t>
   </si>
   <si>
@@ -1078,9 +1069,6 @@
     <t>Vector containing variables that are to be averaged for historical years</t>
   </si>
   <si>
-    <t>Vector containing variables that are to be averaged</t>
-  </si>
-  <si>
     <t>Vector containing variables that are to be used in the construction of the average fronts</t>
   </si>
   <si>
@@ -1306,12 +1294,6 @@
     <t>DEA score stage 1, only including 5 year historical averages</t>
   </si>
   <si>
-    <t>fp_d_pcb</t>
-  </si>
-  <si>
-    <t>Pension costs base included in the operation and maintanance costs</t>
-  </si>
-  <si>
     <t>NVE.ir.t</t>
   </si>
   <si>
@@ -1330,9 +1312,6 @@
     <t>Results of stage 3 calibration</t>
   </si>
   <si>
-    <t>d_gci.cost</t>
-  </si>
-  <si>
     <t>Costs of grid components in interface, regional and distribution grid</t>
   </si>
   <si>
@@ -1381,9 +1360,6 @@
     <t>d_opex</t>
   </si>
   <si>
-    <t>d_OPEX</t>
-  </si>
-  <si>
     <t>Data frame for companies that are exempted from the regular model, critereas described in … (out of the ordinary)</t>
   </si>
   <si>
@@ -1546,9 +1522,6 @@
     <t>ld_gfa</t>
   </si>
   <si>
-    <t>ld_rab</t>
-  </si>
-  <si>
     <t>ld_RAB</t>
   </si>
   <si>
@@ -1624,9 +1597,6 @@
     <t>Kilometers highvoltage sea cabel in local distribution grid</t>
   </si>
   <si>
-    <t>d_OPEXxS</t>
-  </si>
-  <si>
     <t>Operation and maintenence costs, with salaries and pension costs excluded</t>
   </si>
   <si>
@@ -1775,6 +1745,36 @@
   </si>
   <si>
     <t>ld_gci.dummy</t>
+  </si>
+  <si>
+    <t>ld_gci.cost</t>
+  </si>
+  <si>
+    <t>Consumer Price Index, CPI by delivery sector, Services where labor dominates (Norwegian)</t>
+  </si>
+  <si>
+    <t>ld_OPEX</t>
+  </si>
+  <si>
+    <t>ld_OPEXxS</t>
+  </si>
+  <si>
+    <t>Vector with pensions variables averaged over five years before inclusion in OPEX</t>
+  </si>
+  <si>
+    <t>v_av.pen</t>
+  </si>
+  <si>
+    <t>Pension costs base included in the operation and maintanance costs, average values on fixed prices</t>
+  </si>
+  <si>
+    <t>fp_ld_pcb</t>
+  </si>
+  <si>
+    <t>ld_rab.sf</t>
+  </si>
+  <si>
+    <t>Regulatory asset base self funded assets, including 1% working capital</t>
   </si>
 </sst>
 </file>
@@ -1831,7 +1831,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1843,6 +1843,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dårlig" xfId="1" builtinId="27"/>
@@ -3323,8 +3324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3360,7 +3361,7 @@
         <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3368,13 +3369,13 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C4" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="D4" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3382,10 +3383,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="D5" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3396,7 +3397,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3410,10 +3411,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="D7" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3424,7 +3425,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3438,7 +3439,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3452,7 +3453,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3466,10 +3467,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>505</v>
+        <v>580</v>
       </c>
       <c r="D11" t="s">
-        <v>191</v>
+        <v>581</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3477,27 +3478,27 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" t="s">
+        <v>497</v>
+      </c>
+      <c r="D12" t="s">
         <v>192</v>
-      </c>
-      <c r="C12" t="s">
-        <v>506</v>
-      </c>
-      <c r="D12" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="B13" t="s">
-        <v>557</v>
+        <v>547</v>
       </c>
       <c r="C13" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="D13" t="s">
-        <v>558</v>
+        <v>548</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3505,13 +3506,13 @@
         <v>68</v>
       </c>
       <c r="B14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" t="s">
+        <v>498</v>
+      </c>
+      <c r="D14" t="s">
         <v>194</v>
-      </c>
-      <c r="C14" t="s">
-        <v>507</v>
-      </c>
-      <c r="D14" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3519,13 +3520,13 @@
         <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3533,13 +3534,13 @@
         <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="D16" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3550,21 +3551,21 @@
         <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>156</v>
       </c>
-      <c r="B18" t="s">
-        <v>388</v>
+      <c r="B18" s="6" t="s">
+        <v>384</v>
       </c>
       <c r="C18" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="D18" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3575,7 +3576,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3583,13 +3584,13 @@
         <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C20" t="s">
         <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,7 +3601,7 @@
         <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3608,13 +3609,13 @@
         <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C22" t="s">
         <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3625,7 +3626,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3633,10 +3634,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="D24" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3644,10 +3645,10 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D25" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3655,13 +3656,13 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C26" t="s">
+        <v>442</v>
+      </c>
+      <c r="D26" t="s">
         <v>199</v>
-      </c>
-      <c r="C26" t="s">
-        <v>449</v>
-      </c>
-      <c r="D26" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3669,13 +3670,13 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" t="s">
+        <v>574</v>
+      </c>
+      <c r="D27" t="s">
         <v>201</v>
-      </c>
-      <c r="C27" t="s">
-        <v>450</v>
-      </c>
-      <c r="D27" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3683,13 +3684,13 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3697,13 +3698,13 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C29" t="s">
-        <v>531</v>
+        <v>575</v>
       </c>
       <c r="D29" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3714,7 +3715,7 @@
         <v>112</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,21 +3723,21 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D31" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="C32" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="D32" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3744,10 +3745,10 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>433</v>
+        <v>572</v>
       </c>
       <c r="D33" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3755,10 +3756,10 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="D34" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3766,55 +3767,55 @@
         <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C35" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D35" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="B36" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="C36" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="D36" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="B37" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="C37" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="D37" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="B38" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="C38" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="D38" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3822,10 +3823,10 @@
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D39" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3833,13 +3834,13 @@
         <v>48</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C40" t="s">
         <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3847,13 +3848,13 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C41" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="D41" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3861,10 +3862,10 @@
         <v>147</v>
       </c>
       <c r="C42" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D42" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3875,7 +3876,7 @@
         <v>93</v>
       </c>
       <c r="D43" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3883,10 +3884,10 @@
         <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D44" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,13 +3895,13 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
+        <v>209</v>
+      </c>
+      <c r="C45" t="s">
         <v>210</v>
       </c>
-      <c r="C45" t="s">
-        <v>211</v>
-      </c>
       <c r="D45" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3908,27 +3909,27 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
+        <v>211</v>
+      </c>
+      <c r="C46" t="s">
         <v>212</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>213</v>
-      </c>
-      <c r="D46" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="B47" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="C47" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="D47" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3936,13 +3937,13 @@
         <v>71</v>
       </c>
       <c r="B48" t="s">
+        <v>214</v>
+      </c>
+      <c r="C48" t="s">
         <v>215</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>216</v>
-      </c>
-      <c r="D48" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3950,10 +3951,10 @@
         <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D49" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3961,13 +3962,13 @@
         <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C50" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="D50" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3975,10 +3976,10 @@
         <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="D51" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3987,10 +3988,10 @@
       </c>
       <c r="B52" s="6"/>
       <c r="C52" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D52" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3998,10 +3999,10 @@
         <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D53" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4009,13 +4010,13 @@
         <v>46</v>
       </c>
       <c r="B54" t="s">
+        <v>218</v>
+      </c>
+      <c r="C54" t="s">
         <v>219</v>
       </c>
-      <c r="C54" t="s">
-        <v>220</v>
-      </c>
       <c r="D54" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4023,13 +4024,13 @@
         <v>47</v>
       </c>
       <c r="B55" t="s">
+        <v>220</v>
+      </c>
+      <c r="C55" t="s">
         <v>221</v>
       </c>
-      <c r="C55" t="s">
-        <v>222</v>
-      </c>
       <c r="D55" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4037,13 +4038,13 @@
         <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C56" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D56" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4051,13 +4052,13 @@
         <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C57" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D57" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4065,13 +4066,13 @@
         <v>140</v>
       </c>
       <c r="B58" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C58" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D58" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4079,10 +4080,10 @@
         <v>113</v>
       </c>
       <c r="C59" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="D59" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4090,10 +4091,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D60" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4101,10 +4102,10 @@
         <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D61" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4112,10 +4113,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="D62" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4123,13 +4124,13 @@
         <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C63" t="s">
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4137,10 +4138,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D64" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4151,7 +4152,7 @@
         <v>72</v>
       </c>
       <c r="D65" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4159,10 +4160,10 @@
         <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4170,10 +4171,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D67" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,10 +4182,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D68" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4192,24 +4193,24 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D69" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="B70" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="C70" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="D70" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4217,13 +4218,13 @@
         <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C71" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="D71" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4231,13 +4232,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C72" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
       <c r="D72" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4245,13 +4246,13 @@
         <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C73" t="s">
+        <v>222</v>
+      </c>
+      <c r="D73" t="s">
         <v>223</v>
-      </c>
-      <c r="D73" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4259,13 +4260,13 @@
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C74" t="s">
+        <v>225</v>
+      </c>
+      <c r="D74" t="s">
         <v>226</v>
-      </c>
-      <c r="D74" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4273,13 +4274,13 @@
         <v>116</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C75" t="s">
+        <v>228</v>
+      </c>
+      <c r="D75" t="s">
         <v>229</v>
-      </c>
-      <c r="D75" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4287,13 +4288,13 @@
         <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C76" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="D76" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4301,13 +4302,13 @@
         <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C77" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D77" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4315,13 +4316,13 @@
         <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C78" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D78" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4329,27 +4330,27 @@
         <v>111</v>
       </c>
       <c r="B79" t="s">
+        <v>263</v>
+      </c>
+      <c r="C79" t="s">
+        <v>543</v>
+      </c>
+      <c r="D79" t="s">
         <v>264</v>
-      </c>
-      <c r="C79" t="s">
-        <v>553</v>
-      </c>
-      <c r="D79" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="B80" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="C80" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="D80" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4357,13 +4358,13 @@
         <v>119</v>
       </c>
       <c r="B81" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C81" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="D81" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4371,27 +4372,27 @@
         <v>101</v>
       </c>
       <c r="B82" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C82" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="D82" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>559</v>
+        <v>549</v>
       </c>
       <c r="B83" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="C83" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="D83" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4399,13 +4400,13 @@
         <v>102</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C84" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="D84" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4413,13 +4414,13 @@
         <v>110</v>
       </c>
       <c r="B85" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C85" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="D85" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4427,13 +4428,13 @@
         <v>107</v>
       </c>
       <c r="B86" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C86" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="D86" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4441,27 +4442,27 @@
         <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C87" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D87" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="B88" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="C88" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="D88" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4469,13 +4470,13 @@
         <v>104</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4483,13 +4484,13 @@
         <v>176</v>
       </c>
       <c r="B90" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C90" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D90" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4497,13 +4498,13 @@
         <v>162</v>
       </c>
       <c r="B91" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C91" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D91" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4511,24 +4512,24 @@
         <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C92" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D92" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C93" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="D93" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4536,13 +4537,13 @@
         <v>153</v>
       </c>
       <c r="B94" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C94" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D94" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4550,13 +4551,13 @@
         <v>172</v>
       </c>
       <c r="B95" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C95" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D95" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4564,13 +4565,13 @@
         <v>175</v>
       </c>
       <c r="B96" t="s">
+        <v>389</v>
+      </c>
+      <c r="C96" t="s">
+        <v>391</v>
+      </c>
+      <c r="D96" t="s">
         <v>393</v>
-      </c>
-      <c r="C96" t="s">
-        <v>395</v>
-      </c>
-      <c r="D96" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4578,13 +4579,13 @@
         <v>161</v>
       </c>
       <c r="B97" t="s">
+        <v>390</v>
+      </c>
+      <c r="C97" t="s">
+        <v>392</v>
+      </c>
+      <c r="D97" t="s">
         <v>394</v>
-      </c>
-      <c r="C97" t="s">
-        <v>396</v>
-      </c>
-      <c r="D97" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4592,13 +4593,13 @@
         <v>173</v>
       </c>
       <c r="B98" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C98" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D98" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4606,13 +4607,13 @@
         <v>160</v>
       </c>
       <c r="B99" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C99" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D99" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4621,10 +4622,10 @@
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4635,7 +4636,7 @@
         <v>165</v>
       </c>
       <c r="D101" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4646,7 +4647,7 @@
         <v>167</v>
       </c>
       <c r="D102" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4654,10 +4655,10 @@
         <v>170</v>
       </c>
       <c r="C103" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="D103" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4668,7 +4669,7 @@
         <v>168</v>
       </c>
       <c r="D104" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4679,7 +4680,7 @@
         <v>169</v>
       </c>
       <c r="D105" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4687,13 +4688,13 @@
         <v>171</v>
       </c>
       <c r="B106" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C106" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D106" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,13 +4702,13 @@
         <v>155</v>
       </c>
       <c r="B107" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C107" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="D107" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4715,10 +4716,10 @@
         <v>164</v>
       </c>
       <c r="C108" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D108" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4726,10 +4727,10 @@
         <v>174</v>
       </c>
       <c r="C109" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D109" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4737,10 +4738,10 @@
         <v>163</v>
       </c>
       <c r="C110" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D110" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4751,7 +4752,7 @@
         <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4759,10 +4760,10 @@
         <v>92</v>
       </c>
       <c r="C112" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D112" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4770,10 +4771,10 @@
         <v>96</v>
       </c>
       <c r="C113" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D113" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4781,13 +4782,13 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C114" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D114" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4795,10 +4796,10 @@
         <v>60</v>
       </c>
       <c r="C115" t="s">
-        <v>425</v>
+        <v>579</v>
       </c>
       <c r="D115" t="s">
-        <v>426</v>
+        <v>578</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,13 +4807,13 @@
         <v>33</v>
       </c>
       <c r="B116" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C116" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="D116" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4820,13 +4821,13 @@
         <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C117" t="s">
         <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -4834,13 +4835,13 @@
         <v>25</v>
       </c>
       <c r="B118" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C118" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D118" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -4848,13 +4849,13 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4862,13 +4863,13 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C120" t="s">
+        <v>253</v>
+      </c>
+      <c r="D120" t="s">
         <v>254</v>
-      </c>
-      <c r="D120" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4876,13 +4877,13 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C121" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D121" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4890,13 +4891,13 @@
         <v>16</v>
       </c>
       <c r="B122" t="s">
+        <v>270</v>
+      </c>
+      <c r="C122" t="s">
         <v>271</v>
       </c>
-      <c r="C122" t="s">
-        <v>272</v>
-      </c>
       <c r="D122" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4904,13 +4905,13 @@
         <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C123" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D123" t="s">
-        <v>336</v>
+        <v>573</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4918,7 +4919,7 @@
         <v>20</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
@@ -4928,10 +4929,10 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D125" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4939,13 +4940,13 @@
         <v>38</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4953,13 +4954,13 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C127" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="D127" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -4967,13 +4968,13 @@
         <v>28</v>
       </c>
       <c r="B128" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>320</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -4981,13 +4982,13 @@
         <v>30</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4995,13 +4996,13 @@
         <v>27</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="D130" s="4" t="s">
         <v>329</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="D130" s="4" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5009,13 +5010,13 @@
         <v>15</v>
       </c>
       <c r="B131" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C131" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D131" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5023,13 +5024,13 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C132" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
       <c r="D132" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -5037,13 +5038,13 @@
         <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C133" t="s">
+        <v>256</v>
+      </c>
+      <c r="D133" t="s">
         <v>257</v>
-      </c>
-      <c r="D133" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -5051,13 +5052,13 @@
         <v>79</v>
       </c>
       <c r="B134" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C134" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="D134" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5065,13 +5066,13 @@
         <v>77</v>
       </c>
       <c r="B135" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C135" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D135" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -5079,13 +5080,13 @@
         <v>76</v>
       </c>
       <c r="B136" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C136" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D136" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5093,13 +5094,13 @@
         <v>78</v>
       </c>
       <c r="B137" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C137" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D137" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5108,7 +5109,7 @@
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="D138" s="4"/>
     </row>
@@ -5118,7 +5119,7 @@
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="D139" s="4"/>
     </row>
@@ -5127,27 +5128,27 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C140" t="s">
         <v>32</v>
       </c>
       <c r="D140" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="B141" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
       <c r="C141" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
       <c r="D141" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -5155,13 +5156,13 @@
         <v>123</v>
       </c>
       <c r="B142" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C142" t="s">
+        <v>292</v>
+      </c>
+      <c r="D142" t="s">
         <v>291</v>
-      </c>
-      <c r="C142" t="s">
-        <v>293</v>
-      </c>
-      <c r="D142" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -5169,13 +5170,13 @@
         <v>125</v>
       </c>
       <c r="B143" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C143" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="D143" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5183,13 +5184,13 @@
         <v>148</v>
       </c>
       <c r="B144" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C144" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="D144" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -5197,13 +5198,13 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="C145" t="s">
+        <v>249</v>
+      </c>
+      <c r="D145" t="s">
         <v>250</v>
-      </c>
-      <c r="D145" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -5211,13 +5212,13 @@
         <v>22</v>
       </c>
       <c r="B146" t="s">
+        <v>316</v>
+      </c>
+      <c r="C146" t="s">
+        <v>327</v>
+      </c>
+      <c r="D146" t="s">
         <v>317</v>
-      </c>
-      <c r="C146" t="s">
-        <v>328</v>
-      </c>
-      <c r="D146" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5226,10 +5227,10 @@
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4" t="s">
-        <v>488</v>
-      </c>
-      <c r="D147" s="4" t="s">
-        <v>431</v>
+        <v>480</v>
+      </c>
+      <c r="D147" s="7" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,13 +5238,13 @@
         <v>58</v>
       </c>
       <c r="B148" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C148" t="s">
-        <v>340</v>
+        <v>577</v>
       </c>
       <c r="D148" t="s">
-        <v>349</v>
+        <v>576</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5251,13 +5252,13 @@
         <v>56</v>
       </c>
       <c r="B149" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C149" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D149" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5265,13 +5266,13 @@
         <v>41</v>
       </c>
       <c r="B150" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C150" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D150" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5279,13 +5280,13 @@
         <v>44</v>
       </c>
       <c r="B151" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C151" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D151" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5293,13 +5294,13 @@
         <v>73</v>
       </c>
       <c r="B152" t="s">
+        <v>343</v>
+      </c>
+      <c r="C152" t="s">
+        <v>338</v>
+      </c>
+      <c r="D152" t="s">
         <v>346</v>
-      </c>
-      <c r="C152" t="s">
-        <v>341</v>
-      </c>
-      <c r="D152" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5307,13 +5308,13 @@
         <v>26</v>
       </c>
       <c r="B153" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C153" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D153" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5321,13 +5322,13 @@
         <v>87</v>
       </c>
       <c r="B154" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C154" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D154" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5335,13 +5336,13 @@
         <v>85</v>
       </c>
       <c r="B155" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C155" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D155" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5349,13 +5350,13 @@
         <v>88</v>
       </c>
       <c r="B156" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C156" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D156" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5363,13 +5364,13 @@
         <v>86</v>
       </c>
       <c r="B157" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C157" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D157" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1_0 translated until DEA calc
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="595">
   <si>
     <t>dat</t>
   </si>
@@ -607,9 +607,6 @@
     <t>Sum avkastningsgrunnlag DEA Dnett inkl 1% arbeidskapital</t>
   </si>
   <si>
-    <t>Total regulatory asset base, including 1% working capital</t>
-  </si>
-  <si>
     <t>Sum avskrivninger DEA Dnett</t>
   </si>
   <si>
@@ -643,9 +640,6 @@
     <t>Drift- og vedlikeholdskostnader uten lønns- og pensjonskostnader i distribusjonsnett</t>
   </si>
   <si>
-    <t>d_hv</t>
-  </si>
-  <si>
     <t>Km høyspent nett distribusjonsnett</t>
   </si>
   <si>
@@ -676,9 +670,6 @@
     <t>Nettap Dnett i kroner</t>
   </si>
   <si>
-    <t>d_nl.NOK</t>
-  </si>
-  <si>
     <t>Cost of network losses in NOK</t>
   </si>
   <si>
@@ -856,15 +847,9 @@
     <t>Consumer Price Index (Norwegian)</t>
   </si>
   <si>
-    <t>Actual inputs, total expenditures</t>
-  </si>
-  <si>
     <t>Average inputs, total expenditures over the past 5 years</t>
   </si>
   <si>
-    <t>Actual outputs, d_ab, d_hs, d_ns</t>
-  </si>
-  <si>
     <t>Average outputs, d_ab, d_hs, d_ns over the past 5 years</t>
   </si>
   <si>
@@ -880,18 +865,6 @@
     <t>Snitt output</t>
   </si>
   <si>
-    <t>x.act.d</t>
-  </si>
-  <si>
-    <t>y.act.d</t>
-  </si>
-  <si>
-    <t>x.avg.d</t>
-  </si>
-  <si>
-    <t>y.avg.d</t>
-  </si>
-  <si>
     <t>The weight given to the norm cost</t>
   </si>
   <si>
@@ -1045,9 +1018,6 @@
     <t>v_hist</t>
   </si>
   <si>
-    <t>v_sf</t>
-  </si>
-  <si>
     <t>Vektor av variabler som skal gjennomsnittsberegnes</t>
   </si>
   <si>
@@ -1069,9 +1039,6 @@
     <t>Vector containing variables that are to be averaged for historical years</t>
   </si>
   <si>
-    <t>Vector containing variables that are to be used in the construction of the average fronts</t>
-  </si>
-  <si>
     <t>Weighted value of a company's underground cables</t>
   </si>
   <si>
@@ -1240,9 +1207,6 @@
     <t>d_sep.eval</t>
   </si>
   <si>
-    <t>d_eval</t>
-  </si>
-  <si>
     <t>d_cb</t>
   </si>
   <si>
@@ -1273,9 +1237,6 @@
     <t>DEA efficiency after stage 1, only including 5 year historical average</t>
   </si>
   <si>
-    <t>d_EVAL</t>
-  </si>
-  <si>
     <t>drs_cost.RC.x.NL.A.r</t>
   </si>
   <si>
@@ -1348,9 +1309,6 @@
     <t>Vector of company id's to be evaluated in all stages of the DEA model</t>
   </si>
   <si>
-    <t>Data frame for companies that are to be evaluated in the DEA model</t>
-  </si>
-  <si>
     <t>Weights of peers from each company obtained from DEA, actual observation against 5 year historical average</t>
   </si>
   <si>
@@ -1774,7 +1732,88 @@
     <t>ld_rab.sf</t>
   </si>
   <si>
-    <t>Regulatory asset base self funded assets, including 1% working capital</t>
+    <t>Total regulatory asset base, including 1% working capital, used in DEA.</t>
+  </si>
+  <si>
+    <t>Regulatory asset base self funded assets, including 1% working capital, used for revenue cap calculation</t>
+  </si>
+  <si>
+    <t>ld_nl.NOK</t>
+  </si>
+  <si>
+    <t>v_fha</t>
+  </si>
+  <si>
+    <t>ld_hv</t>
+  </si>
+  <si>
+    <t>Vector containing variables that are inputs and outputs in the calculations of frontier based on historical average data</t>
+  </si>
+  <si>
+    <t>ld_EVAL</t>
+  </si>
+  <si>
+    <t>Data frame for companies that are to be evaluated in the normal DEA model, may be peers for all companies</t>
+  </si>
+  <si>
+    <t>ld_TOTXDEA</t>
+  </si>
+  <si>
+    <t>ld_eval</t>
+  </si>
+  <si>
+    <t>fha_ld_TOTXDEA</t>
+  </si>
+  <si>
+    <t>Five years historical average TOTEX, used as input in DEA</t>
+  </si>
+  <si>
+    <t>Five years historical average subscriber in local distribution, used as input in DEA</t>
+  </si>
+  <si>
+    <t>fha_ld_sub</t>
+  </si>
+  <si>
+    <t>Five years historical average km of high voltage lines, used as input in DEA</t>
+  </si>
+  <si>
+    <t>fha_ld_hv</t>
+  </si>
+  <si>
+    <t>fha_ld_ss</t>
+  </si>
+  <si>
+    <t>Five years historical average km of substations in distribution grid, used as input in DEA</t>
+  </si>
+  <si>
+    <t>Gjennomsnittlig antall abonnenter i D-nett siste fem år</t>
+  </si>
+  <si>
+    <t>Gjenomsnittlig antall km høyspent i D-nett siste fem år</t>
+  </si>
+  <si>
+    <t>Gjennomsnittlig TOTEX i D-nett siste fem år</t>
+  </si>
+  <si>
+    <t>Gjennnomsnittlig antall nettstasjoner i D-nett siste fem år</t>
+  </si>
+  <si>
+    <t>Cost base year observations of ld_sub, ld_hv, ld_ss</t>
+  </si>
+  <si>
+    <t>Observations from cost base year, total expenditures in local distribution</t>
+  </si>
+  <si>
+    <t>X.cb.ld</t>
+  </si>
+  <si>
+    <t>X.avg.ld</t>
+  </si>
+  <si>
+    <t>Y.act.ld</t>
+  </si>
+  <si>
+    <t>Y.avg.d</t>
   </si>
 </sst>
 </file>
@@ -2128,7 +2167,7 @@
   <dimension ref="A1:K144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
@@ -3322,10 +3361,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D157"/>
+  <dimension ref="A2:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3361,7 +3400,7 @@
         <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3369,13 +3408,13 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C4" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="D4" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3383,10 +3422,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="D5" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3397,7 +3436,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3411,10 +3450,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="D7" t="s">
-        <v>453</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3425,7 +3464,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3439,7 +3478,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3453,7 +3492,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3467,10 +3506,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="D11" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3481,24 +3520,24 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="B13" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="C13" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="D13" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3506,13 +3545,13 @@
         <v>68</v>
       </c>
       <c r="B14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" t="s">
+        <v>484</v>
+      </c>
+      <c r="D14" t="s">
         <v>193</v>
-      </c>
-      <c r="C14" t="s">
-        <v>498</v>
-      </c>
-      <c r="D14" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3520,13 +3559,13 @@
         <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C15" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3534,13 +3573,13 @@
         <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="D16" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3551,7 +3590,7 @@
         <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3559,13 +3598,13 @@
         <v>156</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="C18" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="D18" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3576,7 +3615,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3584,13 +3623,13 @@
         <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="C20" t="s">
         <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3601,7 +3640,7 @@
         <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3609,13 +3648,13 @@
         <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="C22" t="s">
         <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3626,7 +3665,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3634,10 +3673,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="D24" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3645,10 +3684,10 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="D25" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3656,13 +3695,13 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" t="s">
+        <v>428</v>
+      </c>
+      <c r="D26" t="s">
         <v>198</v>
-      </c>
-      <c r="C26" t="s">
-        <v>442</v>
-      </c>
-      <c r="D26" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3670,13 +3709,13 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" t="s">
+        <v>560</v>
+      </c>
+      <c r="D27" t="s">
         <v>200</v>
-      </c>
-      <c r="C27" t="s">
-        <v>574</v>
-      </c>
-      <c r="D27" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,13 +3723,13 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3698,13 +3737,13 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C29" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="D29" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3715,7 +3754,7 @@
         <v>112</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3723,21 +3762,21 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="D31" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="C32" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="D32" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3745,10 +3784,10 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="D33" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3756,10 +3795,10 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="D34" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3767,55 +3806,55 @@
         <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C35" t="s">
-        <v>204</v>
+        <v>571</v>
       </c>
       <c r="D35" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="B36" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="C36" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="D36" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="B37" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="C37" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="D37" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="B38" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="C38" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
       <c r="D38" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3823,10 +3862,10 @@
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="D39" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3834,13 +3873,13 @@
         <v>48</v>
       </c>
       <c r="B40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C40" t="s">
         <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3848,13 +3887,13 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="D41" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3862,10 +3901,10 @@
         <v>147</v>
       </c>
       <c r="C42" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
       <c r="D42" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3876,7 +3915,7 @@
         <v>93</v>
       </c>
       <c r="D43" t="s">
-        <v>440</v>
+        <v>426</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3884,10 +3923,10 @@
         <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D44" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3895,13 +3934,13 @@
         <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C45" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D45" t="s">
-        <v>448</v>
+        <v>434</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3909,27 +3948,27 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" t="s">
+        <v>210</v>
+      </c>
+      <c r="D46" t="s">
         <v>211</v>
-      </c>
-      <c r="C46" t="s">
-        <v>212</v>
-      </c>
-      <c r="D46" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="B47" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="C47" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="D47" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3937,13 +3976,13 @@
         <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C48" t="s">
-        <v>215</v>
+        <v>569</v>
       </c>
       <c r="D48" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3951,10 +3990,10 @@
         <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>403</v>
+        <v>576</v>
       </c>
       <c r="D49" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3962,13 +4001,13 @@
         <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C50" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="D50" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3976,10 +4015,10 @@
         <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="D51" t="s">
-        <v>443</v>
+        <v>429</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3988,10 +4027,10 @@
       </c>
       <c r="B52" s="6"/>
       <c r="C52" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D52" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3999,10 +4038,10 @@
         <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D53" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4010,13 +4049,13 @@
         <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C54" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D54" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4024,13 +4063,13 @@
         <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C55" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D55" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,13 +4077,13 @@
         <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C56" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D56" t="s">
-        <v>452</v>
+        <v>438</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4052,13 +4091,13 @@
         <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C57" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D57" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,13 +4105,13 @@
         <v>140</v>
       </c>
       <c r="B58" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C58" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D58" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4080,10 +4119,10 @@
         <v>113</v>
       </c>
       <c r="C59" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
       <c r="D59" t="s">
-        <v>450</v>
+        <v>436</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,10 +4130,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="D60" t="s">
-        <v>451</v>
+        <v>437</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4102,10 +4141,10 @@
         <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="D61" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4113,10 +4152,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="D62" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4124,13 +4163,13 @@
         <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="C63" t="s">
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>454</v>
+        <v>440</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4138,10 +4177,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>414</v>
+        <v>573</v>
       </c>
       <c r="D64" t="s">
-        <v>439</v>
+        <v>574</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4149,10 +4188,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>575</v>
       </c>
       <c r="D65" t="s">
-        <v>455</v>
+        <v>441</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4160,10 +4199,10 @@
         <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4171,10 +4210,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D67" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4182,10 +4221,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D68" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4193,24 +4232,24 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D69" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="B70" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="C70" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="D70" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4218,13 +4257,13 @@
         <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C71" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="D71" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,13 +4271,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C72" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="D72" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4246,13 +4285,13 @@
         <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C73" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D73" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4260,13 +4299,13 @@
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C74" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D74" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4274,13 +4313,13 @@
         <v>116</v>
       </c>
       <c r="B75" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C75" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D75" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4288,13 +4327,13 @@
         <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C76" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="D76" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4302,13 +4341,13 @@
         <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C77" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="D77" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4316,13 +4355,13 @@
         <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C78" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="D78" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4330,27 +4369,27 @@
         <v>111</v>
       </c>
       <c r="B79" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C79" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="D79" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>537</v>
+        <v>523</v>
       </c>
       <c r="B80" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
       <c r="C80" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="D80" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4358,13 +4397,13 @@
         <v>119</v>
       </c>
       <c r="B81" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C81" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="D81" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4372,27 +4411,27 @@
         <v>101</v>
       </c>
       <c r="B82" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C82" t="s">
-        <v>531</v>
+        <v>517</v>
       </c>
       <c r="D82" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="B83" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="C83" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="D83" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4400,13 +4439,13 @@
         <v>102</v>
       </c>
       <c r="B84" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="D84" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4414,13 +4453,13 @@
         <v>110</v>
       </c>
       <c r="B85" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C85" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="D85" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4428,13 +4467,13 @@
         <v>107</v>
       </c>
       <c r="B86" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C86" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="D86" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4442,27 +4481,27 @@
         <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C87" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="D87" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="B88" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="C88" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="D88" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4470,13 +4509,13 @@
         <v>104</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>536</v>
+        <v>522</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4484,13 +4523,13 @@
         <v>176</v>
       </c>
       <c r="B90" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="C90" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="D90" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4498,13 +4537,13 @@
         <v>162</v>
       </c>
       <c r="B91" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="C91" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="D91" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4512,24 +4551,24 @@
         <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="C92" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="D92" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="C93" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="D93" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4537,13 +4576,13 @@
         <v>153</v>
       </c>
       <c r="B94" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="C94" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="D94" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,13 +4590,13 @@
         <v>172</v>
       </c>
       <c r="B95" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="C95" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="D95" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4565,13 +4604,13 @@
         <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="C96" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="D96" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4579,13 +4618,13 @@
         <v>161</v>
       </c>
       <c r="B97" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="C97" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D97" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4593,13 +4632,13 @@
         <v>173</v>
       </c>
       <c r="B98" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="C98" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="D98" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4607,13 +4646,13 @@
         <v>160</v>
       </c>
       <c r="B99" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="C99" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="D99" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4622,10 +4661,10 @@
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4636,7 +4675,7 @@
         <v>165</v>
       </c>
       <c r="D101" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4647,7 +4686,7 @@
         <v>167</v>
       </c>
       <c r="D102" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4655,10 +4694,10 @@
         <v>170</v>
       </c>
       <c r="C103" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="D103" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4669,7 +4708,7 @@
         <v>168</v>
       </c>
       <c r="D104" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4680,7 +4719,7 @@
         <v>169</v>
       </c>
       <c r="D105" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4688,13 +4727,13 @@
         <v>171</v>
       </c>
       <c r="B106" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="C106" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="D106" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4702,13 +4741,13 @@
         <v>155</v>
       </c>
       <c r="B107" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="C107" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="D107" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4716,10 +4755,10 @@
         <v>164</v>
       </c>
       <c r="C108" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="D108" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,10 +4766,10 @@
         <v>174</v>
       </c>
       <c r="C109" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="D109" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4738,10 +4777,10 @@
         <v>163</v>
       </c>
       <c r="C110" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="D110" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4752,7 +4791,7 @@
         <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4760,10 +4799,10 @@
         <v>92</v>
       </c>
       <c r="C112" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="D112" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4771,10 +4810,10 @@
         <v>96</v>
       </c>
       <c r="C113" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="D113" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4782,13 +4821,13 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="C114" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="D114" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4796,10 +4835,10 @@
         <v>60</v>
       </c>
       <c r="C115" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="D115" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4807,13 +4846,13 @@
         <v>33</v>
       </c>
       <c r="B116" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="C116" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="D116" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,13 +4860,13 @@
         <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="C117" t="s">
         <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,13 +4874,13 @@
         <v>25</v>
       </c>
       <c r="B118" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C118" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="D118" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -4849,13 +4888,13 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4863,13 +4902,13 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C120" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D120" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4877,13 +4916,13 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="C121" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D121" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4891,13 +4930,13 @@
         <v>16</v>
       </c>
       <c r="B122" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C122" t="s">
+        <v>268</v>
+      </c>
+      <c r="D122" t="s">
         <v>271</v>
-      </c>
-      <c r="D122" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4905,13 +4944,13 @@
         <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C123" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D123" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4919,7 +4958,7 @@
         <v>20</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
@@ -4929,10 +4968,10 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="D125" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4940,13 +4979,13 @@
         <v>38</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4954,13 +4993,13 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C127" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="D127" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -4968,13 +5007,13 @@
         <v>28</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -4982,13 +5021,13 @@
         <v>30</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4996,13 +5035,13 @@
         <v>27</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5010,13 +5049,13 @@
         <v>15</v>
       </c>
       <c r="B131" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C131" t="s">
+        <v>313</v>
+      </c>
+      <c r="D131" t="s">
         <v>322</v>
-      </c>
-      <c r="D131" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5024,13 +5063,13 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C132" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="D132" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -5038,13 +5077,13 @@
         <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C133" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D133" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -5052,13 +5091,13 @@
         <v>79</v>
       </c>
       <c r="B134" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C134" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="D134" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5066,13 +5105,13 @@
         <v>77</v>
       </c>
       <c r="B135" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C135" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="D135" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -5080,13 +5119,13 @@
         <v>76</v>
       </c>
       <c r="B136" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C136" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="D136" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5094,13 +5133,13 @@
         <v>78</v>
       </c>
       <c r="B137" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C137" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="D137" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5109,7 +5148,7 @@
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="D138" s="4"/>
     </row>
@@ -5119,7 +5158,7 @@
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="D139" s="4"/>
     </row>
@@ -5128,27 +5167,27 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C140" t="s">
         <v>32</v>
       </c>
       <c r="D140" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="B141" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="C141" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="D141" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -5156,13 +5195,13 @@
         <v>123</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C142" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D142" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -5170,13 +5209,13 @@
         <v>125</v>
       </c>
       <c r="B143" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C143" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="D143" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5184,13 +5223,13 @@
         <v>148</v>
       </c>
       <c r="B144" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C144" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="D144" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -5198,13 +5237,13 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="C145" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D145" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -5212,13 +5251,13 @@
         <v>22</v>
       </c>
       <c r="B146" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C146" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D146" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5227,10 +5266,10 @@
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5238,13 +5277,13 @@
         <v>58</v>
       </c>
       <c r="B148" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="C148" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
       <c r="D148" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5252,13 +5291,13 @@
         <v>56</v>
       </c>
       <c r="B149" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C149" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="D149" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5266,13 +5305,13 @@
         <v>41</v>
       </c>
       <c r="B150" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="C150" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D150" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5280,13 +5319,13 @@
         <v>44</v>
       </c>
       <c r="B151" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="C151" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="D151" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5294,13 +5333,13 @@
         <v>73</v>
       </c>
       <c r="B152" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="C152" t="s">
-        <v>338</v>
+        <v>570</v>
       </c>
       <c r="D152" t="s">
-        <v>346</v>
+        <v>572</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5308,13 +5347,13 @@
         <v>26</v>
       </c>
       <c r="B153" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="C153" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="D153" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5322,13 +5361,13 @@
         <v>87</v>
       </c>
       <c r="B154" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C154" t="s">
-        <v>283</v>
+        <v>591</v>
       </c>
       <c r="D154" t="s">
-        <v>275</v>
+        <v>590</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5336,13 +5375,13 @@
         <v>85</v>
       </c>
       <c r="B155" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C155" t="s">
-        <v>285</v>
+        <v>592</v>
       </c>
       <c r="D155" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5350,13 +5389,13 @@
         <v>88</v>
       </c>
       <c r="B156" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C156" t="s">
-        <v>284</v>
+        <v>593</v>
       </c>
       <c r="D156" t="s">
-        <v>277</v>
+        <v>589</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5364,13 +5403,57 @@
         <v>86</v>
       </c>
       <c r="B157" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="C157" t="s">
-        <v>286</v>
+        <v>594</v>
       </c>
       <c r="D157" t="s">
-        <v>278</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>587</v>
+      </c>
+      <c r="C158" t="s">
+        <v>577</v>
+      </c>
+      <c r="D158" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>585</v>
+      </c>
+      <c r="C159" t="s">
+        <v>580</v>
+      </c>
+      <c r="D159" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>586</v>
+      </c>
+      <c r="C160" t="s">
+        <v>582</v>
+      </c>
+      <c r="D160" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>588</v>
+      </c>
+      <c r="C161" t="s">
+        <v>583</v>
+      </c>
+      <c r="D161" t="s">
+        <v>584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1_0_DEA translated for all local dist calcs
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -892,9 +892,6 @@
     <t>d_out.NOK</t>
   </si>
   <si>
-    <t>dea.act.avg.d</t>
-  </si>
-  <si>
     <t>dea.avg.avg.d</t>
   </si>
   <si>
@@ -1219,9 +1216,6 @@
     <t>DEA efficiency after stage 2</t>
   </si>
   <si>
-    <t>d_eff.s1</t>
-  </si>
-  <si>
     <t>DEA efficiency after stage 1, regular DEA (last observation against 5 yeras historical average)</t>
   </si>
   <si>
@@ -1810,10 +1804,16 @@
     <t>X.avg.ld</t>
   </si>
   <si>
-    <t>Y.act.ld</t>
-  </si>
-  <si>
     <t>Y.avg.d</t>
+  </si>
+  <si>
+    <t>Y.cb.ld</t>
+  </si>
+  <si>
+    <t>ld_eff.s1.cb</t>
+  </si>
+  <si>
+    <t>dea.cb.avg.ld</t>
   </si>
 </sst>
 </file>
@@ -3363,8 +3363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3408,13 +3408,13 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3422,10 +3422,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3436,7 +3436,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3450,10 +3450,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3464,7 +3464,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3478,7 +3478,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3492,7 +3492,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3506,10 +3506,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
+        <v>564</v>
+      </c>
+      <c r="D11" t="s">
         <v>566</v>
-      </c>
-      <c r="D11" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3520,24 +3520,24 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D12" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>529</v>
+      </c>
+      <c r="B13" t="s">
         <v>531</v>
       </c>
-      <c r="B13" t="s">
-        <v>533</v>
-      </c>
       <c r="C13" t="s">
+        <v>530</v>
+      </c>
+      <c r="D13" t="s">
         <v>532</v>
-      </c>
-      <c r="D13" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3548,7 +3548,7 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D14" t="s">
         <v>193</v>
@@ -3562,7 +3562,7 @@
         <v>195</v>
       </c>
       <c r="C15" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D15" t="s">
         <v>194</v>
@@ -3576,10 +3576,10 @@
         <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D16" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3590,7 +3590,7 @@
         <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3598,13 +3598,13 @@
         <v>156</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C18" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D18" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3615,7 +3615,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3623,13 +3623,13 @@
         <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C20" t="s">
         <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3640,7 +3640,7 @@
         <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3648,13 +3648,13 @@
         <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C22" t="s">
         <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,7 +3665,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3673,10 +3673,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D24" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,10 +3684,10 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
+        <v>393</v>
+      </c>
+      <c r="D25" t="s">
         <v>394</v>
-      </c>
-      <c r="D25" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3698,7 +3698,7 @@
         <v>197</v>
       </c>
       <c r="C26" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D26" t="s">
         <v>198</v>
@@ -3712,7 +3712,7 @@
         <v>199</v>
       </c>
       <c r="C27" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D27" t="s">
         <v>200</v>
@@ -3723,10 +3723,10 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>201</v>
@@ -3740,10 +3740,10 @@
         <v>202</v>
       </c>
       <c r="C29" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D29" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3754,7 +3754,7 @@
         <v>112</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3762,21 +3762,21 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>396</v>
+        <v>593</v>
       </c>
       <c r="D31" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>507</v>
+      </c>
+      <c r="C32" t="s">
+        <v>508</v>
+      </c>
+      <c r="D32" t="s">
         <v>509</v>
-      </c>
-      <c r="C32" t="s">
-        <v>510</v>
-      </c>
-      <c r="D32" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3784,10 +3784,10 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D33" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3795,10 +3795,10 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D34" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3809,52 +3809,52 @@
         <v>203</v>
       </c>
       <c r="C35" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D35" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>497</v>
+      </c>
+      <c r="B36" t="s">
         <v>499</v>
       </c>
-      <c r="B36" t="s">
-        <v>501</v>
-      </c>
       <c r="C36" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D36" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B37" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C37" t="s">
+        <v>492</v>
+      </c>
+      <c r="D37" t="s">
         <v>494</v>
-      </c>
-      <c r="D37" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>501</v>
+      </c>
+      <c r="B38" t="s">
+        <v>502</v>
+      </c>
+      <c r="C38" t="s">
         <v>503</v>
       </c>
-      <c r="B38" t="s">
-        <v>504</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>505</v>
-      </c>
-      <c r="D38" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3862,10 +3862,10 @@
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D39" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3890,10 +3890,10 @@
         <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D41" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3901,10 +3901,10 @@
         <v>147</v>
       </c>
       <c r="C42" t="s">
+        <v>391</v>
+      </c>
+      <c r="D42" t="s">
         <v>392</v>
-      </c>
-      <c r="D42" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3915,7 +3915,7 @@
         <v>93</v>
       </c>
       <c r="D43" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3926,7 +3926,7 @@
         <v>284</v>
       </c>
       <c r="D44" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
         <v>208</v>
       </c>
       <c r="D45" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3959,16 +3959,16 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>472</v>
+      </c>
+      <c r="B47" t="s">
+        <v>473</v>
+      </c>
+      <c r="C47" t="s">
         <v>474</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" t="s">
         <v>475</v>
-      </c>
-      <c r="C47" t="s">
-        <v>476</v>
-      </c>
-      <c r="D47" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3979,7 +3979,7 @@
         <v>212</v>
       </c>
       <c r="C48" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D48" t="s">
         <v>213</v>
@@ -3990,10 +3990,10 @@
         <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D49" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4004,10 +4004,10 @@
         <v>214</v>
       </c>
       <c r="C50" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D50" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4015,10 +4015,10 @@
         <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D51" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4030,7 +4030,7 @@
         <v>285</v>
       </c>
       <c r="D52" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4041,7 +4041,7 @@
         <v>286</v>
       </c>
       <c r="D53" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4055,7 +4055,7 @@
         <v>216</v>
       </c>
       <c r="D54" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>218</v>
       </c>
       <c r="D55" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,13 +4077,13 @@
         <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C56" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D56" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,13 +4091,13 @@
         <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C57" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4105,13 +4105,13 @@
         <v>140</v>
       </c>
       <c r="B58" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C58" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D58" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4119,10 +4119,10 @@
         <v>113</v>
       </c>
       <c r="C59" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D59" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4130,10 +4130,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D60" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4141,10 +4141,10 @@
         <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D61" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4152,10 +4152,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D62" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4163,13 +4163,13 @@
         <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C63" t="s">
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4177,10 +4177,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D64" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4188,10 +4188,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D65" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4199,10 +4199,10 @@
         <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4210,10 +4210,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>287</v>
+        <v>594</v>
       </c>
       <c r="D67" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4221,10 +4221,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D68" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,24 +4232,24 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D69" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>540</v>
+      </c>
+      <c r="B70" t="s">
         <v>542</v>
       </c>
-      <c r="B70" t="s">
-        <v>544</v>
-      </c>
       <c r="C70" t="s">
+        <v>545</v>
+      </c>
+      <c r="D70" t="s">
         <v>547</v>
-      </c>
-      <c r="D70" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4257,13 +4257,13 @@
         <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C71" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D71" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4271,13 +4271,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C72" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D72" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4330,7 +4330,7 @@
         <v>229</v>
       </c>
       <c r="C76" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D76" t="s">
         <v>228</v>
@@ -4344,7 +4344,7 @@
         <v>231</v>
       </c>
       <c r="C77" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D77" t="s">
         <v>230</v>
@@ -4358,10 +4358,10 @@
         <v>232</v>
       </c>
       <c r="C78" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D78" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4372,7 +4372,7 @@
         <v>260</v>
       </c>
       <c r="C79" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D79" t="s">
         <v>261</v>
@@ -4380,16 +4380,16 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>521</v>
+      </c>
+      <c r="B80" t="s">
+        <v>522</v>
+      </c>
+      <c r="C80" t="s">
         <v>523</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>524</v>
-      </c>
-      <c r="C80" t="s">
-        <v>525</v>
-      </c>
-      <c r="D80" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4400,7 +4400,7 @@
         <v>257</v>
       </c>
       <c r="C81" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D81" t="s">
         <v>262</v>
@@ -4414,7 +4414,7 @@
         <v>258</v>
       </c>
       <c r="C82" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D82" t="s">
         <v>263</v>
@@ -4422,16 +4422,16 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>533</v>
+      </c>
+      <c r="B83" t="s">
+        <v>534</v>
+      </c>
+      <c r="C83" t="s">
         <v>535</v>
       </c>
-      <c r="B83" t="s">
-        <v>536</v>
-      </c>
-      <c r="C83" t="s">
-        <v>537</v>
-      </c>
       <c r="D83" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4442,10 +4442,10 @@
         <v>233</v>
       </c>
       <c r="C84" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D84" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4456,7 +4456,7 @@
         <v>259</v>
       </c>
       <c r="C85" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D85" t="s">
         <v>264</v>
@@ -4470,7 +4470,7 @@
         <v>234</v>
       </c>
       <c r="C86" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D86" t="s">
         <v>265</v>
@@ -4484,7 +4484,7 @@
         <v>236</v>
       </c>
       <c r="C87" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D87" t="s">
         <v>235</v>
@@ -4492,16 +4492,16 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>516</v>
+      </c>
+      <c r="B88" t="s">
+        <v>517</v>
+      </c>
+      <c r="C88" t="s">
         <v>518</v>
       </c>
-      <c r="B88" t="s">
+      <c r="D88" t="s">
         <v>519</v>
-      </c>
-      <c r="C88" t="s">
-        <v>520</v>
-      </c>
-      <c r="D88" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4515,7 +4515,7 @@
         <v>237</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4523,13 +4523,13 @@
         <v>176</v>
       </c>
       <c r="B90" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C90" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D90" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4537,13 +4537,13 @@
         <v>162</v>
       </c>
       <c r="B91" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C91" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D91" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,24 +4551,24 @@
         <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C92" t="s">
+        <v>367</v>
+      </c>
+      <c r="D92" t="s">
         <v>368</v>
-      </c>
-      <c r="D92" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C93" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D93" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4576,13 +4576,13 @@
         <v>153</v>
       </c>
       <c r="B94" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C94" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D94" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4590,13 +4590,13 @@
         <v>172</v>
       </c>
       <c r="B95" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C95" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D95" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4604,13 +4604,13 @@
         <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C96" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D96" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4618,13 +4618,13 @@
         <v>161</v>
       </c>
       <c r="B97" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C97" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D97" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4632,13 +4632,13 @@
         <v>173</v>
       </c>
       <c r="B98" t="s">
+        <v>374</v>
+      </c>
+      <c r="C98" t="s">
+        <v>349</v>
+      </c>
+      <c r="D98" t="s">
         <v>375</v>
-      </c>
-      <c r="C98" t="s">
-        <v>350</v>
-      </c>
-      <c r="D98" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4646,13 +4646,13 @@
         <v>160</v>
       </c>
       <c r="B99" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C99" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D99" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4661,10 +4661,10 @@
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4675,7 +4675,7 @@
         <v>165</v>
       </c>
       <c r="D101" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>167</v>
       </c>
       <c r="D102" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4694,10 +4694,10 @@
         <v>170</v>
       </c>
       <c r="C103" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D103" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4708,7 +4708,7 @@
         <v>168</v>
       </c>
       <c r="D104" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4719,7 +4719,7 @@
         <v>169</v>
       </c>
       <c r="D105" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,13 +4727,13 @@
         <v>171</v>
       </c>
       <c r="B106" t="s">
+        <v>360</v>
+      </c>
+      <c r="C106" t="s">
         <v>361</v>
       </c>
-      <c r="C106" t="s">
-        <v>362</v>
-      </c>
       <c r="D106" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4741,13 +4741,13 @@
         <v>155</v>
       </c>
       <c r="B107" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C107" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D107" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4755,10 +4755,10 @@
         <v>164</v>
       </c>
       <c r="C108" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D108" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4766,10 +4766,10 @@
         <v>174</v>
       </c>
       <c r="C109" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D109" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4777,10 +4777,10 @@
         <v>163</v>
       </c>
       <c r="C110" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D110" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4791,7 @@
         <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4799,10 +4799,10 @@
         <v>92</v>
       </c>
       <c r="C112" t="s">
+        <v>402</v>
+      </c>
+      <c r="D112" t="s">
         <v>404</v>
-      </c>
-      <c r="D112" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4810,10 +4810,10 @@
         <v>96</v>
       </c>
       <c r="C113" t="s">
+        <v>403</v>
+      </c>
+      <c r="D113" t="s">
         <v>405</v>
-      </c>
-      <c r="D113" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,13 +4821,13 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C114" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D114" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,10 +4835,10 @@
         <v>60</v>
       </c>
       <c r="C115" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D115" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4846,13 +4846,13 @@
         <v>33</v>
       </c>
       <c r="B116" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C116" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D116" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4860,13 +4860,13 @@
         <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C117" t="s">
         <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -4877,10 +4877,10 @@
         <v>266</v>
       </c>
       <c r="C118" t="s">
+        <v>338</v>
+      </c>
+      <c r="D118" t="s">
         <v>339</v>
-      </c>
-      <c r="D118" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -4916,13 +4916,13 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C121" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D121" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4950,7 +4950,7 @@
         <v>269</v>
       </c>
       <c r="D123" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4958,7 +4958,7 @@
         <v>20</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
@@ -4968,10 +4968,10 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D125" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,13 +4979,13 @@
         <v>38</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4993,13 +4993,13 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C127" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D127" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5007,13 +5007,13 @@
         <v>28</v>
       </c>
       <c r="B128" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5021,13 +5021,13 @@
         <v>30</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -5035,13 +5035,13 @@
         <v>27</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="D130" s="4" t="s">
         <v>319</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="D130" s="4" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5049,13 +5049,13 @@
         <v>15</v>
       </c>
       <c r="B131" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C131" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D131" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5063,13 +5063,13 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C132" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D132" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -5094,10 +5094,10 @@
         <v>239</v>
       </c>
       <c r="C134" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D134" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5108,10 +5108,10 @@
         <v>240</v>
       </c>
       <c r="C135" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D135" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -5122,10 +5122,10 @@
         <v>241</v>
       </c>
       <c r="C136" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D136" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5136,10 +5136,10 @@
         <v>242</v>
       </c>
       <c r="C137" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D137" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D138" s="4"/>
     </row>
@@ -5158,7 +5158,7 @@
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D139" s="4"/>
     </row>
@@ -5178,16 +5178,16 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B141" t="s">
+        <v>539</v>
+      </c>
+      <c r="C141" t="s">
         <v>541</v>
       </c>
-      <c r="C141" t="s">
-        <v>543</v>
-      </c>
       <c r="D141" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -5212,7 +5212,7 @@
         <v>244</v>
       </c>
       <c r="C143" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D143" t="s">
         <v>243</v>
@@ -5226,7 +5226,7 @@
         <v>245</v>
       </c>
       <c r="C144" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D144" t="s">
         <v>280</v>
@@ -5237,7 +5237,7 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C145" t="s">
         <v>246</v>
@@ -5251,13 +5251,13 @@
         <v>22</v>
       </c>
       <c r="B146" t="s">
+        <v>306</v>
+      </c>
+      <c r="C146" t="s">
+        <v>317</v>
+      </c>
+      <c r="D146" t="s">
         <v>307</v>
-      </c>
-      <c r="C146" t="s">
-        <v>318</v>
-      </c>
-      <c r="D146" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5266,10 +5266,10 @@
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5277,13 +5277,13 @@
         <v>58</v>
       </c>
       <c r="B148" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C148" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D148" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5291,13 +5291,13 @@
         <v>56</v>
       </c>
       <c r="B149" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C149" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D149" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5305,13 +5305,13 @@
         <v>41</v>
       </c>
       <c r="B150" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C150" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D150" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5319,13 +5319,13 @@
         <v>44</v>
       </c>
       <c r="B151" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C151" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D151" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5333,13 +5333,13 @@
         <v>73</v>
       </c>
       <c r="B152" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C152" t="s">
+        <v>568</v>
+      </c>
+      <c r="D152" t="s">
         <v>570</v>
-      </c>
-      <c r="D152" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5347,13 +5347,13 @@
         <v>26</v>
       </c>
       <c r="B153" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C153" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D153" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5364,10 +5364,10 @@
         <v>274</v>
       </c>
       <c r="C154" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="D154" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5378,7 +5378,7 @@
         <v>275</v>
       </c>
       <c r="C155" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D155" t="s">
         <v>272</v>
@@ -5392,10 +5392,10 @@
         <v>276</v>
       </c>
       <c r="C156" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D156" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5406,7 +5406,7 @@
         <v>277</v>
       </c>
       <c r="C157" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D157" t="s">
         <v>273</v>
@@ -5414,46 +5414,46 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C158" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D158" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C159" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D159" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C160" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D160" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C161" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D161" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1_0 DEA translated, id 167 in rd_av.eff
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="597">
   <si>
     <t>dat</t>
   </si>
@@ -655,15 +655,9 @@
     <t>Lønnskostnader ekskl pensjon Dnett</t>
   </si>
   <si>
-    <t>d_sal</t>
-  </si>
-  <si>
     <t>Lønnskostnader, aktiverte Dnett</t>
   </si>
   <si>
-    <t>d_sal.cap</t>
-  </si>
-  <si>
     <t>Capitalization of labor costs</t>
   </si>
   <si>
@@ -883,9 +877,6 @@
     <t>rg_Geo1</t>
   </si>
   <si>
-    <t>d_lambda.avg</t>
-  </si>
-  <si>
     <t>d_out</t>
   </si>
   <si>
@@ -1204,9 +1195,6 @@
     <t>d_sep.eval</t>
   </si>
   <si>
-    <t>d_cb</t>
-  </si>
-  <si>
     <t>Company's cost base, used in stage 3 calibration</t>
   </si>
   <si>
@@ -1814,6 +1802,24 @@
   </si>
   <si>
     <t>dea.cb.avg.ld</t>
+  </si>
+  <si>
+    <t>ld_impl</t>
+  </si>
+  <si>
+    <t>ld_cb</t>
+  </si>
+  <si>
+    <t>ld_lambda</t>
+  </si>
+  <si>
+    <t>ld_lambda.avg</t>
+  </si>
+  <si>
+    <t>ld_sal</t>
+  </si>
+  <si>
+    <t>ld_sal.cap</t>
   </si>
 </sst>
 </file>
@@ -3363,8 +3369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,7 +3406,7 @@
         <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3408,13 +3414,13 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3422,10 +3428,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D5" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3436,7 +3442,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3450,10 +3456,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D7" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3464,7 +3470,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3478,7 +3484,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3492,7 +3498,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3506,10 +3512,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D11" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3520,24 +3526,24 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D12" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B13" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C13" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D13" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3548,7 +3554,7 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D14" t="s">
         <v>193</v>
@@ -3562,7 +3568,7 @@
         <v>195</v>
       </c>
       <c r="C15" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="D15" t="s">
         <v>194</v>
@@ -3576,10 +3582,10 @@
         <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D16" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3590,7 +3596,7 @@
         <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3598,13 +3604,13 @@
         <v>156</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C18" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D18" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3615,7 +3621,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3623,13 +3629,13 @@
         <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C20" t="s">
         <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3640,7 +3646,7 @@
         <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3648,13 +3654,13 @@
         <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C22" t="s">
         <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,7 +3671,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3673,10 +3679,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="D24" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,10 +3690,10 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D25" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3698,7 +3704,7 @@
         <v>197</v>
       </c>
       <c r="C26" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="D26" t="s">
         <v>198</v>
@@ -3712,7 +3718,7 @@
         <v>199</v>
       </c>
       <c r="C27" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D27" t="s">
         <v>200</v>
@@ -3723,10 +3729,10 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>201</v>
@@ -3740,10 +3746,10 @@
         <v>202</v>
       </c>
       <c r="C29" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D29" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3754,7 +3760,7 @@
         <v>112</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3762,21 +3768,21 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D31" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C32" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D32" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3784,10 +3790,10 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="D33" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3795,10 +3801,10 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D34" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3809,52 +3815,52 @@
         <v>203</v>
       </c>
       <c r="C35" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D35" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B36" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C36" t="s">
+        <v>496</v>
+      </c>
+      <c r="D36" t="s">
         <v>500</v>
-      </c>
-      <c r="D36" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B37" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C37" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D37" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>497</v>
+      </c>
+      <c r="B38" t="s">
+        <v>498</v>
+      </c>
+      <c r="C38" t="s">
+        <v>499</v>
+      </c>
+      <c r="D38" t="s">
         <v>501</v>
-      </c>
-      <c r="B38" t="s">
-        <v>502</v>
-      </c>
-      <c r="C38" t="s">
-        <v>503</v>
-      </c>
-      <c r="D38" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3862,10 +3868,10 @@
         <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D39" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3876,7 +3882,7 @@
         <v>205</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>591</v>
       </c>
       <c r="D40" t="s">
         <v>206</v>
@@ -3890,10 +3896,10 @@
         <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D41" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3901,10 +3907,10 @@
         <v>147</v>
       </c>
       <c r="C42" t="s">
-        <v>391</v>
+        <v>592</v>
       </c>
       <c r="D42" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3912,10 +3918,10 @@
         <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>593</v>
       </c>
       <c r="D43" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3923,10 +3929,10 @@
         <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>284</v>
+        <v>594</v>
       </c>
       <c r="D44" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3937,10 +3943,10 @@
         <v>207</v>
       </c>
       <c r="C45" t="s">
-        <v>208</v>
+        <v>595</v>
       </c>
       <c r="D45" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3948,27 +3954,27 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" t="s">
+        <v>596</v>
+      </c>
+      <c r="D46" t="s">
         <v>209</v>
-      </c>
-      <c r="C46" t="s">
-        <v>210</v>
-      </c>
-      <c r="D46" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B47" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C47" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D47" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3976,13 +3982,13 @@
         <v>71</v>
       </c>
       <c r="B48" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C48" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3990,10 +3996,10 @@
         <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D49" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4001,13 +4007,13 @@
         <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C50" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D50" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4015,10 +4021,10 @@
         <v>136</v>
       </c>
       <c r="C51" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D51" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4027,10 +4033,10 @@
       </c>
       <c r="B52" s="6"/>
       <c r="C52" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D52" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,10 +4044,10 @@
         <v>143</v>
       </c>
       <c r="C53" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D53" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4049,13 +4055,13 @@
         <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C54" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D54" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4063,13 +4069,13 @@
         <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C55" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D55" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,13 +4083,13 @@
         <v>138</v>
       </c>
       <c r="B56" t="s">
+        <v>292</v>
+      </c>
+      <c r="C56" t="s">
         <v>295</v>
       </c>
-      <c r="C56" t="s">
-        <v>298</v>
-      </c>
       <c r="D56" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,13 +4097,13 @@
         <v>139</v>
       </c>
       <c r="B57" t="s">
+        <v>293</v>
+      </c>
+      <c r="C57" t="s">
         <v>296</v>
       </c>
-      <c r="C57" t="s">
-        <v>299</v>
-      </c>
       <c r="D57" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4105,13 +4111,13 @@
         <v>140</v>
       </c>
       <c r="B58" t="s">
+        <v>294</v>
+      </c>
+      <c r="C58" t="s">
         <v>297</v>
       </c>
-      <c r="C58" t="s">
-        <v>300</v>
-      </c>
       <c r="D58" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4119,10 +4125,10 @@
         <v>113</v>
       </c>
       <c r="C59" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D59" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4130,10 +4136,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D60" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4141,10 +4147,10 @@
         <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D61" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4152,10 +4158,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D62" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4163,13 +4169,13 @@
         <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C63" t="s">
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4177,10 +4183,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D64" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4188,10 +4194,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D65" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4199,10 +4205,10 @@
         <v>50</v>
       </c>
       <c r="C66" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4210,10 +4216,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D67" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4221,10 +4227,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D68" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4232,24 +4238,24 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D69" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B70" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C70" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D70" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4257,13 +4263,13 @@
         <v>105</v>
       </c>
       <c r="B71" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C71" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D71" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4271,13 +4277,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C72" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="D72" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4285,13 +4291,13 @@
         <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D73" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4299,13 +4305,13 @@
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C74" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4313,13 +4319,13 @@
         <v>116</v>
       </c>
       <c r="B75" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D75" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4327,13 +4333,13 @@
         <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C76" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="D76" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4341,13 +4347,13 @@
         <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C77" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D77" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4355,13 +4361,13 @@
         <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C78" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D78" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4369,27 +4375,27 @@
         <v>111</v>
       </c>
       <c r="B79" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C79" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D79" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B80" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="C80" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D80" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4397,13 +4403,13 @@
         <v>119</v>
       </c>
       <c r="B81" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C81" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D81" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4411,27 +4417,27 @@
         <v>101</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C82" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D82" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B83" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C83" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D83" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4439,13 +4445,13 @@
         <v>102</v>
       </c>
       <c r="B84" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C84" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D84" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4453,13 +4459,13 @@
         <v>110</v>
       </c>
       <c r="B85" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C85" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D85" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4467,13 +4473,13 @@
         <v>107</v>
       </c>
       <c r="B86" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C86" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D86" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4481,27 +4487,27 @@
         <v>108</v>
       </c>
       <c r="B87" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C87" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D87" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B88" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="C88" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D88" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4509,13 +4515,13 @@
         <v>104</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4523,13 +4529,13 @@
         <v>176</v>
       </c>
       <c r="B90" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C90" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D90" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4537,13 +4543,13 @@
         <v>162</v>
       </c>
       <c r="B91" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C91" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D91" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,24 +4557,24 @@
         <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C92" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D92" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C93" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D93" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4576,13 +4582,13 @@
         <v>153</v>
       </c>
       <c r="B94" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="C94" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D94" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4590,13 +4596,13 @@
         <v>172</v>
       </c>
       <c r="B95" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C95" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D95" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4604,13 +4610,13 @@
         <v>175</v>
       </c>
       <c r="B96" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C96" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D96" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4618,13 +4624,13 @@
         <v>161</v>
       </c>
       <c r="B97" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C97" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D97" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4632,13 +4638,13 @@
         <v>173</v>
       </c>
       <c r="B98" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C98" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D98" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4646,13 +4652,13 @@
         <v>160</v>
       </c>
       <c r="B99" t="s">
+        <v>370</v>
+      </c>
+      <c r="C99" t="s">
+        <v>347</v>
+      </c>
+      <c r="D99" t="s">
         <v>373</v>
-      </c>
-      <c r="C99" t="s">
-        <v>350</v>
-      </c>
-      <c r="D99" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4661,10 +4667,10 @@
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4675,7 +4681,7 @@
         <v>165</v>
       </c>
       <c r="D101" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4686,7 +4692,7 @@
         <v>167</v>
       </c>
       <c r="D102" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4694,10 +4700,10 @@
         <v>170</v>
       </c>
       <c r="C103" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D103" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4708,7 +4714,7 @@
         <v>168</v>
       </c>
       <c r="D104" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4719,7 +4725,7 @@
         <v>169</v>
       </c>
       <c r="D105" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,13 +4733,13 @@
         <v>171</v>
       </c>
       <c r="B106" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C106" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D106" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4741,13 +4747,13 @@
         <v>155</v>
       </c>
       <c r="B107" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C107" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D107" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4755,10 +4761,10 @@
         <v>164</v>
       </c>
       <c r="C108" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D108" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4766,10 +4772,10 @@
         <v>174</v>
       </c>
       <c r="C109" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D109" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4777,10 +4783,10 @@
         <v>163</v>
       </c>
       <c r="C110" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D110" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,7 +4797,7 @@
         <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4799,10 +4805,10 @@
         <v>92</v>
       </c>
       <c r="C112" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D112" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4810,10 +4816,10 @@
         <v>96</v>
       </c>
       <c r="C113" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D113" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,13 +4827,13 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C114" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D114" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,10 +4841,10 @@
         <v>60</v>
       </c>
       <c r="C115" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D115" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4846,13 +4852,13 @@
         <v>33</v>
       </c>
       <c r="B116" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C116" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D116" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4860,13 +4866,13 @@
         <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C117" t="s">
         <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -4874,13 +4880,13 @@
         <v>25</v>
       </c>
       <c r="B118" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C118" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D118" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -4888,13 +4894,13 @@
         <v>1</v>
       </c>
       <c r="B119" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
       </c>
       <c r="D119" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4902,13 +4908,13 @@
         <v>10</v>
       </c>
       <c r="B120" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C120" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D120" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4916,13 +4922,13 @@
         <v>24</v>
       </c>
       <c r="B121" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C121" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D121" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4930,13 +4936,13 @@
         <v>16</v>
       </c>
       <c r="B122" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C122" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D122" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4944,13 +4950,13 @@
         <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C123" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D123" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4958,7 +4964,7 @@
         <v>20</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
@@ -4968,10 +4974,10 @@
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D125" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,13 +4985,13 @@
         <v>38</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4993,13 +4999,13 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C127" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D127" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5007,13 +5013,13 @@
         <v>28</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5021,13 +5027,13 @@
         <v>30</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -5035,13 +5041,13 @@
         <v>27</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5049,13 +5055,13 @@
         <v>15</v>
       </c>
       <c r="B131" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C131" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D131" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5063,13 +5069,13 @@
         <v>19</v>
       </c>
       <c r="B132" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C132" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D132" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -5077,13 +5083,13 @@
         <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C133" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D133" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,13 +5097,13 @@
         <v>79</v>
       </c>
       <c r="B134" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C134" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D134" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5105,13 +5111,13 @@
         <v>77</v>
       </c>
       <c r="B135" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C135" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D135" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -5119,13 +5125,13 @@
         <v>76</v>
       </c>
       <c r="B136" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C136" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D136" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5133,13 +5139,13 @@
         <v>78</v>
       </c>
       <c r="B137" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C137" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D137" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5148,7 +5154,7 @@
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D138" s="4"/>
     </row>
@@ -5158,7 +5164,7 @@
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D139" s="4"/>
     </row>
@@ -5167,27 +5173,27 @@
         <v>32</v>
       </c>
       <c r="B140" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C140" t="s">
         <v>32</v>
       </c>
       <c r="D140" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B141" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C141" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D141" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -5195,13 +5201,13 @@
         <v>123</v>
       </c>
       <c r="B142" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C142" t="s">
         <v>281</v>
       </c>
-      <c r="C142" t="s">
-        <v>283</v>
-      </c>
       <c r="D142" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -5209,13 +5215,13 @@
         <v>125</v>
       </c>
       <c r="B143" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C143" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D143" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5223,13 +5229,13 @@
         <v>148</v>
       </c>
       <c r="B144" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C144" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D144" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,13 +5243,13 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C145" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D145" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -5251,13 +5257,13 @@
         <v>22</v>
       </c>
       <c r="B146" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C146" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D146" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5266,10 +5272,10 @@
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5277,13 +5283,13 @@
         <v>58</v>
       </c>
       <c r="B148" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C148" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D148" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5291,13 +5297,13 @@
         <v>56</v>
       </c>
       <c r="B149" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C149" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D149" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5305,13 +5311,13 @@
         <v>41</v>
       </c>
       <c r="B150" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C150" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D150" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5319,13 +5325,13 @@
         <v>44</v>
       </c>
       <c r="B151" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C151" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D151" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5333,13 +5339,13 @@
         <v>73</v>
       </c>
       <c r="B152" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C152" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D152" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5347,13 +5353,13 @@
         <v>26</v>
       </c>
       <c r="B153" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C153" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D153" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5361,13 +5367,13 @@
         <v>87</v>
       </c>
       <c r="B154" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C154" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D154" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5375,13 +5381,13 @@
         <v>85</v>
       </c>
       <c r="B155" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C155" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D155" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5389,13 +5395,13 @@
         <v>88</v>
       </c>
       <c r="B156" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C156" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="D156" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5403,57 +5409,57 @@
         <v>86</v>
       </c>
       <c r="B157" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C157" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D157" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="C158" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D158" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="C159" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D159" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C160" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D160" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="C161" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D161" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2_X_translated, 2_0 translated ld, fixed bug/typo in 02_calculated. QA ok
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -682,27 +682,18 @@
     <t>d_pens.eq</t>
   </si>
   <si>
-    <t>dg_Geo1</t>
-  </si>
-  <si>
     <t>Fjellbekk, GEO-variable estimated through PCA.</t>
   </si>
   <si>
     <t>Fjellbekk, Geovariabel estimert vha faktoranalyse</t>
   </si>
   <si>
-    <t>dg_Geo2</t>
-  </si>
-  <si>
     <t>Oyvind, GEO-variable estimated through PCA.</t>
   </si>
   <si>
     <t>Øyvind, Geovariabel estimert vha faktoranalyse</t>
   </si>
   <si>
-    <t>dg_Geo3</t>
-  </si>
-  <si>
     <t>Frost, GEO-variable estimated through PCA.</t>
   </si>
   <si>
@@ -1946,6 +1937,15 @@
   </si>
   <si>
     <t>ldz_wind squared</t>
+  </si>
+  <si>
+    <t>ldz_Geo1</t>
+  </si>
+  <si>
+    <t>ldz_Geo2</t>
+  </si>
+  <si>
+    <t>ldz_Geo3</t>
   </si>
 </sst>
 </file>
@@ -3495,8 +3495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,7 +3532,7 @@
         <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3540,13 +3540,13 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D4" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,10 +3554,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D5" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3568,7 +3568,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3582,10 +3582,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D7" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3596,7 +3596,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3610,7 +3610,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3624,7 +3624,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3638,10 +3638,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D11" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3652,24 +3652,24 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D12" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B13" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C13" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D13" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3680,7 +3680,7 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D14" t="s">
         <v>193</v>
@@ -3694,7 +3694,7 @@
         <v>195</v>
       </c>
       <c r="C15" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D15" t="s">
         <v>194</v>
@@ -3708,10 +3708,10 @@
         <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D16" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,7 +3722,7 @@
         <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3730,13 +3730,13 @@
         <v>156</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C18" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D18" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3747,7 +3747,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3755,13 +3755,13 @@
         <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C20" t="s">
         <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
         <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3780,13 +3780,13 @@
         <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C22" t="s">
         <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,7 +3797,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,10 +3805,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D24" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3816,10 +3816,10 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D25" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3830,7 +3830,7 @@
         <v>197</v>
       </c>
       <c r="C26" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D26" t="s">
         <v>198</v>
@@ -3844,7 +3844,7 @@
         <v>199</v>
       </c>
       <c r="C27" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D27" t="s">
         <v>200</v>
@@ -3855,10 +3855,10 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>201</v>
@@ -3872,10 +3872,10 @@
         <v>202</v>
       </c>
       <c r="C29" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D29" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3886,7 +3886,7 @@
         <v>112</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,10 +3894,10 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D31" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3905,21 +3905,21 @@
         <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D32" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="C33" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D33" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3927,10 +3927,10 @@
         <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D34" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3938,10 +3938,10 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D35" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3952,52 +3952,52 @@
         <v>203</v>
       </c>
       <c r="C36" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D36" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>484</v>
+      </c>
+      <c r="B37" t="s">
+        <v>486</v>
+      </c>
+      <c r="C37" t="s">
         <v>487</v>
       </c>
-      <c r="B37" t="s">
-        <v>489</v>
-      </c>
-      <c r="C37" t="s">
-        <v>490</v>
-      </c>
       <c r="D37" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>478</v>
+      </c>
+      <c r="B38" t="s">
+        <v>485</v>
+      </c>
+      <c r="C38" t="s">
+        <v>479</v>
+      </c>
+      <c r="D38" t="s">
         <v>481</v>
-      </c>
-      <c r="B38" t="s">
-        <v>488</v>
-      </c>
-      <c r="C38" t="s">
-        <v>482</v>
-      </c>
-      <c r="D38" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B39" t="s">
+        <v>489</v>
+      </c>
+      <c r="C39" t="s">
+        <v>490</v>
+      </c>
+      <c r="D39" t="s">
         <v>492</v>
-      </c>
-      <c r="C39" t="s">
-        <v>493</v>
-      </c>
-      <c r="D39" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4005,10 +4005,10 @@
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D40" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4019,7 +4019,7 @@
         <v>205</v>
       </c>
       <c r="C41" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D41" t="s">
         <v>206</v>
@@ -4033,10 +4033,10 @@
         <v>204</v>
       </c>
       <c r="C42" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D42" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4044,10 +4044,10 @@
         <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D43" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4055,10 +4055,10 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D44" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,10 +4066,10 @@
         <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D45" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4080,10 +4080,10 @@
         <v>207</v>
       </c>
       <c r="C46" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D46" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4094,7 +4094,7 @@
         <v>208</v>
       </c>
       <c r="C47" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D47" t="s">
         <v>209</v>
@@ -4102,16 +4102,16 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>459</v>
+      </c>
+      <c r="B48" t="s">
+        <v>460</v>
+      </c>
+      <c r="C48" t="s">
+        <v>461</v>
+      </c>
+      <c r="D48" t="s">
         <v>462</v>
-      </c>
-      <c r="B48" t="s">
-        <v>463</v>
-      </c>
-      <c r="C48" t="s">
-        <v>464</v>
-      </c>
-      <c r="D48" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4122,7 +4122,7 @@
         <v>210</v>
       </c>
       <c r="C49" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D49" t="s">
         <v>211</v>
@@ -4133,10 +4133,10 @@
         <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D50" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4147,10 +4147,10 @@
         <v>212</v>
       </c>
       <c r="C51" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D51" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4158,10 +4158,10 @@
         <v>136</v>
       </c>
       <c r="C52" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D52" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4170,10 +4170,10 @@
       </c>
       <c r="B53" s="6"/>
       <c r="C53" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D53" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,10 +4181,10 @@
         <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D54" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4198,7 +4198,7 @@
         <v>214</v>
       </c>
       <c r="D55" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4212,7 +4212,7 @@
         <v>216</v>
       </c>
       <c r="D56" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4220,13 +4220,13 @@
         <v>138</v>
       </c>
       <c r="B57" t="s">
+        <v>288</v>
+      </c>
+      <c r="C57" t="s">
         <v>291</v>
       </c>
-      <c r="C57" t="s">
-        <v>294</v>
-      </c>
       <c r="D57" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4234,13 +4234,13 @@
         <v>139</v>
       </c>
       <c r="B58" t="s">
+        <v>289</v>
+      </c>
+      <c r="C58" t="s">
         <v>292</v>
       </c>
-      <c r="C58" t="s">
-        <v>295</v>
-      </c>
       <c r="D58" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4248,13 +4248,13 @@
         <v>140</v>
       </c>
       <c r="B59" t="s">
+        <v>290</v>
+      </c>
+      <c r="C59" t="s">
         <v>293</v>
       </c>
-      <c r="C59" t="s">
-        <v>296</v>
-      </c>
       <c r="D59" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4262,10 +4262,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D60" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4273,10 +4273,10 @@
         <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D61" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4284,10 +4284,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D62" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4295,13 +4295,13 @@
         <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C63" t="s">
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,10 +4309,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D64" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4320,10 +4320,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D65" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4331,10 +4331,10 @@
         <v>50</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4342,10 +4342,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D67" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4353,10 +4353,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D68" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4364,38 +4364,38 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D69" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B70" t="s">
+        <v>525</v>
+      </c>
+      <c r="C70" t="s">
         <v>528</v>
       </c>
-      <c r="C70" t="s">
-        <v>531</v>
-      </c>
       <c r="D70" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B71" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C71" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D71" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4403,13 +4403,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C72" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D72" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4417,13 +4417,13 @@
         <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C73" t="s">
+        <v>636</v>
+      </c>
+      <c r="D73" t="s">
         <v>217</v>
-      </c>
-      <c r="D73" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,13 +4431,13 @@
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C74" t="s">
-        <v>220</v>
+        <v>637</v>
       </c>
       <c r="D74" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4445,13 +4445,13 @@
         <v>116</v>
       </c>
       <c r="B75" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C75" t="s">
-        <v>223</v>
+        <v>638</v>
       </c>
       <c r="D75" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4459,13 +4459,13 @@
         <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C76" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D76" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4473,13 +4473,13 @@
         <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C77" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D77" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4487,27 +4487,27 @@
         <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D78" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>624</v>
+      </c>
+      <c r="B79" t="s">
+        <v>625</v>
+      </c>
+      <c r="C79" t="s">
+        <v>626</v>
+      </c>
+      <c r="D79" t="s">
         <v>627</v>
-      </c>
-      <c r="B79" t="s">
-        <v>628</v>
-      </c>
-      <c r="C79" t="s">
-        <v>629</v>
-      </c>
-      <c r="D79" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4515,27 +4515,27 @@
         <v>111</v>
       </c>
       <c r="B80" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C80" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D80" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>507</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="C81" t="s">
+        <v>509</v>
+      </c>
+      <c r="D81" t="s">
         <v>510</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>511</v>
-      </c>
-      <c r="C81" t="s">
-        <v>512</v>
-      </c>
-      <c r="D81" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4543,13 +4543,13 @@
         <v>119</v>
       </c>
       <c r="B82" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C82" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D82" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4557,41 +4557,41 @@
         <v>101</v>
       </c>
       <c r="B83" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C83" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D83" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B84" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C84" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D84" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="B85" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C85" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D85" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4599,13 +4599,13 @@
         <v>102</v>
       </c>
       <c r="B86" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C86" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D86" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4613,13 +4613,13 @@
         <v>110</v>
       </c>
       <c r="B87" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C87" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D87" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4627,13 +4627,13 @@
         <v>107</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C88" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D88" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,27 +4641,27 @@
         <v>108</v>
       </c>
       <c r="B89" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C89" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D89" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>503</v>
+      </c>
+      <c r="B90" t="s">
+        <v>504</v>
+      </c>
+      <c r="C90" t="s">
+        <v>505</v>
+      </c>
+      <c r="D90" t="s">
         <v>506</v>
-      </c>
-      <c r="B90" t="s">
-        <v>507</v>
-      </c>
-      <c r="C90" t="s">
-        <v>508</v>
-      </c>
-      <c r="D90" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4669,13 +4669,13 @@
         <v>104</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4683,13 +4683,13 @@
         <v>176</v>
       </c>
       <c r="B92" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C92" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D92" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4697,13 +4697,13 @@
         <v>162</v>
       </c>
       <c r="B93" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C93" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D93" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4711,24 +4711,24 @@
         <v>154</v>
       </c>
       <c r="B94" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C94" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D94" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C95" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D95" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4736,13 +4736,13 @@
         <v>153</v>
       </c>
       <c r="B96" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C96" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D96" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4750,13 +4750,13 @@
         <v>172</v>
       </c>
       <c r="B97" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C97" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D97" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4764,13 +4764,13 @@
         <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C98" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D98" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4778,13 +4778,13 @@
         <v>161</v>
       </c>
       <c r="B99" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C99" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D99" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4792,13 +4792,13 @@
         <v>173</v>
       </c>
       <c r="B100" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C100" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D100" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,13 +4806,13 @@
         <v>160</v>
       </c>
       <c r="B101" t="s">
+        <v>364</v>
+      </c>
+      <c r="C101" t="s">
+        <v>341</v>
+      </c>
+      <c r="D101" t="s">
         <v>367</v>
-      </c>
-      <c r="C101" t="s">
-        <v>344</v>
-      </c>
-      <c r="D101" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,10 +4821,10 @@
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,7 +4835,7 @@
         <v>165</v>
       </c>
       <c r="D103" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4846,7 +4846,7 @@
         <v>167</v>
       </c>
       <c r="D104" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4854,10 +4854,10 @@
         <v>170</v>
       </c>
       <c r="C105" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D105" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4868,7 +4868,7 @@
         <v>168</v>
       </c>
       <c r="D106" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4879,7 +4879,7 @@
         <v>169</v>
       </c>
       <c r="D107" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4887,13 +4887,13 @@
         <v>171</v>
       </c>
       <c r="B108" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C108" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D108" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4901,13 +4901,13 @@
         <v>155</v>
       </c>
       <c r="B109" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C109" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D109" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4915,10 +4915,10 @@
         <v>164</v>
       </c>
       <c r="C110" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D110" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,10 +4926,10 @@
         <v>174</v>
       </c>
       <c r="C111" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D111" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4937,10 +4937,10 @@
         <v>163</v>
       </c>
       <c r="C112" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D112" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4951,7 +4951,7 @@
         <v>166</v>
       </c>
       <c r="D113" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4959,10 +4959,10 @@
         <v>92</v>
       </c>
       <c r="C114" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D114" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4970,10 +4970,10 @@
         <v>96</v>
       </c>
       <c r="C115" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D115" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4981,13 +4981,13 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C116" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D116" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4995,10 +4995,10 @@
         <v>60</v>
       </c>
       <c r="C117" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D117" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5006,13 +5006,13 @@
         <v>33</v>
       </c>
       <c r="B118" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C118" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D118" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5020,13 +5020,13 @@
         <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C119" t="s">
         <v>18</v>
       </c>
       <c r="D119" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5034,13 +5034,13 @@
         <v>25</v>
       </c>
       <c r="B120" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C120" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D120" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5048,13 +5048,13 @@
         <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -5062,13 +5062,13 @@
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C122" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D122" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,13 +5076,13 @@
         <v>24</v>
       </c>
       <c r="B123" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C123" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D123" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -5090,13 +5090,13 @@
         <v>16</v>
       </c>
       <c r="B124" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C124" t="s">
+        <v>262</v>
+      </c>
+      <c r="D124" t="s">
         <v>265</v>
-      </c>
-      <c r="D124" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -5104,13 +5104,13 @@
         <v>17</v>
       </c>
       <c r="B125" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C125" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D125" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5118,7 +5118,7 @@
         <v>20</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -5128,10 +5128,10 @@
         <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D127" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5139,13 +5139,13 @@
         <v>38</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5153,13 +5153,13 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C129" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D129" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -5167,13 +5167,13 @@
         <v>28</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,13 +5181,13 @@
         <v>30</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5195,13 +5195,13 @@
         <v>27</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -5209,13 +5209,13 @@
         <v>15</v>
       </c>
       <c r="B133" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C133" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D133" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -5223,13 +5223,13 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C134" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D134" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,13 +5237,13 @@
         <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C135" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D135" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -5251,13 +5251,13 @@
         <v>79</v>
       </c>
       <c r="B136" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C136" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D136" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5265,13 +5265,13 @@
         <v>77</v>
       </c>
       <c r="B137" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C137" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D137" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5279,13 +5279,13 @@
         <v>76</v>
       </c>
       <c r="B138" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C138" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D138" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -5293,13 +5293,13 @@
         <v>78</v>
       </c>
       <c r="B139" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C139" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D139" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -5308,7 +5308,7 @@
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D140" s="4"/>
     </row>
@@ -5318,7 +5318,7 @@
       </c>
       <c r="B141" s="4"/>
       <c r="C141" s="4" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D141" s="4"/>
     </row>
@@ -5327,27 +5327,27 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C142" t="s">
         <v>32</v>
       </c>
       <c r="D142" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>521</v>
+      </c>
+      <c r="B143" t="s">
+        <v>522</v>
+      </c>
+      <c r="C143" t="s">
         <v>524</v>
       </c>
-      <c r="B143" t="s">
-        <v>525</v>
-      </c>
-      <c r="C143" t="s">
-        <v>527</v>
-      </c>
       <c r="D143" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5355,13 +5355,13 @@
         <v>123</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C144" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D144" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -5369,13 +5369,13 @@
         <v>125</v>
       </c>
       <c r="B145" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C145" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D145" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -5383,13 +5383,13 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C146" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D146" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5397,13 +5397,13 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C147" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D147" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5411,13 +5411,13 @@
         <v>22</v>
       </c>
       <c r="B148" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C148" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D148" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5426,10 +5426,10 @@
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5437,13 +5437,13 @@
         <v>58</v>
       </c>
       <c r="B150" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C150" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="D150" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5451,13 +5451,13 @@
         <v>56</v>
       </c>
       <c r="B151" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C151" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D151" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5465,13 +5465,13 @@
         <v>41</v>
       </c>
       <c r="B152" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C152" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D152" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5479,13 +5479,13 @@
         <v>44</v>
       </c>
       <c r="B153" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C153" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D153" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5493,13 +5493,13 @@
         <v>73</v>
       </c>
       <c r="B154" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C154" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D154" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5507,13 +5507,13 @@
         <v>26</v>
       </c>
       <c r="B155" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C155" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D155" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5521,13 +5521,13 @@
         <v>87</v>
       </c>
       <c r="B156" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C156" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D156" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5535,13 +5535,13 @@
         <v>85</v>
       </c>
       <c r="B157" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C157" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D157" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -5549,13 +5549,13 @@
         <v>88</v>
       </c>
       <c r="B158" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C158" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D158" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -5563,83 +5563,83 @@
         <v>86</v>
       </c>
       <c r="B159" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C159" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D159" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C160" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D160" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C161" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D161" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C162" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D162" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C163" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="D163" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5647,97 +5647,97 @@
         <v>113</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="D167" s="4" t="s">
         <v>603</v>
-      </c>
-      <c r="B167" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="C167" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="D168" s="4" t="s">
         <v>608</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="D168" s="4" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="D169" s="4" t="s">
         <v>612</v>
-      </c>
-      <c r="B169" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="C169" s="4" t="s">
-        <v>614</v>
-      </c>
-      <c r="D169" s="4" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="C170" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="D170" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>618</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>619</v>
-      </c>
-      <c r="D170" s="4" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="C171" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="D171" s="4" t="s">
         <v>621</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>622</v>
-      </c>
-      <c r="C171" s="7" t="s">
-        <v>623</v>
-      </c>
-      <c r="D171" s="4" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="C172" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="B172" s="4" t="s">
-        <v>634</v>
-      </c>
-      <c r="C172" s="7" t="s">
-        <v>636</v>
-      </c>
       <c r="D172" s="4" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2_0 finished ld grid, almost finished rd
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -20,6 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Ark2'!$A$2:$D$159</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="641">
   <si>
     <t>dat</t>
   </si>
@@ -610,9 +611,6 @@
     <t>Sum avskrivninger DEA Dnett</t>
   </si>
   <si>
-    <t xml:space="preserve">Total depreciations </t>
-  </si>
-  <si>
     <t>Depreciation associated with self-funded assets</t>
   </si>
   <si>
@@ -1246,9 +1244,6 @@
     <t>Cost norms from stage 3</t>
   </si>
   <si>
-    <t>Geo coefficients used in stage 2</t>
-  </si>
-  <si>
     <t>Cost recovery model, data frame containing data from the cost base year, t-2</t>
   </si>
   <si>
@@ -1264,9 +1259,6 @@
     <t>d_opex2012</t>
   </si>
   <si>
-    <t>Vector of DEA efficiencies after boot strap, equals d_score_bs100</t>
-  </si>
-  <si>
     <t>Vector of company id's to be evaluated in all stages of the DEA model</t>
   </si>
   <si>
@@ -1420,9 +1412,6 @@
     <t>Network losses in MWh</t>
   </si>
   <si>
-    <t>ld_coeff</t>
-  </si>
-  <si>
     <t>ld_391</t>
   </si>
   <si>
@@ -1432,9 +1421,6 @@
     <t>ld_rab.gf</t>
   </si>
   <si>
-    <t>ld_gfa</t>
-  </si>
-  <si>
     <t>ld_RAB</t>
   </si>
   <si>
@@ -1582,9 +1568,6 @@
     <t>Antall øyer: Forsyning av øyer uten fastlandsforbindelse og mer enn 1 km fra fastland eller nærmeste forsynte øy</t>
   </si>
   <si>
-    <t>Number of islands connected without mainland connection, more than 1 km of coast and without power production</t>
-  </si>
-  <si>
     <t>installed capacity micro power plants</t>
   </si>
   <si>
@@ -1946,6 +1929,30 @@
   </si>
   <si>
     <t>ldz_Geo3</t>
+  </si>
+  <si>
+    <t>ld_eff.bs</t>
+  </si>
+  <si>
+    <t>Vector of DEA efficiencies after boot strap, equals d_score_bs100 (Stata) &amp; ld_eff.bs.is2.cZ. Used for creating Z-variables. TEMP?</t>
+  </si>
+  <si>
+    <t>Geovar.ldz</t>
+  </si>
+  <si>
+    <t>Estimated Geo coefficients used in stage 2</t>
+  </si>
+  <si>
+    <t>ldz.coeff</t>
+  </si>
+  <si>
+    <t>ld_bv.gf</t>
+  </si>
+  <si>
+    <t>Number of islands connected without mainland connection, more than 1 km off mainland or island with grid connection</t>
+  </si>
+  <si>
+    <t>Total depreciations used in TOTEX/TOTCO calculations</t>
   </si>
 </sst>
 </file>
@@ -3493,10 +3500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D172"/>
+  <dimension ref="A2:D173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3532,7 +3539,7 @@
         <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3540,13 +3547,13 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C4" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3554,10 +3561,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>463</v>
+        <v>637</v>
       </c>
       <c r="D5" t="s">
-        <v>405</v>
+        <v>636</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3568,7 +3575,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3582,10 +3589,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D7" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3596,7 +3603,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3610,7 +3617,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3624,7 +3631,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>467</v>
+        <v>638</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3638,10 +3645,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D11" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3652,24 +3659,24 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D12" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="B13" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="C13" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="D13" t="s">
-        <v>517</v>
+        <v>639</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3680,10 +3687,10 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="D14" t="s">
-        <v>193</v>
+        <v>640</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3691,13 +3698,13 @@
         <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3705,13 +3712,13 @@
         <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C16" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D16" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3722,7 +3729,7 @@
         <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3730,13 +3737,13 @@
         <v>156</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C18" t="s">
+        <v>402</v>
+      </c>
+      <c r="D18" t="s">
         <v>403</v>
-      </c>
-      <c r="D18" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3747,7 +3754,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3755,13 +3762,13 @@
         <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C20" t="s">
         <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3772,7 +3779,7 @@
         <v>158</v>
       </c>
       <c r="D21" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3780,13 +3787,13 @@
         <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C22" t="s">
         <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3797,7 +3804,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,10 +3812,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="D24" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3816,10 +3823,10 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
+        <v>382</v>
+      </c>
+      <c r="D25" t="s">
         <v>383</v>
-      </c>
-      <c r="D25" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,13 +3834,13 @@
         <v>61</v>
       </c>
       <c r="B26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" t="s">
+        <v>412</v>
+      </c>
+      <c r="D26" t="s">
         <v>197</v>
-      </c>
-      <c r="C26" t="s">
-        <v>415</v>
-      </c>
-      <c r="D26" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3841,13 +3848,13 @@
         <v>62</v>
       </c>
       <c r="B27" t="s">
+        <v>198</v>
+      </c>
+      <c r="C27" t="s">
+        <v>535</v>
+      </c>
+      <c r="D27" t="s">
         <v>199</v>
-      </c>
-      <c r="C27" t="s">
-        <v>541</v>
-      </c>
-      <c r="D27" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3855,13 +3862,13 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3869,13 +3876,13 @@
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C29" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="D29" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3883,10 +3890,10 @@
         <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>633</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>411</v>
+        <v>634</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,10 +3901,10 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="D31" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3905,21 +3912,21 @@
         <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="D32" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C33" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D33" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3927,10 +3934,10 @@
         <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="D34" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3938,10 +3945,10 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="D35" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3949,55 +3956,55 @@
         <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C36" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="D36" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B37" t="s">
+        <v>481</v>
+      </c>
+      <c r="C37" t="s">
+        <v>482</v>
+      </c>
+      <c r="D37" t="s">
         <v>486</v>
-      </c>
-      <c r="C37" t="s">
-        <v>487</v>
-      </c>
-      <c r="D37" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="B38" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="C38" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D38" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B39" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C39" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D39" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4005,10 +4012,10 @@
         <v>14</v>
       </c>
       <c r="C40" t="s">
+        <v>384</v>
+      </c>
+      <c r="D40" t="s">
         <v>385</v>
-      </c>
-      <c r="D40" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4016,13 +4023,13 @@
         <v>48</v>
       </c>
       <c r="B41" t="s">
+        <v>204</v>
+      </c>
+      <c r="C41" t="s">
+        <v>572</v>
+      </c>
+      <c r="D41" t="s">
         <v>205</v>
-      </c>
-      <c r="C41" t="s">
-        <v>578</v>
-      </c>
-      <c r="D41" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4030,13 +4037,13 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C42" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D42" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4044,10 +4051,10 @@
         <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="D43" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4055,10 +4062,10 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="D44" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,10 +4073,10 @@
         <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="D45" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,13 +4084,13 @@
         <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C46" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="D46" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,27 +4098,27 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
+        <v>207</v>
+      </c>
+      <c r="C47" t="s">
+        <v>577</v>
+      </c>
+      <c r="D47" t="s">
         <v>208</v>
-      </c>
-      <c r="C47" t="s">
-        <v>583</v>
-      </c>
-      <c r="D47" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>456</v>
+      </c>
+      <c r="B48" t="s">
+        <v>457</v>
+      </c>
+      <c r="C48" t="s">
+        <v>458</v>
+      </c>
+      <c r="D48" t="s">
         <v>459</v>
-      </c>
-      <c r="B48" t="s">
-        <v>460</v>
-      </c>
-      <c r="C48" t="s">
-        <v>461</v>
-      </c>
-      <c r="D48" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4119,13 +4126,13 @@
         <v>71</v>
       </c>
       <c r="B49" t="s">
+        <v>209</v>
+      </c>
+      <c r="C49" t="s">
+        <v>544</v>
+      </c>
+      <c r="D49" t="s">
         <v>210</v>
-      </c>
-      <c r="C49" t="s">
-        <v>550</v>
-      </c>
-      <c r="D49" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4133,10 +4140,10 @@
         <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="D50" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4144,13 +4151,13 @@
         <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C51" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="D51" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4158,10 +4165,10 @@
         <v>136</v>
       </c>
       <c r="C52" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="D52" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4170,10 +4177,10 @@
       </c>
       <c r="B53" s="6"/>
       <c r="C53" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D53" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,10 +4188,10 @@
         <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D54" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4192,13 +4199,13 @@
         <v>46</v>
       </c>
       <c r="B55" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" t="s">
         <v>213</v>
       </c>
-      <c r="C55" t="s">
-        <v>214</v>
-      </c>
       <c r="D55" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4206,13 +4213,13 @@
         <v>47</v>
       </c>
       <c r="B56" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" t="s">
         <v>215</v>
       </c>
-      <c r="C56" t="s">
-        <v>216</v>
-      </c>
       <c r="D56" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4220,13 +4227,13 @@
         <v>138</v>
       </c>
       <c r="B57" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C57" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D57" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4234,13 +4241,13 @@
         <v>139</v>
       </c>
       <c r="B58" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C58" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D58" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4248,13 +4255,13 @@
         <v>140</v>
       </c>
       <c r="B59" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C59" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D59" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4262,10 +4269,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D60" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4273,10 +4280,10 @@
         <v>95</v>
       </c>
       <c r="C61" t="s">
+        <v>386</v>
+      </c>
+      <c r="D61" t="s">
         <v>387</v>
-      </c>
-      <c r="D61" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4284,10 +4291,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="D62" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4295,13 +4302,13 @@
         <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C63" t="s">
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4309,10 +4316,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="D64" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4320,10 +4327,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="D65" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4331,10 +4338,10 @@
         <v>50</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4342,10 +4349,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D67" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4353,10 +4360,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D68" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4364,38 +4371,38 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D69" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="B70" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="C70" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="D70" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="B71" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C71" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="D71" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4403,13 +4410,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C72" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D72" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4417,13 +4424,13 @@
         <v>114</v>
       </c>
       <c r="B73" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C73" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="D73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4431,13 +4438,13 @@
         <v>115</v>
       </c>
       <c r="B74" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C74" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="D74" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4445,13 +4452,13 @@
         <v>116</v>
       </c>
       <c r="B75" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C75" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="D75" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4459,13 +4466,13 @@
         <v>100</v>
       </c>
       <c r="B76" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C76" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="D76" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4473,13 +4480,13 @@
         <v>117</v>
       </c>
       <c r="B77" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C77" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="D77" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4487,27 +4494,27 @@
         <v>118</v>
       </c>
       <c r="B78" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="D78" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B79" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="C79" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="D79" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4515,27 +4522,27 @@
         <v>111</v>
       </c>
       <c r="B80" t="s">
+        <v>253</v>
+      </c>
+      <c r="C80" t="s">
+        <v>508</v>
+      </c>
+      <c r="D80" t="s">
         <v>254</v>
-      </c>
-      <c r="C80" t="s">
-        <v>513</v>
-      </c>
-      <c r="D80" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="C81" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="D81" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4543,13 +4550,13 @@
         <v>119</v>
       </c>
       <c r="B82" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C82" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="D82" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4557,41 +4564,41 @@
         <v>101</v>
       </c>
       <c r="B83" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C83" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="D83" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="B84" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="C84" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="D84" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="B85" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="C85" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="D85" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4599,13 +4606,13 @@
         <v>102</v>
       </c>
       <c r="B86" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C86" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="D86" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4613,13 +4620,13 @@
         <v>110</v>
       </c>
       <c r="B87" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C87" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="D87" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4627,13 +4634,13 @@
         <v>107</v>
       </c>
       <c r="B88" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C88" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="D88" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,27 +4648,27 @@
         <v>108</v>
       </c>
       <c r="B89" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C89" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D89" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B90" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C90" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D90" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4669,13 +4676,13 @@
         <v>104</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4683,13 +4690,13 @@
         <v>176</v>
       </c>
       <c r="B92" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C92" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D92" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4697,13 +4704,13 @@
         <v>162</v>
       </c>
       <c r="B93" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C93" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D93" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4711,24 +4718,24 @@
         <v>154</v>
       </c>
       <c r="B94" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C94" t="s">
+        <v>357</v>
+      </c>
+      <c r="D94" t="s">
         <v>358</v>
-      </c>
-      <c r="D94" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C95" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D95" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4736,13 +4743,13 @@
         <v>153</v>
       </c>
       <c r="B96" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C96" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D96" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4750,13 +4757,13 @@
         <v>172</v>
       </c>
       <c r="B97" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C97" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D97" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4764,13 +4771,13 @@
         <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C98" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D98" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4778,13 +4785,13 @@
         <v>161</v>
       </c>
       <c r="B99" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C99" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D99" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4792,13 +4799,13 @@
         <v>173</v>
       </c>
       <c r="B100" t="s">
+        <v>364</v>
+      </c>
+      <c r="C100" t="s">
+        <v>339</v>
+      </c>
+      <c r="D100" t="s">
         <v>365</v>
-      </c>
-      <c r="C100" t="s">
-        <v>340</v>
-      </c>
-      <c r="D100" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4806,13 +4813,13 @@
         <v>160</v>
       </c>
       <c r="B101" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C101" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D101" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4821,10 +4828,10 @@
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,7 +4842,7 @@
         <v>165</v>
       </c>
       <c r="D103" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4846,7 +4853,7 @@
         <v>167</v>
       </c>
       <c r="D104" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4854,10 +4861,10 @@
         <v>170</v>
       </c>
       <c r="C105" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D105" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4868,7 +4875,7 @@
         <v>168</v>
       </c>
       <c r="D106" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4879,7 +4886,7 @@
         <v>169</v>
       </c>
       <c r="D107" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4887,13 +4894,13 @@
         <v>171</v>
       </c>
       <c r="B108" t="s">
+        <v>350</v>
+      </c>
+      <c r="C108" t="s">
         <v>351</v>
       </c>
-      <c r="C108" t="s">
-        <v>352</v>
-      </c>
       <c r="D108" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4901,13 +4908,13 @@
         <v>155</v>
       </c>
       <c r="B109" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C109" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D109" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4915,10 +4922,10 @@
         <v>164</v>
       </c>
       <c r="C110" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D110" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4926,10 +4933,10 @@
         <v>174</v>
       </c>
       <c r="C111" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D111" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4937,10 +4944,10 @@
         <v>163</v>
       </c>
       <c r="C112" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D112" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4951,7 +4958,7 @@
         <v>166</v>
       </c>
       <c r="D113" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4959,10 +4966,10 @@
         <v>92</v>
       </c>
       <c r="C114" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D114" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4970,10 +4977,10 @@
         <v>96</v>
       </c>
       <c r="C115" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D115" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4981,13 +4988,13 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C116" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D116" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4995,10 +5002,10 @@
         <v>60</v>
       </c>
       <c r="C117" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="D117" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5006,13 +5013,13 @@
         <v>33</v>
       </c>
       <c r="B118" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C118" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D118" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5020,13 +5027,13 @@
         <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C119" t="s">
         <v>18</v>
       </c>
       <c r="D119" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5034,13 +5041,13 @@
         <v>25</v>
       </c>
       <c r="B120" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C120" t="s">
+        <v>330</v>
+      </c>
+      <c r="D120" t="s">
         <v>331</v>
-      </c>
-      <c r="D120" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5048,13 +5055,13 @@
         <v>1</v>
       </c>
       <c r="B121" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -5062,13 +5069,13 @@
         <v>10</v>
       </c>
       <c r="B122" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C122" t="s">
+        <v>243</v>
+      </c>
+      <c r="D122" t="s">
         <v>244</v>
-      </c>
-      <c r="D122" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -5076,13 +5083,13 @@
         <v>24</v>
       </c>
       <c r="B123" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C123" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D123" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -5090,13 +5097,13 @@
         <v>16</v>
       </c>
       <c r="B124" t="s">
+        <v>260</v>
+      </c>
+      <c r="C124" t="s">
         <v>261</v>
       </c>
-      <c r="C124" t="s">
-        <v>262</v>
-      </c>
       <c r="D124" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -5104,13 +5111,13 @@
         <v>17</v>
       </c>
       <c r="B125" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C125" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D125" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5118,7 +5125,7 @@
         <v>20</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -5128,10 +5135,10 @@
         <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D127" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5139,13 +5146,13 @@
         <v>38</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5153,13 +5160,13 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C129" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D129" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -5167,13 +5174,13 @@
         <v>28</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D130" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="D130" s="4" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5181,13 +5188,13 @@
         <v>30</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5195,13 +5202,13 @@
         <v>27</v>
       </c>
       <c r="B132" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="D132" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="D132" s="4" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -5209,13 +5216,13 @@
         <v>15</v>
       </c>
       <c r="B133" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C133" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D133" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -5223,13 +5230,13 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C134" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="D134" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,13 +5244,13 @@
         <v>6</v>
       </c>
       <c r="B135" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C135" t="s">
+        <v>246</v>
+      </c>
+      <c r="D135" t="s">
         <v>247</v>
-      </c>
-      <c r="D135" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -5251,13 +5258,13 @@
         <v>79</v>
       </c>
       <c r="B136" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C136" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="D136" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5265,13 +5272,13 @@
         <v>77</v>
       </c>
       <c r="B137" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C137" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D137" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5279,13 +5286,13 @@
         <v>76</v>
       </c>
       <c r="B138" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C138" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D138" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -5293,13 +5300,13 @@
         <v>78</v>
       </c>
       <c r="B139" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C139" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D139" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -5308,7 +5315,7 @@
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D140" s="4"/>
     </row>
@@ -5318,7 +5325,7 @@
       </c>
       <c r="B141" s="4"/>
       <c r="C141" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D141" s="4"/>
     </row>
@@ -5327,27 +5334,27 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C142" t="s">
         <v>32</v>
       </c>
       <c r="D142" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="B143" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="C143" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="D143" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5355,13 +5362,13 @@
         <v>123</v>
       </c>
       <c r="B144" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C144" t="s">
+        <v>276</v>
+      </c>
+      <c r="D144" t="s">
         <v>275</v>
-      </c>
-      <c r="C144" t="s">
-        <v>277</v>
-      </c>
-      <c r="D144" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -5369,13 +5376,13 @@
         <v>125</v>
       </c>
       <c r="B145" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C145" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D145" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -5383,13 +5390,13 @@
         <v>148</v>
       </c>
       <c r="B146" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C146" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D146" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -5397,13 +5404,13 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C147" t="s">
+        <v>239</v>
+      </c>
+      <c r="D147" t="s">
         <v>240</v>
-      </c>
-      <c r="D147" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -5411,13 +5418,13 @@
         <v>22</v>
       </c>
       <c r="B148" t="s">
+        <v>298</v>
+      </c>
+      <c r="C148" t="s">
+        <v>309</v>
+      </c>
+      <c r="D148" t="s">
         <v>299</v>
-      </c>
-      <c r="C148" t="s">
-        <v>310</v>
-      </c>
-      <c r="D148" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5426,10 +5433,10 @@
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5437,13 +5444,13 @@
         <v>58</v>
       </c>
       <c r="B150" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C150" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="D150" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5451,13 +5458,13 @@
         <v>56</v>
       </c>
       <c r="B151" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C151" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D151" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5465,13 +5472,13 @@
         <v>41</v>
       </c>
       <c r="B152" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C152" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D152" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5479,13 +5486,13 @@
         <v>44</v>
       </c>
       <c r="B153" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C153" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D153" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5493,13 +5500,13 @@
         <v>73</v>
       </c>
       <c r="B154" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C154" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="D154" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5507,13 +5514,13 @@
         <v>26</v>
       </c>
       <c r="B155" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C155" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D155" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5521,13 +5528,13 @@
         <v>87</v>
       </c>
       <c r="B156" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C156" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="D156" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5535,13 +5542,13 @@
         <v>85</v>
       </c>
       <c r="B157" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C157" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="D157" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -5549,13 +5556,13 @@
         <v>88</v>
       </c>
       <c r="B158" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C158" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="D158" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -5563,83 +5570,83 @@
         <v>86</v>
       </c>
       <c r="B159" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C159" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="D159" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="C160" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="D160" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="C161" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="D161" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C162" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="D162" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="C163" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D163" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="B164" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="B164" s="4" t="s">
-        <v>590</v>
-      </c>
       <c r="C164" s="4" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="D165" s="4" t="s">
         <v>592</v>
-      </c>
-      <c r="D165" s="4" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5647,96 +5654,104 @@
         <v>113</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="C172" s="7" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="D172" s="4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>127</v>
+      </c>
+      <c r="C173" s="7" t="s">
         <v>635</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3_0 - tidy and translated
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="649">
   <si>
     <t>dat</t>
   </si>
@@ -1297,9 +1297,6 @@
     <t>Sum of CPI adjusted OPEX, CENS, depreciation and network losses</t>
   </si>
   <si>
-    <t>Total expenditures used as input in DEA</t>
-  </si>
-  <si>
     <t>DEA efficiency scores, most recent observations, peers determined by 5 year historical average</t>
   </si>
   <si>
@@ -1630,9 +1627,6 @@
     <t>ld_gci.cost</t>
   </si>
   <si>
-    <t>Consumer Price Index, CPI by delivery sector, Services where labor dominates (Norwegian)</t>
-  </si>
-  <si>
     <t>ld_OPEX</t>
   </si>
   <si>
@@ -1952,6 +1946,36 @@
   </si>
   <si>
     <t>ld_eff.s2</t>
+  </si>
+  <si>
+    <t>Total costs used as input in DEA</t>
+  </si>
+  <si>
+    <t>faktisk.aar.kpilfaktor</t>
+  </si>
+  <si>
+    <t>KPI-lønn-faktor for estimering av fremdtidige  kostnader</t>
+  </si>
+  <si>
+    <t>y.cb.cpi.l.factor</t>
+  </si>
+  <si>
+    <t>Consumer Price Index, CPI by delivery sector, Services where labor dominates (Norwegian) (CPI Labour)</t>
+  </si>
+  <si>
+    <t>Factor of cpi.l used for estimating future cost base</t>
+  </si>
+  <si>
+    <t>faktisk.aar.kpifaktor</t>
+  </si>
+  <si>
+    <t>KPI-faktor for estimering av fremdtidige  kostnader</t>
+  </si>
+  <si>
+    <t>y.cb.cpi.factor</t>
+  </si>
+  <si>
+    <t>Factor of cpi used for estimating future cost base</t>
   </si>
 </sst>
 </file>
@@ -3499,10 +3523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D173"/>
+  <dimension ref="A2:D175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3549,10 +3573,10 @@
         <v>305</v>
       </c>
       <c r="C4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3560,10 +3584,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D5" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3574,7 +3598,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3588,7 +3612,7 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D7" t="s">
         <v>420</v>
@@ -3602,7 +3626,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3616,7 +3640,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3630,7 +3654,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3644,10 +3668,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
+        <v>538</v>
+      </c>
+      <c r="D11" t="s">
         <v>540</v>
-      </c>
-      <c r="D11" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,24 +3682,24 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>508</v>
+      </c>
+      <c r="B13" t="s">
         <v>509</v>
       </c>
-      <c r="B13" t="s">
-        <v>510</v>
-      </c>
       <c r="C13" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D13" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3686,10 +3710,10 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D14" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3700,7 +3724,7 @@
         <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D15" t="s">
         <v>193</v>
@@ -3714,10 +3738,10 @@
         <v>195</v>
       </c>
       <c r="C16" t="s">
+        <v>467</v>
+      </c>
+      <c r="D16" t="s">
         <v>468</v>
-      </c>
-      <c r="D16" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3811,10 +3835,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
+        <v>527</v>
+      </c>
+      <c r="D24" t="s">
         <v>528</v>
-      </c>
-      <c r="D24" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3822,7 +3846,7 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D25" t="s">
         <v>382</v>
@@ -3850,7 +3874,7 @@
         <v>198</v>
       </c>
       <c r="C27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D27" t="s">
         <v>199</v>
@@ -3878,10 +3902,10 @@
         <v>201</v>
       </c>
       <c r="C29" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D29" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3889,10 +3913,10 @@
         <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3900,10 +3924,10 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D31" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3911,21 +3935,21 @@
         <v>95</v>
       </c>
       <c r="C32" t="s">
+        <v>577</v>
+      </c>
+      <c r="D32" t="s">
         <v>579</v>
-      </c>
-      <c r="D32" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>487</v>
+      </c>
+      <c r="C33" t="s">
         <v>488</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>489</v>
-      </c>
-      <c r="D33" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3933,7 +3957,7 @@
         <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D34" t="s">
         <v>399</v>
@@ -3944,7 +3968,7 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D35" t="s">
         <v>400</v>
@@ -3958,52 +3982,52 @@
         <v>202</v>
       </c>
       <c r="C36" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D36" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B37" t="s">
+        <v>479</v>
+      </c>
+      <c r="C37" t="s">
         <v>480</v>
       </c>
-      <c r="C37" t="s">
-        <v>481</v>
-      </c>
       <c r="D37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>471</v>
+      </c>
+      <c r="B38" t="s">
+        <v>478</v>
+      </c>
+      <c r="C38" t="s">
         <v>472</v>
       </c>
-      <c r="B38" t="s">
-        <v>479</v>
-      </c>
-      <c r="C38" t="s">
-        <v>473</v>
-      </c>
       <c r="D38" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>481</v>
+      </c>
+      <c r="B39" t="s">
         <v>482</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>483</v>
       </c>
-      <c r="C39" t="s">
-        <v>484</v>
-      </c>
       <c r="D39" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4025,7 +4049,7 @@
         <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D41" t="s">
         <v>205</v>
@@ -4039,10 +4063,10 @@
         <v>203</v>
       </c>
       <c r="C42" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4050,7 +4074,7 @@
         <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D43" t="s">
         <v>381</v>
@@ -4061,7 +4085,7 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D44" t="s">
         <v>409</v>
@@ -4072,7 +4096,7 @@
         <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D45" t="s">
         <v>410</v>
@@ -4086,7 +4110,7 @@
         <v>206</v>
       </c>
       <c r="C46" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D46" t="s">
         <v>417</v>
@@ -4100,7 +4124,7 @@
         <v>207</v>
       </c>
       <c r="C47" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D47" t="s">
         <v>208</v>
@@ -4108,16 +4132,16 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>454</v>
+      </c>
+      <c r="B48" t="s">
         <v>455</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>456</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>457</v>
-      </c>
-      <c r="D48" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4128,7 +4152,7 @@
         <v>209</v>
       </c>
       <c r="C49" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D49" t="s">
         <v>210</v>
@@ -4139,7 +4163,7 @@
         <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D50" t="s">
         <v>408</v>
@@ -4153,10 +4177,10 @@
         <v>211</v>
       </c>
       <c r="C51" t="s">
+        <v>469</v>
+      </c>
+      <c r="D51" t="s">
         <v>470</v>
-      </c>
-      <c r="D51" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4164,7 +4188,7 @@
         <v>136</v>
       </c>
       <c r="C52" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D52" t="s">
         <v>412</v>
@@ -4290,10 +4314,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D62" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4315,10 +4339,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D64" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,10 +4350,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D65" t="s">
-        <v>422</v>
+        <v>639</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4337,10 +4361,10 @@
         <v>50</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4348,10 +4372,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D67" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4362,7 +4386,7 @@
         <v>280</v>
       </c>
       <c r="D68" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4373,32 +4397,32 @@
         <v>279</v>
       </c>
       <c r="D69" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B70" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C70" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D70" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B71" t="s">
         <v>281</v>
       </c>
       <c r="C71" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D71" t="s">
         <v>283</v>
@@ -4412,7 +4436,7 @@
         <v>282</v>
       </c>
       <c r="C72" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D72" t="s">
         <v>284</v>
@@ -4426,7 +4450,7 @@
         <v>217</v>
       </c>
       <c r="C73" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D73" t="s">
         <v>216</v>
@@ -4440,7 +4464,7 @@
         <v>219</v>
       </c>
       <c r="C74" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D74" t="s">
         <v>218</v>
@@ -4454,7 +4478,7 @@
         <v>221</v>
       </c>
       <c r="C75" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D75" t="s">
         <v>220</v>
@@ -4468,7 +4492,7 @@
         <v>223</v>
       </c>
       <c r="C76" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D76" t="s">
         <v>222</v>
@@ -4482,7 +4506,7 @@
         <v>225</v>
       </c>
       <c r="C77" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D77" t="s">
         <v>224</v>
@@ -4496,24 +4520,24 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D78" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>615</v>
+      </c>
+      <c r="B79" t="s">
+        <v>616</v>
+      </c>
+      <c r="C79" t="s">
         <v>617</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>618</v>
-      </c>
-      <c r="C79" t="s">
-        <v>619</v>
-      </c>
-      <c r="D79" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4524,7 +4548,7 @@
         <v>253</v>
       </c>
       <c r="C80" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D80" t="s">
         <v>254</v>
@@ -4532,16 +4556,16 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>500</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>501</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="C81" t="s">
         <v>502</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>503</v>
-      </c>
-      <c r="D81" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4552,7 +4576,7 @@
         <v>250</v>
       </c>
       <c r="C82" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D82" t="s">
         <v>255</v>
@@ -4566,7 +4590,7 @@
         <v>251</v>
       </c>
       <c r="C83" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D83" t="s">
         <v>256</v>
@@ -4574,30 +4598,30 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B84" t="s">
+        <v>510</v>
+      </c>
+      <c r="C84" t="s">
         <v>511</v>
       </c>
-      <c r="C84" t="s">
-        <v>512</v>
-      </c>
       <c r="D84" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>586</v>
+      </c>
+      <c r="B85" t="s">
+        <v>587</v>
+      </c>
+      <c r="C85" t="s">
         <v>588</v>
       </c>
-      <c r="B85" t="s">
-        <v>589</v>
-      </c>
-      <c r="C85" t="s">
-        <v>590</v>
-      </c>
       <c r="D85" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4608,10 +4632,10 @@
         <v>227</v>
       </c>
       <c r="C86" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D86" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4622,7 +4646,7 @@
         <v>252</v>
       </c>
       <c r="C87" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D87" t="s">
         <v>257</v>
@@ -4636,7 +4660,7 @@
         <v>228</v>
       </c>
       <c r="C88" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D88" t="s">
         <v>258</v>
@@ -4658,16 +4682,16 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>496</v>
+      </c>
+      <c r="B90" t="s">
         <v>497</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>498</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>499</v>
-      </c>
-      <c r="D90" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4678,10 +4702,10 @@
         <v>231</v>
       </c>
       <c r="C91" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="D91" s="4" t="s">
         <v>625</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4728,13 +4752,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>437</v>
+      </c>
+      <c r="C95" t="s">
+        <v>437</v>
+      </c>
+      <c r="D95" t="s">
         <v>438</v>
-      </c>
-      <c r="C95" t="s">
-        <v>438</v>
-      </c>
-      <c r="D95" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4748,7 +4772,7 @@
         <v>387</v>
       </c>
       <c r="D96" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4762,7 +4786,7 @@
         <v>349</v>
       </c>
       <c r="D97" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4827,10 +4851,10 @@
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4841,7 +4865,7 @@
         <v>165</v>
       </c>
       <c r="D103" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4852,7 +4876,7 @@
         <v>167</v>
       </c>
       <c r="D104" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4860,10 +4884,10 @@
         <v>170</v>
       </c>
       <c r="C105" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D105" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4874,7 +4898,7 @@
         <v>168</v>
       </c>
       <c r="D106" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4885,7 +4909,7 @@
         <v>169</v>
       </c>
       <c r="D107" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4899,7 +4923,7 @@
         <v>351</v>
       </c>
       <c r="D108" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4910,10 +4934,10 @@
         <v>361</v>
       </c>
       <c r="C109" t="s">
+        <v>441</v>
+      </c>
+      <c r="D109" t="s">
         <v>442</v>
-      </c>
-      <c r="D109" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4924,7 +4948,7 @@
         <v>388</v>
       </c>
       <c r="D110" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4935,7 +4959,7 @@
         <v>342</v>
       </c>
       <c r="D111" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4946,7 +4970,7 @@
         <v>341</v>
       </c>
       <c r="D112" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4957,7 +4981,7 @@
         <v>166</v>
       </c>
       <c r="D113" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -5001,10 +5025,10 @@
         <v>60</v>
       </c>
       <c r="C117" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D117" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5015,10 +5039,10 @@
         <v>336</v>
       </c>
       <c r="C118" t="s">
+        <v>449</v>
+      </c>
+      <c r="D118" t="s">
         <v>450</v>
-      </c>
-      <c r="D118" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5116,7 +5140,7 @@
         <v>262</v>
       </c>
       <c r="D125" t="s">
-        <v>533</v>
+        <v>643</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5137,7 +5161,7 @@
         <v>338</v>
       </c>
       <c r="D127" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5148,10 +5172,10 @@
         <v>396</v>
       </c>
       <c r="C128" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5162,7 +5186,7 @@
         <v>286</v>
       </c>
       <c r="C129" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D129" t="s">
         <v>285</v>
@@ -5232,7 +5256,7 @@
         <v>297</v>
       </c>
       <c r="C134" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D134" t="s">
         <v>296</v>
@@ -5260,10 +5284,10 @@
         <v>232</v>
       </c>
       <c r="C136" t="s">
+        <v>490</v>
+      </c>
+      <c r="D136" t="s">
         <v>491</v>
-      </c>
-      <c r="D136" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5314,7 +5338,7 @@
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D140" s="4"/>
     </row>
@@ -5344,16 +5368,16 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>513</v>
+      </c>
+      <c r="B143" t="s">
         <v>514</v>
       </c>
-      <c r="B143" t="s">
-        <v>515</v>
-      </c>
       <c r="C143" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D143" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5378,7 +5402,7 @@
         <v>237</v>
       </c>
       <c r="C145" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D145" t="s">
         <v>236</v>
@@ -5392,7 +5416,7 @@
         <v>238</v>
       </c>
       <c r="C146" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D146" t="s">
         <v>273</v>
@@ -5432,7 +5456,7 @@
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D149" s="7" t="s">
         <v>397</v>
@@ -5446,10 +5470,10 @@
         <v>320</v>
       </c>
       <c r="C150" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D150" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5502,10 +5526,10 @@
         <v>324</v>
       </c>
       <c r="C154" t="s">
+        <v>542</v>
+      </c>
+      <c r="D154" t="s">
         <v>544</v>
-      </c>
-      <c r="D154" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5519,7 +5543,7 @@
         <v>337</v>
       </c>
       <c r="D155" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5530,10 +5554,10 @@
         <v>267</v>
       </c>
       <c r="C156" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D156" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5544,7 +5568,7 @@
         <v>268</v>
       </c>
       <c r="C157" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D157" t="s">
         <v>265</v>
@@ -5558,10 +5582,10 @@
         <v>269</v>
       </c>
       <c r="C158" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D158" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -5572,7 +5596,7 @@
         <v>270</v>
       </c>
       <c r="C159" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D159" t="s">
         <v>266</v>
@@ -5580,72 +5604,72 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C160" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D160" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C161" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D161" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C162" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D162" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C163" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D163" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5653,105 +5677,133 @@
         <v>113</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="C167" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="D167" s="4" t="s">
         <v>594</v>
-      </c>
-      <c r="C167" s="4" t="s">
-        <v>595</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="C168" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="D168" s="4" t="s">
         <v>599</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="D168" s="4" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C169" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="D169" s="4" t="s">
         <v>603</v>
-      </c>
-      <c r="C169" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="D169" s="4" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C170" s="7" t="s">
         <v>607</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="D170" s="4" t="s">
         <v>608</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>609</v>
-      </c>
-      <c r="D170" s="4" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="C171" s="7" t="s">
         <v>611</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="D171" s="4" t="s">
         <v>612</v>
-      </c>
-      <c r="C171" s="7" t="s">
-        <v>613</v>
-      </c>
-      <c r="D171" s="4" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B172" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="C172" s="7" t="s">
         <v>624</v>
       </c>
-      <c r="C172" s="7" t="s">
+      <c r="D172" s="4" t="s">
         <v>626</v>
-      </c>
-      <c r="D172" s="4" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>127</v>
       </c>
-      <c r="C173" s="7" t="s">
-        <v>634</v>
+      <c r="C173" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>640</v>
+      </c>
+      <c r="B174" t="s">
+        <v>641</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>645</v>
+      </c>
+      <c r="B175" t="s">
+        <v>646</v>
+      </c>
+      <c r="C175" s="7" t="s">
+        <v>647</v>
+      </c>
+      <c r="D175" s="4" t="s">
+        <v>648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OOTO translated, micro dev for ids 35, 162 & 173 due to lack of rounding i Stata
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="659">
   <si>
     <t>dat</t>
   </si>
@@ -862,12 +862,6 @@
     <t>rg_Geo1</t>
   </si>
   <si>
-    <t>d_out</t>
-  </si>
-  <si>
-    <t>d_out.NOK</t>
-  </si>
-  <si>
     <t>dea.avg.avg.d</t>
   </si>
   <si>
@@ -901,15 +895,6 @@
     <t>Normpris per nettstasjon</t>
   </si>
   <si>
-    <t>d_sub.NOK</t>
-  </si>
-  <si>
-    <t>d_hv.NOK</t>
-  </si>
-  <si>
-    <t>d_gs.NOK</t>
-  </si>
-  <si>
     <t>Datasett for Hammerfest</t>
   </si>
   <si>
@@ -1060,9 +1045,6 @@
     <t>drs_TOTRC.poscal</t>
   </si>
   <si>
-    <t>Norm price per grid station</t>
-  </si>
-  <si>
     <t>Norm price per km high voltage grid</t>
   </si>
   <si>
@@ -1270,12 +1252,6 @@
     <t>Data frame for companies that are exempted from the regular model, critereas described in … (out of the ordinary)</t>
   </si>
   <si>
-    <t>Calculated costs of outputs for companies in the OOTO model</t>
-  </si>
-  <si>
-    <t>Calculated output for companies in the OOTO model</t>
-  </si>
-  <si>
     <t>Pension costs</t>
   </si>
   <si>
@@ -1976,6 +1952,60 @@
   </si>
   <si>
     <t>Factor of cpi used for estimating future cost base</t>
+  </si>
+  <si>
+    <t>ld_sub.NOK</t>
+  </si>
+  <si>
+    <t>ld_hv.NOK</t>
+  </si>
+  <si>
+    <t>Norm price per substation</t>
+  </si>
+  <si>
+    <t>ld_ss.NOK</t>
+  </si>
+  <si>
+    <t>sf_d_ab</t>
+  </si>
+  <si>
+    <t>sf_d_hs</t>
+  </si>
+  <si>
+    <t>sf_d_ns</t>
+  </si>
+  <si>
+    <t>sf_d_TOTXDEA</t>
+  </si>
+  <si>
+    <t>ld_output</t>
+  </si>
+  <si>
+    <t>ld_output.NOK</t>
+  </si>
+  <si>
+    <t>d_sf_d_oppgave</t>
+  </si>
+  <si>
+    <t>fha_ld_output</t>
+  </si>
+  <si>
+    <t>output i kroner, for årene i  y.avg</t>
+  </si>
+  <si>
+    <t>output in NOK, five years historical average (years in y.avg)</t>
+  </si>
+  <si>
+    <t>Calculate ratio between costs and outputs i NOK for companies in the OOTO model</t>
+  </si>
+  <si>
+    <t>Calculated output for companies in the OOTO model, in NOK</t>
+  </si>
+  <si>
+    <t>ld_ooto</t>
+  </si>
+  <si>
+    <t>ld_cn.cal.RAB</t>
   </si>
 </sst>
 </file>
@@ -3523,10 +3553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D175"/>
+  <dimension ref="A2:D176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3570,13 +3600,13 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C4" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="D4" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3584,10 +3614,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>634</v>
+        <v>626</v>
       </c>
       <c r="D5" t="s">
-        <v>633</v>
+        <v>625</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3598,7 +3628,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3612,10 +3642,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="D7" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3626,7 +3656,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3640,7 +3670,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3654,7 +3684,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3668,10 +3698,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="D11" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3682,24 +3712,24 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="D12" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="B13" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="C13" t="s">
-        <v>620</v>
+        <v>612</v>
       </c>
       <c r="D13" t="s">
-        <v>636</v>
+        <v>628</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3710,10 +3740,10 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="D14" t="s">
-        <v>637</v>
+        <v>629</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3724,7 +3754,7 @@
         <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="D15" t="s">
         <v>193</v>
@@ -3738,10 +3768,10 @@
         <v>195</v>
       </c>
       <c r="C16" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="D16" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3752,7 +3782,7 @@
         <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3760,13 +3790,13 @@
         <v>156</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C18" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D18" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3777,7 +3807,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3785,13 +3815,13 @@
         <v>152</v>
       </c>
       <c r="B20" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C20" t="s">
         <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3799,10 +3829,10 @@
         <v>158</v>
       </c>
       <c r="C21" t="s">
-        <v>158</v>
+        <v>658</v>
       </c>
       <c r="D21" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3810,13 +3840,13 @@
         <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C22" t="s">
         <v>159</v>
       </c>
       <c r="D22" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,7 +3857,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,10 +3865,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="D24" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,10 +3876,10 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>638</v>
+        <v>630</v>
       </c>
       <c r="D25" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3860,7 +3890,7 @@
         <v>196</v>
       </c>
       <c r="C26" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D26" t="s">
         <v>197</v>
@@ -3874,7 +3904,7 @@
         <v>198</v>
       </c>
       <c r="C27" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="D27" t="s">
         <v>199</v>
@@ -3885,10 +3915,10 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>200</v>
@@ -3902,10 +3932,10 @@
         <v>201</v>
       </c>
       <c r="C29" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="D29" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3913,10 +3943,10 @@
         <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>630</v>
+        <v>622</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3924,10 +3954,10 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="D31" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3935,21 +3965,21 @@
         <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="D32" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C33" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="D33" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3957,10 +3987,10 @@
         <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="D34" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3968,10 +3998,10 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="D35" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3982,52 +4012,52 @@
         <v>202</v>
       </c>
       <c r="C36" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="D36" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="B37" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C37" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="D37" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B38" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="C38" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="D38" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B39" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="C39" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="D39" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4035,10 +4065,10 @@
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D40" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4049,7 +4079,7 @@
         <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="D41" t="s">
         <v>205</v>
@@ -4063,10 +4093,10 @@
         <v>203</v>
       </c>
       <c r="C42" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="D42" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4074,10 +4104,10 @@
         <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="D43" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4085,10 +4115,10 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="D44" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4096,10 +4126,10 @@
         <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="D45" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4110,10 +4140,10 @@
         <v>206</v>
       </c>
       <c r="C46" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="D46" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4124,7 +4154,7 @@
         <v>207</v>
       </c>
       <c r="C47" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="D47" t="s">
         <v>208</v>
@@ -4132,16 +4162,16 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B48" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="C48" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="D48" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4152,7 +4182,7 @@
         <v>209</v>
       </c>
       <c r="C49" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="D49" t="s">
         <v>210</v>
@@ -4163,10 +4193,10 @@
         <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="D50" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4177,10 +4207,10 @@
         <v>211</v>
       </c>
       <c r="C51" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="D51" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4188,10 +4218,10 @@
         <v>136</v>
       </c>
       <c r="C52" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="D52" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4200,10 +4230,10 @@
       </c>
       <c r="B53" s="6"/>
       <c r="C53" t="s">
-        <v>277</v>
+        <v>649</v>
       </c>
       <c r="D53" t="s">
-        <v>414</v>
+        <v>656</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4211,10 +4241,10 @@
         <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>278</v>
+        <v>650</v>
       </c>
       <c r="D54" t="s">
-        <v>413</v>
+        <v>655</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4228,7 +4258,7 @@
         <v>213</v>
       </c>
       <c r="D55" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4242,7 +4272,7 @@
         <v>215</v>
       </c>
       <c r="D56" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4250,13 +4280,13 @@
         <v>138</v>
       </c>
       <c r="B57" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C57" t="s">
-        <v>290</v>
+        <v>641</v>
       </c>
       <c r="D57" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4264,13 +4294,13 @@
         <v>139</v>
       </c>
       <c r="B58" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C58" t="s">
-        <v>291</v>
+        <v>642</v>
       </c>
       <c r="D58" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4278,13 +4308,13 @@
         <v>140</v>
       </c>
       <c r="B59" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C59" t="s">
-        <v>292</v>
+        <v>644</v>
       </c>
       <c r="D59" t="s">
-        <v>343</v>
+        <v>643</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4292,10 +4322,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="D60" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4303,10 +4333,10 @@
         <v>95</v>
       </c>
       <c r="C61" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D61" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4314,10 +4344,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>526</v>
+        <v>657</v>
       </c>
       <c r="D62" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4325,13 +4355,13 @@
         <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C63" t="s">
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4339,10 +4369,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="D64" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4350,10 +4380,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="D65" t="s">
-        <v>639</v>
+        <v>631</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4361,10 +4391,10 @@
         <v>50</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4372,10 +4402,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="D67" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4383,10 +4413,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D68" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4394,38 +4424,38 @@
         <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D69" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="B70" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="C70" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="D70" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>619</v>
+        <v>611</v>
       </c>
       <c r="B71" t="s">
+        <v>279</v>
+      </c>
+      <c r="C71" t="s">
+        <v>510</v>
+      </c>
+      <c r="D71" t="s">
         <v>281</v>
-      </c>
-      <c r="C71" t="s">
-        <v>518</v>
-      </c>
-      <c r="D71" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4433,13 +4463,13 @@
         <v>109</v>
       </c>
       <c r="B72" t="s">
+        <v>280</v>
+      </c>
+      <c r="C72" t="s">
+        <v>511</v>
+      </c>
+      <c r="D72" t="s">
         <v>282</v>
-      </c>
-      <c r="C72" t="s">
-        <v>519</v>
-      </c>
-      <c r="D72" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4450,7 +4480,7 @@
         <v>217</v>
       </c>
       <c r="C73" t="s">
-        <v>627</v>
+        <v>619</v>
       </c>
       <c r="D73" t="s">
         <v>216</v>
@@ -4464,7 +4494,7 @@
         <v>219</v>
       </c>
       <c r="C74" t="s">
-        <v>628</v>
+        <v>620</v>
       </c>
       <c r="D74" t="s">
         <v>218</v>
@@ -4478,7 +4508,7 @@
         <v>221</v>
       </c>
       <c r="C75" t="s">
-        <v>629</v>
+        <v>621</v>
       </c>
       <c r="D75" t="s">
         <v>220</v>
@@ -4492,7 +4522,7 @@
         <v>223</v>
       </c>
       <c r="C76" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="D76" t="s">
         <v>222</v>
@@ -4506,7 +4536,7 @@
         <v>225</v>
       </c>
       <c r="C77" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="D77" t="s">
         <v>224</v>
@@ -4520,24 +4550,24 @@
         <v>226</v>
       </c>
       <c r="C78" t="s">
-        <v>614</v>
+        <v>606</v>
       </c>
       <c r="D78" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>615</v>
+        <v>607</v>
       </c>
       <c r="B79" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
       <c r="C79" t="s">
-        <v>617</v>
+        <v>609</v>
       </c>
       <c r="D79" t="s">
-        <v>618</v>
+        <v>610</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4548,7 +4578,7 @@
         <v>253</v>
       </c>
       <c r="C80" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="D80" t="s">
         <v>254</v>
@@ -4556,16 +4586,16 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="C81" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="D81" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4576,7 +4606,7 @@
         <v>250</v>
       </c>
       <c r="C82" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="D82" t="s">
         <v>255</v>
@@ -4590,7 +4620,7 @@
         <v>251</v>
       </c>
       <c r="C83" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="D83" t="s">
         <v>256</v>
@@ -4598,30 +4628,30 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="B84" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="C84" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="D84" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="B85" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="C85" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="D85" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4632,10 +4662,10 @@
         <v>227</v>
       </c>
       <c r="C86" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="D86" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4646,7 +4676,7 @@
         <v>252</v>
       </c>
       <c r="C87" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="D87" t="s">
         <v>257</v>
@@ -4660,7 +4690,7 @@
         <v>228</v>
       </c>
       <c r="C88" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="D88" t="s">
         <v>258</v>
@@ -4674,7 +4704,7 @@
         <v>230</v>
       </c>
       <c r="C89" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D89" t="s">
         <v>229</v>
@@ -4682,16 +4712,16 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="B90" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="C90" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="D90" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4702,10 +4732,10 @@
         <v>231</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>623</v>
+        <v>615</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4713,13 +4743,13 @@
         <v>176</v>
       </c>
       <c r="B92" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C92" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D92" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,13 +4757,13 @@
         <v>162</v>
       </c>
       <c r="B93" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C93" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D93" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4741,24 +4771,24 @@
         <v>154</v>
       </c>
       <c r="B94" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C94" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D94" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="C95" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="D95" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4766,13 +4796,13 @@
         <v>153</v>
       </c>
       <c r="B96" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C96" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D96" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4780,13 +4810,13 @@
         <v>172</v>
       </c>
       <c r="B97" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C97" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D97" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4794,13 +4824,13 @@
         <v>175</v>
       </c>
       <c r="B98" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="C98" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D98" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4808,13 +4838,13 @@
         <v>161</v>
       </c>
       <c r="B99" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C99" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D99" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4822,13 +4852,13 @@
         <v>173</v>
       </c>
       <c r="B100" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C100" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D100" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,13 +4866,13 @@
         <v>160</v>
       </c>
       <c r="B101" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="C101" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D101" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4851,10 +4881,10 @@
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4865,7 +4895,7 @@
         <v>165</v>
       </c>
       <c r="D103" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4876,7 +4906,7 @@
         <v>167</v>
       </c>
       <c r="D104" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4884,10 +4914,10 @@
         <v>170</v>
       </c>
       <c r="C105" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="D105" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4898,7 +4928,7 @@
         <v>168</v>
       </c>
       <c r="D106" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4909,7 +4939,7 @@
         <v>169</v>
       </c>
       <c r="D107" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4917,13 +4947,13 @@
         <v>171</v>
       </c>
       <c r="B108" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C108" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D108" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4931,13 +4961,13 @@
         <v>155</v>
       </c>
       <c r="B109" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C109" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="D109" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4945,10 +4975,10 @@
         <v>164</v>
       </c>
       <c r="C110" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D110" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4956,10 +4986,10 @@
         <v>174</v>
       </c>
       <c r="C111" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D111" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4967,10 +4997,10 @@
         <v>163</v>
       </c>
       <c r="C112" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D112" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4981,7 +5011,7 @@
         <v>166</v>
       </c>
       <c r="D113" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4989,10 +5019,10 @@
         <v>92</v>
       </c>
       <c r="C114" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="D114" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -5000,10 +5030,10 @@
         <v>96</v>
       </c>
       <c r="C115" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D115" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -5011,13 +5041,13 @@
         <v>23</v>
       </c>
       <c r="B116" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C116" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D116" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -5025,10 +5055,10 @@
         <v>60</v>
       </c>
       <c r="C117" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="D117" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5036,13 +5066,13 @@
         <v>33</v>
       </c>
       <c r="B118" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="C118" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="D118" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5050,13 +5080,13 @@
         <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C119" t="s">
         <v>18</v>
       </c>
       <c r="D119" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -5067,10 +5097,10 @@
         <v>259</v>
       </c>
       <c r="C120" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D120" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -5106,13 +5136,13 @@
         <v>24</v>
       </c>
       <c r="B123" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C123" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D123" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -5140,7 +5170,7 @@
         <v>262</v>
       </c>
       <c r="D125" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5148,7 +5178,7 @@
         <v>20</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -5158,10 +5188,10 @@
         <v>5</v>
       </c>
       <c r="C127" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D127" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5169,13 +5199,13 @@
         <v>38</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5183,13 +5213,13 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C129" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="D129" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -5197,13 +5227,13 @@
         <v>28</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -5211,13 +5241,13 @@
         <v>30</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -5225,13 +5255,13 @@
         <v>27</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -5239,13 +5269,13 @@
         <v>15</v>
       </c>
       <c r="B133" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C133" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D133" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -5253,13 +5283,13 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C134" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="D134" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -5284,10 +5314,10 @@
         <v>232</v>
       </c>
       <c r="C136" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="D136" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5298,10 +5328,10 @@
         <v>233</v>
       </c>
       <c r="C137" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D137" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -5312,10 +5342,10 @@
         <v>234</v>
       </c>
       <c r="C138" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D138" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -5326,10 +5356,10 @@
         <v>235</v>
       </c>
       <c r="C139" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D139" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -5338,7 +5368,7 @@
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="D140" s="4"/>
     </row>
@@ -5348,7 +5378,7 @@
       </c>
       <c r="B141" s="4"/>
       <c r="C141" s="4" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="D141" s="4"/>
     </row>
@@ -5368,16 +5398,16 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>505</v>
+      </c>
+      <c r="B143" t="s">
+        <v>506</v>
+      </c>
+      <c r="C143" t="s">
+        <v>508</v>
+      </c>
+      <c r="D143" t="s">
         <v>513</v>
-      </c>
-      <c r="B143" t="s">
-        <v>514</v>
-      </c>
-      <c r="C143" t="s">
-        <v>516</v>
-      </c>
-      <c r="D143" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5402,7 +5432,7 @@
         <v>237</v>
       </c>
       <c r="C145" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="D145" t="s">
         <v>236</v>
@@ -5416,7 +5446,7 @@
         <v>238</v>
       </c>
       <c r="C146" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="D146" t="s">
         <v>273</v>
@@ -5427,7 +5457,7 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C147" t="s">
         <v>239</v>
@@ -5441,13 +5471,13 @@
         <v>22</v>
       </c>
       <c r="B148" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C148" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D148" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -5456,10 +5486,10 @@
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5467,13 +5497,13 @@
         <v>58</v>
       </c>
       <c r="B150" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C150" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="D150" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5481,13 +5511,13 @@
         <v>56</v>
       </c>
       <c r="B151" t="s">
+        <v>316</v>
+      </c>
+      <c r="C151" t="s">
+        <v>314</v>
+      </c>
+      <c r="D151" t="s">
         <v>321</v>
-      </c>
-      <c r="C151" t="s">
-        <v>319</v>
-      </c>
-      <c r="D151" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -5495,13 +5525,13 @@
         <v>41</v>
       </c>
       <c r="B152" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C152" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D152" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -5509,13 +5539,13 @@
         <v>44</v>
       </c>
       <c r="B153" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C153" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D153" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -5523,13 +5553,13 @@
         <v>73</v>
       </c>
       <c r="B154" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C154" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="D154" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5537,13 +5567,13 @@
         <v>26</v>
       </c>
       <c r="B155" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C155" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D155" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5554,10 +5584,10 @@
         <v>267</v>
       </c>
       <c r="C156" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="D156" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5568,7 +5598,7 @@
         <v>268</v>
       </c>
       <c r="C157" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="D157" t="s">
         <v>265</v>
@@ -5582,10 +5612,10 @@
         <v>269</v>
       </c>
       <c r="C158" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="D158" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -5596,80 +5626,92 @@
         <v>270</v>
       </c>
       <c r="C159" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="D159" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>648</v>
+      </c>
       <c r="B160" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="C160" t="s">
+        <v>541</v>
+      </c>
+      <c r="D160" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>645</v>
+      </c>
+      <c r="B161" t="s">
         <v>549</v>
       </c>
-      <c r="D160" t="s">
+      <c r="C161" t="s">
+        <v>544</v>
+      </c>
+      <c r="D161" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>646</v>
+      </c>
+      <c r="B162" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
-        <v>557</v>
-      </c>
-      <c r="C161" t="s">
+      <c r="C162" t="s">
+        <v>546</v>
+      </c>
+      <c r="D162" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>647</v>
+      </c>
+      <c r="B163" t="s">
         <v>552</v>
       </c>
-      <c r="D161" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
-        <v>558</v>
-      </c>
-      <c r="C162" t="s">
-        <v>554</v>
-      </c>
-      <c r="D162" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>560</v>
-      </c>
       <c r="C163" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="D163" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5677,97 +5719,97 @@
         <v>113</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>610</v>
+        <v>602</v>
       </c>
       <c r="C171" s="7" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>612</v>
+        <v>604</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>622</v>
+        <v>614</v>
       </c>
       <c r="C172" s="7" t="s">
-        <v>624</v>
+        <v>616</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5775,35 +5817,49 @@
         <v>127</v>
       </c>
       <c r="C173" t="s">
-        <v>632</v>
+        <v>624</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="B174" t="s">
-        <v>641</v>
-      </c>
-      <c r="C174" s="7" t="s">
-        <v>642</v>
-      </c>
-      <c r="D174" s="4" t="s">
-        <v>644</v>
+        <v>633</v>
+      </c>
+      <c r="C174" t="s">
+        <v>634</v>
+      </c>
+      <c r="D174" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="B175" t="s">
-        <v>646</v>
-      </c>
-      <c r="C175" s="7" t="s">
-        <v>647</v>
-      </c>
-      <c r="D175" s="4" t="s">
-        <v>648</v>
+        <v>638</v>
+      </c>
+      <c r="C175" t="s">
+        <v>639</v>
+      </c>
+      <c r="D175" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>651</v>
+      </c>
+      <c r="B176" t="s">
+        <v>653</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="D176" s="6" t="s">
+        <v>654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RevCap - 50 % translated
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -3564,8 +3564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Merger part of HI calc ok
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -1192,9 +1192,6 @@
     <t>NVE.ir.RC</t>
   </si>
   <si>
-    <t>NVE.ir.t-2</t>
-  </si>
-  <si>
     <t>Referansepris på kraft, estimert i varsel</t>
   </si>
   <si>
@@ -2015,6 +2012,9 @@
   </si>
   <si>
     <t>faktisk.aar.kpiafaktor</t>
+  </si>
+  <si>
+    <t>NVE.ir.t_2</t>
   </si>
 </sst>
 </file>
@@ -3564,8 +3564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3612,10 +3612,10 @@
         <v>298</v>
       </c>
       <c r="C4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3623,10 +3623,10 @@
         <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3637,7 +3637,7 @@
         <v>182</v>
       </c>
       <c r="C6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D6" t="s">
         <v>181</v>
@@ -3651,10 +3651,10 @@
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,7 +3665,7 @@
         <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D8" t="s">
         <v>185</v>
@@ -3679,7 +3679,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D9" t="s">
         <v>186</v>
@@ -3693,7 +3693,7 @@
         <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D10" t="s">
         <v>189</v>
@@ -3707,10 +3707,10 @@
         <v>190</v>
       </c>
       <c r="C11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D11" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3721,24 +3721,24 @@
         <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D12" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>497</v>
+      </c>
+      <c r="B13" t="s">
         <v>498</v>
       </c>
-      <c r="B13" t="s">
-        <v>499</v>
-      </c>
       <c r="C13" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D13" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3749,10 +3749,10 @@
         <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D14" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3763,7 +3763,7 @@
         <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D15" t="s">
         <v>193</v>
@@ -3777,10 +3777,10 @@
         <v>195</v>
       </c>
       <c r="C16" t="s">
+        <v>456</v>
+      </c>
+      <c r="D16" t="s">
         <v>457</v>
-      </c>
-      <c r="D16" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3791,7 +3791,7 @@
         <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3802,10 +3802,10 @@
         <v>354</v>
       </c>
       <c r="C18" t="s">
+        <v>392</v>
+      </c>
+      <c r="D18" t="s">
         <v>393</v>
-      </c>
-      <c r="D18" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3816,7 +3816,7 @@
         <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3838,10 +3838,10 @@
         <v>158</v>
       </c>
       <c r="C21" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3866,7 +3866,7 @@
         <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3874,10 +3874,10 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
+        <v>516</v>
+      </c>
+      <c r="D24" t="s">
         <v>517</v>
-      </c>
-      <c r="D24" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3885,7 +3885,7 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D25" t="s">
         <v>374</v>
@@ -3899,7 +3899,7 @@
         <v>196</v>
       </c>
       <c r="C26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D26" t="s">
         <v>197</v>
@@ -3913,7 +3913,7 @@
         <v>198</v>
       </c>
       <c r="C27" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D27" t="s">
         <v>199</v>
@@ -3927,7 +3927,7 @@
         <v>288</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>200</v>
@@ -3941,10 +3941,10 @@
         <v>201</v>
       </c>
       <c r="C29" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3952,10 +3952,10 @@
         <v>112</v>
       </c>
       <c r="C30" t="s">
+        <v>619</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>620</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3963,10 +3963,10 @@
         <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D31" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3974,21 +3974,21 @@
         <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D32" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>476</v>
+      </c>
+      <c r="C33" t="s">
         <v>477</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>478</v>
-      </c>
-      <c r="D33" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3996,10 +3996,10 @@
         <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D34" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4007,10 +4007,10 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D35" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4021,52 +4021,52 @@
         <v>202</v>
       </c>
       <c r="C36" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D36" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B37" t="s">
+        <v>468</v>
+      </c>
+      <c r="C37" t="s">
         <v>469</v>
       </c>
-      <c r="C37" t="s">
-        <v>470</v>
-      </c>
       <c r="D37" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>460</v>
+      </c>
+      <c r="B38" t="s">
+        <v>467</v>
+      </c>
+      <c r="C38" t="s">
         <v>461</v>
       </c>
-      <c r="B38" t="s">
-        <v>468</v>
-      </c>
-      <c r="C38" t="s">
-        <v>462</v>
-      </c>
       <c r="D38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>470</v>
+      </c>
+      <c r="B39" t="s">
         <v>471</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>472</v>
       </c>
-      <c r="C39" t="s">
-        <v>473</v>
-      </c>
       <c r="D39" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4088,7 +4088,7 @@
         <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D41" t="s">
         <v>205</v>
@@ -4102,10 +4102,10 @@
         <v>203</v>
       </c>
       <c r="C42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D42" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4113,7 +4113,7 @@
         <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D43" t="s">
         <v>373</v>
@@ -4124,10 +4124,10 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D44" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4135,10 +4135,10 @@
         <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D45" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4149,10 +4149,10 @@
         <v>206</v>
       </c>
       <c r="C46" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D46" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4163,7 +4163,7 @@
         <v>207</v>
       </c>
       <c r="C47" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D47" t="s">
         <v>208</v>
@@ -4171,16 +4171,16 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>443</v>
+      </c>
+      <c r="B48" t="s">
         <v>444</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>445</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>446</v>
-      </c>
-      <c r="D48" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4191,7 +4191,7 @@
         <v>209</v>
       </c>
       <c r="C49" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D49" t="s">
         <v>210</v>
@@ -4202,10 +4202,10 @@
         <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D50" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4216,10 +4216,10 @@
         <v>211</v>
       </c>
       <c r="C51" t="s">
+        <v>458</v>
+      </c>
+      <c r="D51" t="s">
         <v>459</v>
-      </c>
-      <c r="D51" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4227,10 +4227,10 @@
         <v>136</v>
       </c>
       <c r="C52" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D52" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4239,10 +4239,10 @@
       </c>
       <c r="B53" s="6"/>
       <c r="C53" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D53" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4250,10 +4250,10 @@
         <v>143</v>
       </c>
       <c r="C54" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D54" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4264,10 +4264,10 @@
         <v>212</v>
       </c>
       <c r="C55" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D55" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4278,10 +4278,10 @@
         <v>213</v>
       </c>
       <c r="C56" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D56" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4292,10 +4292,10 @@
         <v>283</v>
       </c>
       <c r="C57" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D57" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4306,7 +4306,7 @@
         <v>284</v>
       </c>
       <c r="C58" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D58" t="s">
         <v>336</v>
@@ -4320,10 +4320,10 @@
         <v>285</v>
       </c>
       <c r="C59" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D59" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4334,7 +4334,7 @@
         <v>372</v>
       </c>
       <c r="D60" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4353,10 +4353,10 @@
         <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D62" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4370,7 +4370,7 @@
         <v>151</v>
       </c>
       <c r="D63" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4378,10 +4378,10 @@
         <v>81</v>
       </c>
       <c r="C64" t="s">
+        <v>534</v>
+      </c>
+      <c r="D64" t="s">
         <v>535</v>
-      </c>
-      <c r="D64" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4389,10 +4389,10 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D65" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4400,10 +4400,10 @@
         <v>50</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4411,10 +4411,10 @@
         <v>90</v>
       </c>
       <c r="C67" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D67" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4425,7 +4425,7 @@
         <v>276</v>
       </c>
       <c r="D68" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4436,32 +4436,32 @@
         <v>275</v>
       </c>
       <c r="D69" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B70" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C70" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D70" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B71" t="s">
         <v>277</v>
       </c>
       <c r="C71" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D71" t="s">
         <v>279</v>
@@ -4475,7 +4475,7 @@
         <v>278</v>
       </c>
       <c r="C72" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D72" t="s">
         <v>280</v>
@@ -4489,7 +4489,7 @@
         <v>215</v>
       </c>
       <c r="C73" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D73" t="s">
         <v>214</v>
@@ -4503,7 +4503,7 @@
         <v>217</v>
       </c>
       <c r="C74" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D74" t="s">
         <v>216</v>
@@ -4517,7 +4517,7 @@
         <v>219</v>
       </c>
       <c r="C75" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D75" t="s">
         <v>218</v>
@@ -4531,7 +4531,7 @@
         <v>221</v>
       </c>
       <c r="C76" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D76" t="s">
         <v>220</v>
@@ -4545,7 +4545,7 @@
         <v>223</v>
       </c>
       <c r="C77" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D77" t="s">
         <v>222</v>
@@ -4559,24 +4559,24 @@
         <v>224</v>
       </c>
       <c r="C78" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D78" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>604</v>
+      </c>
+      <c r="B79" t="s">
         <v>605</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>606</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>607</v>
-      </c>
-      <c r="D79" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4587,7 +4587,7 @@
         <v>251</v>
       </c>
       <c r="C80" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D80" t="s">
         <v>252</v>
@@ -4595,16 +4595,16 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>489</v>
+      </c>
+      <c r="B81" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="B81" s="6" t="s">
+      <c r="C81" t="s">
         <v>491</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>492</v>
-      </c>
-      <c r="D81" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4615,7 +4615,7 @@
         <v>248</v>
       </c>
       <c r="C82" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D82" t="s">
         <v>253</v>
@@ -4629,7 +4629,7 @@
         <v>249</v>
       </c>
       <c r="C83" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D83" t="s">
         <v>254</v>
@@ -4637,30 +4637,30 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B84" t="s">
+        <v>499</v>
+      </c>
+      <c r="C84" t="s">
         <v>500</v>
       </c>
-      <c r="C84" t="s">
-        <v>501</v>
-      </c>
       <c r="D84" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>575</v>
+      </c>
+      <c r="B85" t="s">
         <v>576</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>577</v>
       </c>
-      <c r="C85" t="s">
-        <v>578</v>
-      </c>
       <c r="D85" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,10 +4671,10 @@
         <v>225</v>
       </c>
       <c r="C86" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D86" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4685,7 +4685,7 @@
         <v>250</v>
       </c>
       <c r="C87" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D87" t="s">
         <v>255</v>
@@ -4699,7 +4699,7 @@
         <v>226</v>
       </c>
       <c r="C88" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D88" t="s">
         <v>256</v>
@@ -4721,16 +4721,16 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>485</v>
+      </c>
+      <c r="B90" t="s">
         <v>486</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>487</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>488</v>
-      </c>
-      <c r="D90" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4741,10 +4741,10 @@
         <v>229</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4791,13 +4791,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>426</v>
+      </c>
+      <c r="C95" t="s">
+        <v>426</v>
+      </c>
+      <c r="D95" t="s">
         <v>427</v>
-      </c>
-      <c r="C95" t="s">
-        <v>427</v>
-      </c>
-      <c r="D95" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4811,7 +4811,7 @@
         <v>379</v>
       </c>
       <c r="D96" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4825,7 +4825,7 @@
         <v>341</v>
       </c>
       <c r="D97" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4890,10 +4890,10 @@
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4904,7 +4904,7 @@
         <v>165</v>
       </c>
       <c r="D103" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4915,7 +4915,7 @@
         <v>167</v>
       </c>
       <c r="D104" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4923,10 +4923,10 @@
         <v>170</v>
       </c>
       <c r="C105" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D105" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4937,7 +4937,7 @@
         <v>168</v>
       </c>
       <c r="D106" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4948,7 +4948,7 @@
         <v>169</v>
       </c>
       <c r="D107" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4962,7 +4962,7 @@
         <v>343</v>
       </c>
       <c r="D108" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4973,10 +4973,10 @@
         <v>353</v>
       </c>
       <c r="C109" t="s">
+        <v>430</v>
+      </c>
+      <c r="D109" t="s">
         <v>431</v>
-      </c>
-      <c r="D109" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4987,7 +4987,7 @@
         <v>380</v>
       </c>
       <c r="D110" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4998,7 +4998,7 @@
         <v>335</v>
       </c>
       <c r="D111" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -5009,7 +5009,7 @@
         <v>334</v>
       </c>
       <c r="D112" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -5020,7 +5020,7 @@
         <v>166</v>
       </c>
       <c r="D113" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -5064,10 +5064,10 @@
         <v>60</v>
       </c>
       <c r="C117" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D117" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -5078,10 +5078,10 @@
         <v>329</v>
       </c>
       <c r="C118" t="s">
+        <v>438</v>
+      </c>
+      <c r="D118" t="s">
         <v>439</v>
-      </c>
-      <c r="D118" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -5179,7 +5179,7 @@
         <v>260</v>
       </c>
       <c r="D125" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -5200,7 +5200,7 @@
         <v>331</v>
       </c>
       <c r="D127" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -5208,13 +5208,13 @@
         <v>38</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C128" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D128" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -5225,7 +5225,7 @@
         <v>282</v>
       </c>
       <c r="C129" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D129" t="s">
         <v>281</v>
@@ -5267,7 +5267,7 @@
         <v>303</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>387</v>
+        <v>661</v>
       </c>
       <c r="D132" s="4" t="s">
         <v>304</v>
@@ -5295,7 +5295,7 @@
         <v>290</v>
       </c>
       <c r="C134" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D134" t="s">
         <v>289</v>
@@ -5323,10 +5323,10 @@
         <v>230</v>
       </c>
       <c r="C136" t="s">
+        <v>479</v>
+      </c>
+      <c r="D136" t="s">
         <v>480</v>
-      </c>
-      <c r="D136" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D140" s="4"/>
     </row>
@@ -5407,16 +5407,16 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>502</v>
+      </c>
+      <c r="B143" t="s">
         <v>503</v>
       </c>
-      <c r="B143" t="s">
-        <v>504</v>
-      </c>
       <c r="C143" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D143" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -5441,7 +5441,7 @@
         <v>235</v>
       </c>
       <c r="C145" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D145" t="s">
         <v>234</v>
@@ -5455,7 +5455,7 @@
         <v>236</v>
       </c>
       <c r="C146" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D146" t="s">
         <v>271</v>
@@ -5466,7 +5466,7 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C147" t="s">
         <v>237</v>
@@ -5495,10 +5495,10 @@
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D149" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -5509,10 +5509,10 @@
         <v>313</v>
       </c>
       <c r="C150" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D150" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -5565,10 +5565,10 @@
         <v>317</v>
       </c>
       <c r="C154" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D154" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -5582,7 +5582,7 @@
         <v>330</v>
       </c>
       <c r="D155" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -5593,10 +5593,10 @@
         <v>265</v>
       </c>
       <c r="C156" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D156" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -5607,7 +5607,7 @@
         <v>266</v>
       </c>
       <c r="C157" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D157" t="s">
         <v>263</v>
@@ -5621,10 +5621,10 @@
         <v>267</v>
       </c>
       <c r="C158" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D158" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -5635,7 +5635,7 @@
         <v>268</v>
       </c>
       <c r="C159" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D159" t="s">
         <v>264</v>
@@ -5643,84 +5643,84 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B160" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C160" t="s">
+        <v>538</v>
+      </c>
+      <c r="D160" t="s">
         <v>539</v>
-      </c>
-      <c r="D160" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B161" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C161" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D161" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B162" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C162" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D162" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B163" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C163" t="s">
+        <v>544</v>
+      </c>
+      <c r="D163" t="s">
         <v>545</v>
-      </c>
-      <c r="D163" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B164" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="C164" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="C164" s="4" t="s">
-        <v>572</v>
-      </c>
       <c r="D164" s="4" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5728,97 +5728,97 @@
         <v>113</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="B167" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="C167" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="C167" s="4" t="s">
+      <c r="D167" s="4" t="s">
         <v>583</v>
-      </c>
-      <c r="D167" s="4" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B168" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="C168" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="C168" s="4" t="s">
+      <c r="D168" s="4" t="s">
         <v>588</v>
-      </c>
-      <c r="D168" s="4" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="B169" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="C169" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="C169" s="4" t="s">
+      <c r="D169" s="4" t="s">
         <v>592</v>
-      </c>
-      <c r="D169" s="4" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B170" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="C170" s="7" t="s">
         <v>596</v>
       </c>
-      <c r="C170" s="7" t="s">
+      <c r="D170" s="4" t="s">
         <v>597</v>
-      </c>
-      <c r="D170" s="4" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B171" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="C171" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="C171" s="7" t="s">
+      <c r="D171" s="4" t="s">
         <v>601</v>
-      </c>
-      <c r="D171" s="4" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="B172" s="4" t="s">
         <v>611</v>
       </c>
-      <c r="B172" s="4" t="s">
-        <v>612</v>
-      </c>
       <c r="C172" s="7" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5826,49 +5826,49 @@
         <v>127</v>
       </c>
       <c r="C173" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B174" t="s">
+        <v>629</v>
+      </c>
+      <c r="C174" t="s">
         <v>630</v>
       </c>
-      <c r="C174" t="s">
-        <v>631</v>
-      </c>
       <c r="D174" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>633</v>
+      </c>
+      <c r="B175" t="s">
         <v>634</v>
       </c>
-      <c r="B175" t="s">
+      <c r="C175" t="s">
         <v>635</v>
       </c>
-      <c r="C175" t="s">
+      <c r="D175" t="s">
         <v>636</v>
-      </c>
-      <c r="D175" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>647</v>
+      </c>
+      <c r="B176" t="s">
+        <v>649</v>
+      </c>
+      <c r="C176" s="6" t="s">
         <v>648</v>
       </c>
-      <c r="B176" t="s">
+      <c r="D176" s="6" t="s">
         <v>650</v>
-      </c>
-      <c r="C176" s="6" t="s">
-        <v>649</v>
-      </c>
-      <c r="D176" s="6" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -5876,13 +5876,13 @@
         <v>150</v>
       </c>
       <c r="B177" t="s">
+        <v>657</v>
+      </c>
+      <c r="C177" s="6" t="s">
         <v>658</v>
       </c>
-      <c r="C177" s="6" t="s">
+      <c r="D177" s="6" t="s">
         <v>659</v>
-      </c>
-      <c r="D177" s="6" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
simple merger ok (must be converted to function), input values ok
</commit_message>
<xml_diff>
--- a/Variablelist - translated and explained.xlsx
+++ b/Variablelist - translated and explained.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" firstSheet="1" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="663">
   <si>
     <t>dat</t>
   </si>
@@ -2015,6 +2015,9 @@
   </si>
   <si>
     <t>NVE.ir.t_2</t>
+  </si>
+  <si>
+    <t>HI.NVE.ir_2</t>
   </si>
 </sst>
 </file>
@@ -3564,8 +3567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5885,6 +5888,11 @@
         <v>659</v>
       </c>
     </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C178" s="6" t="s">
+        <v>662</v>
+      </c>
+    </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="6"/>
     </row>

</xml_diff>